<commit_message>
revised: 2020/04/10 data added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3477BAB8-732E-4A90-826D-F0AB6D4C278F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBDE013-4E6B-42C2-AFB7-58E3AC62CFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="718" firstSheet="1" activeTab="9" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="11730" yWindow="950" windowWidth="12110" windowHeight="12420" tabRatio="718" firstSheet="9" activeTab="10" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,11 @@
     <sheet name="2020年4月7日" sheetId="8" r:id="rId8"/>
     <sheet name="2020年4月8日" sheetId="9" r:id="rId9"/>
     <sheet name="2020年4月9日" sheetId="10" r:id="rId10"/>
+    <sheet name="2020年4月10日" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'2020年4月10日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -2417,7 +2419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D741B8C-88FF-46E2-839C-23DBAA9B29EC}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -2464,11 +2466,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>4.8506686993278356E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>48.506686993278358</v>
       </c>
     </row>
@@ -2486,11 +2488,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>2.8310951476744985E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>28.310951476744986</v>
       </c>
     </row>
@@ -2508,11 +2510,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>2.2585772667805898E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>22.585772667805898</v>
       </c>
     </row>
@@ -2530,11 +2532,11 @@
         <v>209244</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>1.9116438225229876E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>19.116438225229874</v>
       </c>
     </row>
@@ -2552,11 +2554,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>1.876987782199899E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>18.769877821998989</v>
       </c>
     </row>
@@ -2574,11 +2576,11 @@
         <v>167794</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>1.8475034864178695E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>18.475034864178696</v>
       </c>
     </row>
@@ -2596,11 +2598,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>1.5653301728571749E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>15.65330172857175</v>
       </c>
     </row>
@@ -2618,11 +2620,11 @@
         <v>342296</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>1.4607240516979456E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>14.607240516979456</v>
       </c>
     </row>
@@ -2640,11 +2642,11 @@
         <v>65891</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.3658921552260551E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>13.658921552260551</v>
       </c>
     </row>
@@ -2662,11 +2664,11 @@
         <v>411792</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.3599098574037379E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>13.599098574037379</v>
       </c>
     </row>
@@ -2684,11 +2686,11 @@
         <v>585470</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.3151826737492954E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>13.151826737492954</v>
       </c>
     </row>
@@ -2706,11 +2708,11 @@
         <v>301185</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.2948852034463868E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>12.948852034463869</v>
       </c>
     </row>
@@ -2728,11 +2730,11 @@
         <v>54709</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -2750,11 +2752,11 @@
         <v>270227</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>7.7712441761926083E-3</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>7.7712441761926083</v>
       </c>
     </row>
@@ -2772,11 +2774,11 @@
         <v>519212</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>7.5113826336833511E-3</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>7.5113826336833514</v>
       </c>
     </row>
@@ -2794,11 +2796,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>7.4729709235493097E-3</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>7.47297092354931</v>
       </c>
     </row>
@@ -2816,11 +2818,11 @@
         <v>739575</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>7.0310651387621272E-3</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>7.031065138762127</v>
       </c>
     </row>
@@ -2838,11 +2840,11 @@
         <v>742652</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>7.0019336108971628E-3</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>7.0019336108971633</v>
       </c>
     </row>
@@ -2860,11 +2862,11 @@
         <v>235836</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>6.7843755830322766E-3</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>6.7843755830322765</v>
       </c>
     </row>
@@ -2882,11 +2884,11 @@
         <v>192518</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>6.2331833906439918E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>6.2331833906439922</v>
       </c>
     </row>
@@ -2904,11 +2906,11 @@
         <v>83826</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>5.9647364779424044E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>5.9647364779424041</v>
       </c>
     </row>
@@ -2926,11 +2928,11 @@
         <v>583702</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>5.4822495040277404E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>5.4822495040277399</v>
       </c>
     </row>
@@ -2948,11 +2950,11 @@
         <v>206268</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>4.8480617449143835E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>4.8480617449143839</v>
       </c>
     </row>
@@ -2970,11 +2972,11 @@
         <v>683365</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>4.8290445076935463E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>4.8290445076935464</v>
       </c>
     </row>
@@ -2992,11 +2994,11 @@
         <v>190006</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>4.7366925254991952E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>4.736692525499195</v>
       </c>
     </row>
@@ -3014,11 +3016,11 @@
         <v>434170</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>4.6064905451781556E-3</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>4.6064905451781559</v>
       </c>
     </row>
@@ -3036,11 +3038,11 @@
         <v>354425</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>4.5143542357339349E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>4.5143542357339346</v>
       </c>
     </row>
@@ -3058,11 +3060,11 @@
         <v>125851</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>3.9729521418184997E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>3.9729521418184999</v>
       </c>
     </row>
@@ -3080,11 +3082,11 @@
         <v>218775</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>3.656724945720489E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>3.6567249457204891</v>
       </c>
     </row>
@@ -3102,11 +3104,11 @@
         <v>84247</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>3.56095766021342E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>3.5609576602134201</v>
       </c>
     </row>
@@ -3124,11 +3126,11 @@
         <v>148350</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>3.370407819346141E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>3.3704078193461409</v>
       </c>
     </row>
@@ -3146,11 +3148,11 @@
         <v>239824</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>3.3357795716859031E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>3.3357795716859031</v>
       </c>
     </row>
@@ -3168,11 +3170,11 @@
         <v>91850</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>3.2661948829613499E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>3.2661948829613499</v>
       </c>
     </row>
@@ -3190,11 +3192,11 @@
         <v>196435</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>3.0544454908748441E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0544454908748442</v>
       </c>
     </row>
@@ -3212,11 +3214,11 @@
         <v>695797</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>3.0181216647959105E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0181216647959106</v>
       </c>
     </row>
@@ -3234,11 +3236,11 @@
         <v>180822</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>2.765150258265034E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>2.765150258265034</v>
       </c>
     </row>
@@ -3256,11 +3258,11 @@
         <v>112055</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>2.6772567042969968E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>2.677256704296997</v>
       </c>
     </row>
@@ -3278,11 +3280,11 @@
         <v>75167</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>2.6607420809663814E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>2.6607420809663815</v>
       </c>
     </row>
@@ -3300,11 +3302,11 @@
         <v>75168</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>2.6607066836951895E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>2.6607066836951896</v>
       </c>
     </row>
@@ -3322,11 +3324,11 @@
         <v>127998</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>2.3437866216659635E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>2.3437866216659637</v>
       </c>
     </row>
@@ -3344,11 +3346,11 @@
         <v>263407</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>2.2778437930654843E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2778437930654842</v>
       </c>
     </row>
@@ -3366,11 +3368,11 @@
         <v>577212</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>1.905712285953861E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>1.9057122859538611</v>
       </c>
     </row>
@@ -3388,11 +3390,11 @@
         <v>116446</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>1.7175343077477972E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7175343077477971</v>
       </c>
     </row>
@@ -3410,11 +3412,11 @@
         <v>71544</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -3432,11 +3434,11 @@
         <v>80055</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>1.2491412154144025E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>1.2491412154144026</v>
       </c>
     </row>
@@ -3454,11 +3456,11 @@
         <v>133573</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>7.4865429390670265E-4</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>0.74865429390670268</v>
       </c>
     </row>
@@ -3476,11 +3478,11 @@
         <v>150417</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>6.6481847131640709E-4</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>0.66481847131640714</v>
       </c>
     </row>
@@ -3498,11 +3500,11 @@
         <v>57443</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3520,11 +3522,11 @@
         <v>147790</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3542,11 +3544,11 @@
         <v>32394</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3564,11 +3566,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3586,11 +3588,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3608,11 +3610,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3630,11 +3632,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3652,11 +3654,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3674,11 +3676,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3696,11 +3698,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3718,11 +3720,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3740,11 +3742,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3762,11 +3764,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3784,11 +3786,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3806,11 +3808,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3846,6 +3848,1446 @@
   <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
     <sortCondition descending="1" ref="F2:F66"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCADD9F-D6A4-429E-83CC-3643BB01A3B4}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>143</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>5.5051240000307977E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>55.051240000307978</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>133</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>3.8033904509162456E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>38.033904509162454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>2.7273385863010896E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>27.273385863010898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>209244</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>2.0072260136491368E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>20.072260136491369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>167794</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>1.9666972597351513E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>19.666972597351513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>56</v>
+      </c>
+      <c r="D7">
+        <v>287695</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>1.9465058482073028E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>19.465058482073026</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>173</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>1.8421912918659269E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>18.42191291865927</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>411792</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>1.6998873217546721E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>16.99887321754672</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>53</v>
+      </c>
+      <c r="D10">
+        <v>342296</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>1.5483674947998224E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>15.483674947998225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>1.5176579502511724E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>15.176579502511723</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>301185</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>1.4940983116689078E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>14.940983116689079</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>85</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>1.451825029463508E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>14.518250294635081</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>54709</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>270227</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>8.8814219156486962E-3</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>8.881421915648696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>235836</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>8.4804694787903451E-3</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>8.4804694787903454</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>519212</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>8.4743804072324978E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>8.4743804072324984</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>739575</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>7.842341885542373E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>7.842341885542373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>35</v>
+      </c>
+      <c r="D19">
+        <v>454973</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>7.6927641860066419E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>7.6927641860066416</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>54</v>
+      </c>
+      <c r="D20">
+        <v>742652</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>7.2712387497778233E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>7.2712387497778233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>83826</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>7.1576837735308858E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>7.157683773530886</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>125851</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>6.3567234269095996E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>6.3567234269095998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>37</v>
+      </c>
+      <c r="D23">
+        <v>583702</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>6.3388509890320742E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>6.3388509890320739</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>192518</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>6.2331833906439918E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>6.2331833906439922</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>190006</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>5.262991694999105E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>5.2629916949991049</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>683365</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>5.1217138717961847E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>5.1217138717961843</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>206268</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>4.8480617449143835E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>4.8480617449143839</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>354425</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>4.7965013754673064E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>4.7965013754673063</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>84247</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>4.7479435469512266E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>4.7479435469512268</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>434170</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>4.6064905451781556E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>4.6064905451781559</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>218775</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>4.570906182150611E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>4.570906182150611</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>91850</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>4.3549265106151338E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>4.354926510615134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>4.0444893832153692E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>4.0444893832153692</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>75168</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>3.9910600255427843E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>3.9910600255427844</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>239824</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>3.7527520181466407E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>3.7527520181466407</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36">
+        <v>25</v>
+      </c>
+      <c r="D36">
+        <v>695797</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>3.5930019818998932E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>3.5930019818998931</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>196435</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>3.0544454908748441E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>3.0544454908748442</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>180822</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>2.765150258265034E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>2.765150258265034</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>112055</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>75167</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>2.6607420809663814E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>2.6607420809663815</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>116446</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>2.5763014616216958E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>2.5763014616216959</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>127998</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>2.3437866216659635E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>2.3437866216659637</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>263407</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>2.2778437930654843E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>2.2778437930654842</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>577212</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>2.2522054288545632E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>2.252205428854563</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>71544</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>80055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>1.2491412154144025E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>1.2491412154144026</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>133573</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>7.4865429390670265E-4</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>0.74865429390670268</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>150417</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>6.6481847131640709E-4</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>0.66481847131640714</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>39</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>57443</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>147790</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>48</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>249</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10348,11 +11790,11 @@
         <v>112055</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.7848378028646648E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>1.7848378028646648</v>
       </c>
     </row>
@@ -11788,11 +13230,11 @@
         <v>695797</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>2.2995212684159315E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>2.2995212684159316</v>
       </c>
     </row>
@@ -13228,11 +14670,11 @@
         <v>84247</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>2.3739717734756133E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>2.3739717734756134</v>
       </c>
     </row>
@@ -13964,11 +15406,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>4.1192186573657016E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>41.192186573657018</v>
       </c>
     </row>
@@ -13986,11 +15428,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>2.4021413374207864E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>24.021413374207864</v>
       </c>
     </row>
@@ -14008,11 +15450,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>2.0881186051367719E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>20.88118605136772</v>
       </c>
     </row>
@@ -14030,11 +15472,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>1.8475034864178695E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>18.475034864178696</v>
       </c>
     </row>
@@ -14052,11 +15494,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>1.7727106831887936E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>17.727106831887937</v>
       </c>
     </row>
@@ -14074,11 +15516,11 @@
         <v>209244</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>1.6726883447076141E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>16.72688344707614</v>
       </c>
     </row>
@@ -14096,11 +15538,11 @@
         <v>65891</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>1.3658921552260551E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>13.658921552260551</v>
       </c>
     </row>
@@ -14118,11 +15560,11 @@
         <v>411792</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>1.3599098574037379E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>13.599098574037379</v>
       </c>
     </row>
@@ -14140,11 +15582,11 @@
         <v>342296</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.34386612756211E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>13.438661275621101</v>
       </c>
     </row>
@@ -14162,11 +15604,11 @@
         <v>939099</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.3204145675802019E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>13.204145675802019</v>
       </c>
     </row>
@@ -14184,11 +15626,11 @@
         <v>585470</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.298102379285019E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>12.981023792850189</v>
       </c>
     </row>
@@ -14206,11 +15648,11 @@
         <v>301185</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.0292677258163588E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>10.292677258163588</v>
       </c>
     </row>
@@ -14228,11 +15670,11 @@
         <v>54709</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -14250,11 +15692,11 @@
         <v>739575</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>6.8958523476320864E-3</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>6.8958523476320863</v>
       </c>
     </row>
@@ -14272,11 +15714,11 @@
         <v>742652</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>6.4633233331358427E-3</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>6.4633233331358424</v>
       </c>
     </row>
@@ -14294,11 +15736,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>6.3740046112626464E-3</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3740046112626461</v>
       </c>
     </row>
@@ -14316,11 +15758,11 @@
         <v>192518</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>6.2331833906439918E-3</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>6.2331833906439922</v>
       </c>
     </row>
@@ -14338,11 +15780,11 @@
         <v>83826</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>5.9647364779424044E-3</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>5.9647364779424041</v>
       </c>
     </row>
@@ -14360,11 +15802,11 @@
         <v>270227</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>5.1808294507950719E-3</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>5.1808294507950716</v>
       </c>
     </row>
@@ -14382,11 +15824,11 @@
         <v>583702</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>5.1396089100260063E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>5.1396089100260065</v>
       </c>
     </row>
@@ -14404,11 +15846,11 @@
         <v>235836</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>5.0882816872742072E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>5.0882816872742076</v>
       </c>
     </row>
@@ -14426,11 +15868,11 @@
         <v>519212</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>5.0075884224555674E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>5.0075884224555676</v>
       </c>
     </row>
@@ -14448,11 +15890,11 @@
         <v>206268</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>4.8480617449143835E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>4.8480617449143839</v>
       </c>
     </row>
@@ -14470,11 +15912,11 @@
         <v>434170</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>4.6064905451781556E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>4.6064905451781559</v>
       </c>
     </row>
@@ -14492,11 +15934,11 @@
         <v>190006</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>4.2103933559992845E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>4.2103933559992841</v>
       </c>
     </row>
@@ -14514,11 +15956,11 @@
         <v>683365</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>4.0973710974369481E-3</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>4.0973710974369482</v>
       </c>
     </row>
@@ -14536,11 +15978,11 @@
         <v>125851</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>3.9729521418184997E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>3.9729521418184999</v>
       </c>
     </row>
@@ -14558,11 +16000,11 @@
         <v>354425</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>3.6679128165338225E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>3.6679128165338226</v>
       </c>
     </row>
@@ -14580,11 +16022,11 @@
         <v>84247</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>3.56095766021342E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>3.5609576602134201</v>
       </c>
     </row>
@@ -14602,11 +16044,11 @@
         <v>148350</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>3.370407819346141E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>3.3704078193461409</v>
       </c>
     </row>
@@ -14624,11 +16066,11 @@
         <v>91850</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>3.2661948829613499E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>3.2661948829613499</v>
       </c>
     </row>
@@ -14646,11 +16088,11 @@
         <v>218775</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>3.199634327505428E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>3.1996343275054278</v>
       </c>
     </row>
@@ -14668,11 +16110,11 @@
         <v>112055</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>2.6772567042969968E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>2.677256704296997</v>
       </c>
     </row>
@@ -14690,11 +16132,11 @@
         <v>695797</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>2.5869614269679233E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>2.5869614269679233</v>
       </c>
     </row>
@@ -14712,11 +16154,11 @@
         <v>196435</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>2.5453712423957036E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>2.5453712423957038</v>
       </c>
     </row>
@@ -14734,11 +16176,11 @@
         <v>239824</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>2.5018346787644271E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>2.501834678764427</v>
       </c>
     </row>
@@ -14756,11 +16198,11 @@
         <v>577212</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>1.905712285953861E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>1.9057122859538611</v>
       </c>
     </row>
@@ -14778,11 +16220,11 @@
         <v>263407</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>1.8982031608879035E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>1.8982031608879035</v>
       </c>
     </row>
@@ -14800,11 +16242,11 @@
         <v>116446</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>1.7175343077477972E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7175343077477971</v>
       </c>
     </row>
@@ -14822,11 +16264,11 @@
         <v>180822</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>1.6590901549590204E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>1.6590901549590205</v>
       </c>
     </row>
@@ -14844,11 +16286,11 @@
         <v>127998</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>1.5625244144439757E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>1.5625244144439756</v>
       </c>
     </row>
@@ -14866,11 +16308,11 @@
         <v>71544</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -14888,11 +16330,11 @@
         <v>75168</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>1.3303533418475948E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3303533418475948</v>
       </c>
     </row>
@@ -14910,11 +16352,11 @@
         <v>80055</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>1.2491412154144025E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>1.2491412154144026</v>
       </c>
     </row>
@@ -14932,11 +16374,11 @@
         <v>133573</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>7.4865429390670265E-4</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>0.74865429390670268</v>
       </c>
     </row>
@@ -14954,11 +16396,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>6.6481847131640709E-4</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>0.66481847131640714</v>
       </c>
     </row>
@@ -14976,11 +16418,11 @@
         <v>75167</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -14998,11 +16440,11 @@
         <v>57443</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15020,11 +16462,11 @@
         <v>147790</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15042,11 +16484,11 @@
         <v>32394</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15064,11 +16506,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15086,11 +16528,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15108,11 +16550,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15130,11 +16572,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15152,11 +16594,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15174,11 +16616,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15196,11 +16638,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15218,11 +16660,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15240,11 +16682,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15262,11 +16704,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15284,11 +16726,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -15306,11 +16748,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revised: add 2020/4/11 and 2020/4/12 data
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBDE013-4E6B-42C2-AFB7-58E3AC62CFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D48CE1-0B73-4024-BD9E-449F6582C86F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11730" yWindow="950" windowWidth="12110" windowHeight="12420" tabRatio="718" firstSheet="9" activeTab="10" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="14630" yWindow="1030" windowWidth="12110" windowHeight="12420" tabRatio="718" firstSheet="9" activeTab="11" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,12 @@
     <sheet name="2020年4月8日" sheetId="9" r:id="rId9"/>
     <sheet name="2020年4月9日" sheetId="10" r:id="rId10"/>
     <sheet name="2020年4月10日" sheetId="11" r:id="rId11"/>
+    <sheet name="2020年4月11日" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'2020年4月10日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'2020年4月11日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -2420,7 +2422,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3170,11 +3172,11 @@
         <v>91850</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>3.2661948829613499E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>3.2661948829613499</v>
       </c>
     </row>
@@ -3859,8 +3861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCADD9F-D6A4-429E-83CC-3643BB01A3B4}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3906,11 +3908,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>5.5051240000307977E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>55.051240000307978</v>
       </c>
     </row>
@@ -3928,11 +3930,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>3.8033904509162456E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>38.033904509162454</v>
       </c>
     </row>
@@ -3950,11 +3952,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>2.7273385863010896E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>27.273385863010898</v>
       </c>
     </row>
@@ -3972,11 +3974,11 @@
         <v>209244</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>2.0072260136491368E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>20.072260136491369</v>
       </c>
     </row>
@@ -3994,11 +3996,11 @@
         <v>167794</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>1.9666972597351513E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>19.666972597351513</v>
       </c>
     </row>
@@ -4016,11 +4018,11 @@
         <v>287695</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>1.9465058482073028E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>19.465058482073026</v>
       </c>
     </row>
@@ -4038,11 +4040,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>1.8421912918659269E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>18.42191291865927</v>
       </c>
     </row>
@@ -4060,11 +4062,11 @@
         <v>411792</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>1.6998873217546721E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>16.99887321754672</v>
       </c>
     </row>
@@ -4082,11 +4084,11 @@
         <v>342296</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.5483674947998224E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>15.483674947998225</v>
       </c>
     </row>
@@ -4104,11 +4106,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.5176579502511724E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>15.176579502511723</v>
       </c>
     </row>
@@ -4126,11 +4128,11 @@
         <v>301185</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.4940983116689078E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>14.940983116689079</v>
       </c>
     </row>
@@ -4148,11 +4150,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.451825029463508E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>14.518250294635081</v>
       </c>
     </row>
@@ -4170,11 +4172,11 @@
         <v>54709</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -4192,11 +4194,11 @@
         <v>270227</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>8.8814219156486962E-3</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>8.881421915648696</v>
       </c>
     </row>
@@ -4214,11 +4216,11 @@
         <v>235836</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>8.4804694787903451E-3</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>8.4804694787903454</v>
       </c>
     </row>
@@ -4236,11 +4238,11 @@
         <v>519212</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>8.4743804072324978E-3</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>8.4743804072324984</v>
       </c>
     </row>
@@ -4258,11 +4260,11 @@
         <v>739575</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>7.842341885542373E-3</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>7.842341885542373</v>
       </c>
     </row>
@@ -4280,11 +4282,11 @@
         <v>454973</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>7.6927641860066419E-3</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>7.6927641860066416</v>
       </c>
     </row>
@@ -4302,11 +4304,11 @@
         <v>742652</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>7.2712387497778233E-3</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>7.2712387497778233</v>
       </c>
     </row>
@@ -4324,11 +4326,11 @@
         <v>83826</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>7.1576837735308858E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>7.157683773530886</v>
       </c>
     </row>
@@ -4346,11 +4348,11 @@
         <v>125851</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>6.3567234269095996E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3567234269095998</v>
       </c>
     </row>
@@ -4368,11 +4370,11 @@
         <v>583702</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>6.3388509890320742E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3388509890320739</v>
       </c>
     </row>
@@ -4390,11 +4392,11 @@
         <v>192518</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>6.2331833906439918E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>6.2331833906439922</v>
       </c>
     </row>
@@ -4412,11 +4414,11 @@
         <v>190006</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>5.262991694999105E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>5.2629916949991049</v>
       </c>
     </row>
@@ -4434,11 +4436,11 @@
         <v>683365</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>5.1217138717961847E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>5.1217138717961843</v>
       </c>
     </row>
@@ -4456,11 +4458,11 @@
         <v>206268</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>4.8480617449143835E-3</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>4.8480617449143839</v>
       </c>
     </row>
@@ -4478,11 +4480,11 @@
         <v>354425</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>4.7965013754673064E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>4.7965013754673063</v>
       </c>
     </row>
@@ -4500,11 +4502,11 @@
         <v>84247</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>4.7479435469512266E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>4.7479435469512268</v>
       </c>
     </row>
@@ -4522,11 +4524,11 @@
         <v>434170</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>4.6064905451781556E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>4.6064905451781559</v>
       </c>
     </row>
@@ -4544,11 +4546,11 @@
         <v>218775</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>4.570906182150611E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>4.570906182150611</v>
       </c>
     </row>
@@ -4566,11 +4568,11 @@
         <v>91850</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>4.3549265106151338E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>4.354926510615134</v>
       </c>
     </row>
@@ -4588,11 +4590,11 @@
         <v>148350</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>4.0444893832153692E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>4.0444893832153692</v>
       </c>
     </row>
@@ -4610,11 +4612,11 @@
         <v>75168</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>3.9910600255427843E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>3.9910600255427844</v>
       </c>
     </row>
@@ -4632,11 +4634,11 @@
         <v>239824</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>3.7527520181466407E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>3.7527520181466407</v>
       </c>
     </row>
@@ -4654,11 +4656,11 @@
         <v>695797</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>3.5930019818998932E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>3.5930019818998931</v>
       </c>
     </row>
@@ -4676,11 +4678,11 @@
         <v>196435</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>3.0544454908748441E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0544454908748442</v>
       </c>
     </row>
@@ -4698,11 +4700,11 @@
         <v>180822</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>2.765150258265034E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>2.765150258265034</v>
       </c>
     </row>
@@ -4720,11 +4722,11 @@
         <v>112055</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>2.6772567042969968E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>2.677256704296997</v>
       </c>
     </row>
@@ -4742,11 +4744,11 @@
         <v>75167</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>2.6607420809663814E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>2.6607420809663815</v>
       </c>
     </row>
@@ -4764,11 +4766,11 @@
         <v>116446</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>2.5763014616216958E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>2.5763014616216959</v>
       </c>
     </row>
@@ -4786,11 +4788,11 @@
         <v>127998</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>2.3437866216659635E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>2.3437866216659637</v>
       </c>
     </row>
@@ -4808,11 +4810,11 @@
         <v>263407</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>2.2778437930654843E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2778437930654842</v>
       </c>
     </row>
@@ -4830,11 +4832,11 @@
         <v>577212</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>2.2522054288545632E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>2.252205428854563</v>
       </c>
     </row>
@@ -4852,11 +4854,11 @@
         <v>71544</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -4874,11 +4876,11 @@
         <v>80055</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>1.2491412154144025E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>1.2491412154144026</v>
       </c>
     </row>
@@ -4896,11 +4898,11 @@
         <v>133573</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>7.4865429390670265E-4</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>0.74865429390670268</v>
       </c>
     </row>
@@ -4918,11 +4920,11 @@
         <v>150417</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>6.6481847131640709E-4</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>0.66481847131640714</v>
       </c>
     </row>
@@ -4940,11 +4942,11 @@
         <v>57443</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4962,11 +4964,11 @@
         <v>147790</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4984,11 +4986,11 @@
         <v>32394</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5006,11 +5008,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5028,11 +5030,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5050,11 +5052,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5072,11 +5074,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5094,11 +5096,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5116,11 +5118,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5138,11 +5140,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5160,11 +5162,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5182,11 +5184,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5204,11 +5206,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5226,11 +5228,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5248,11 +5250,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5279,6 +5281,1446 @@
       </c>
       <c r="C65">
         <v>249</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB8681F-DAFE-4DE6-B191-23CE8F6906F4}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>155</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>5.9670924475858297E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>59.6709244758583</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>139</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>3.9749719750177298E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>39.749719750177299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>2.9404119133558622E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>29.404119133558623</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>209244</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>2.1983903959014357E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>21.983903959014356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>167794</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>2.0858910330524335E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>20.858910330524335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>84</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>2.0398647861056066E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>20.398647861056066</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>191</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>2.0338643742566012E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>20.338643742566013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>58</v>
+      </c>
+      <c r="D9">
+        <v>287695</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.0160239142147065E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>20.160239142147066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>342296</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>1.8112978241054525E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>18.112978241054524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>301185</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>1.6269070504839219E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>16.26907050483922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>92</v>
+      </c>
+      <c r="D12">
+        <v>585470</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>1.5713870907134438E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>15.713870907134439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>65891</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>1.5176579502511724E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>15.176579502511723</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>51</v>
+      </c>
+      <c r="D14">
+        <v>519212</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>9.8225772902013047E-3</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>9.8225772902013055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>454973</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>9.6709035481226356E-3</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>9.6709035481226362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>235836</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>9.3285164266693806E-3</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>9.3285164266693812</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>270227</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>9.2514811621340568E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>9.2514811621340574</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>54709</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>65</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>8.7888314234526588E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>8.7888314234526597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>83826</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>8.3506310691193655E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>8.3506310691193661</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21">
+        <v>742652</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>8.0791541664198031E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>8.0791541664198032</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>192518</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>6.7526153398643242E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>6.7526153398643238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>583702</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>6.5101712860329416E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>6.5101712860329419</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>44</v>
+      </c>
+      <c r="D24">
+        <v>683365</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>6.4387260102580614E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>6.438726010258061</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>125851</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>6.3567234269095996E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>6.3567234269095998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>190006</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>5.7892908644990157E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>5.7892908644990158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>39</v>
+      </c>
+      <c r="D27">
+        <v>695797</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>5.6050830917638338E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>5.6050830917638335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>354425</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>5.3607956549340478E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>5.3607956549340479</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>206268</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>5.3328679194058213E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>5.3328679194058211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>218775</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>5.0279968003656729E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>5.0279968003656732</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>239824</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>5.0036693575288543E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>5.003669357528854</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>434170</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>4.8368150724370637E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>4.836815072437064</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>84247</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>4.7479435469512266E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>4.7479435469512268</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>148350</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>4.7185709470845974E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>4.7185709470845971</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>180822</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>4.4242404132240542E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>4.4242404132240543</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>91850</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>4.3549265106151338E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>4.354926510615134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>75168</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>3.9910600255427843E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>3.9910600255427844</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>263407</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>3.796406321775807E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>3.7964063217758071</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>147790</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>3.3831788348332092E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>3.3831788348332092</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>196435</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>3.0544454908748441E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>3.0544454908748442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>112055</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>2.6607420809663814E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>2.6607420809663815</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>577212</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>2.5986985717552651E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>2.5986985717552651</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>116446</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>2.5763014616216958E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>2.5763014616216959</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>127998</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>2.3437866216659635E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>2.3437866216659637</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>28</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>133573</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>1.4973085878134053E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>1.4973085878134054</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>71544</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>80055</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>1.2491412154144025E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>1.2491412154144026</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>150417</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>6.6481847131640709E-4</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>0.66481847131640714</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>278</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>
@@ -16110,11 +17552,11 @@
         <v>112055</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>2.6772567042969968E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>2.677256704296997</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revised: data add 2020/04/12 adn 2020/04/13.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D48CE1-0B73-4024-BD9E-449F6582C86F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6D4DFB-5519-4B2C-B722-8F10B2770C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14630" yWindow="1030" windowWidth="12110" windowHeight="12420" tabRatio="718" firstSheet="9" activeTab="11" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="9030" yWindow="480" windowWidth="17070" windowHeight="12420" tabRatio="718" firstSheet="8" activeTab="12" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,13 @@
     <sheet name="2020年4月9日" sheetId="10" r:id="rId10"/>
     <sheet name="2020年4月10日" sheetId="11" r:id="rId11"/>
     <sheet name="2020年4月11日" sheetId="12" r:id="rId12"/>
+    <sheet name="2020年4月12日" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'2020年4月10日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'2020年4月11日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'2020年4月12日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -5301,7 +5303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB8681F-DAFE-4DE6-B191-23CE8F6906F4}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -5348,11 +5350,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>5.9670924475858297E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>59.6709244758583</v>
       </c>
     </row>
@@ -5370,11 +5372,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>3.9749719750177298E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>39.749719750177299</v>
       </c>
     </row>
@@ -5392,11 +5394,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>2.9404119133558622E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>29.404119133558623</v>
       </c>
     </row>
@@ -5414,11 +5416,11 @@
         <v>209244</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>2.1983903959014357E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>21.983903959014356</v>
       </c>
     </row>
@@ -5436,11 +5438,11 @@
         <v>167794</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.0858910330524335E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>20.858910330524335</v>
       </c>
     </row>
@@ -5458,11 +5460,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2.0398647861056066E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>20.398647861056066</v>
       </c>
     </row>
@@ -5480,11 +5482,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.0338643742566012E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>20.338643742566013</v>
       </c>
     </row>
@@ -5502,11 +5504,11 @@
         <v>287695</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.0160239142147065E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>20.160239142147066</v>
       </c>
     </row>
@@ -5524,11 +5526,11 @@
         <v>342296</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.8112978241054525E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>18.112978241054524</v>
       </c>
     </row>
@@ -5546,11 +5548,11 @@
         <v>301185</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.6269070504839219E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>16.26907050483922</v>
       </c>
     </row>
@@ -5568,11 +5570,11 @@
         <v>585470</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.5713870907134438E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>15.713870907134439</v>
       </c>
     </row>
@@ -5590,11 +5592,11 @@
         <v>65891</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.5176579502511724E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>15.176579502511723</v>
       </c>
     </row>
@@ -5612,6 +5614,1446 @@
         <v>519212</v>
       </c>
       <c r="E14">
+        <f t="shared" si="0"/>
+        <v>9.8225772902013047E-3</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>9.8225772902013055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>454973</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>9.6709035481226356E-3</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6709035481226362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>235836</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>9.3285164266693806E-3</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>9.3285164266693812</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>270227</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>9.2514811621340568E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>9.2514811621340574</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>54709</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>65</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>8.7888314234526588E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>8.7888314234526597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>83826</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>8.3506310691193655E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>8.3506310691193661</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21">
+        <v>742652</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>8.0791541664198031E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>8.0791541664198032</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>192518</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>6.7526153398643242E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>6.7526153398643238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>583702</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>6.5101712860329416E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5101712860329419</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>44</v>
+      </c>
+      <c r="D24">
+        <v>683365</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>6.4387260102580614E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>6.438726010258061</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>125851</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>6.3567234269095996E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>6.3567234269095998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>190006</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>5.7892908644990157E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7892908644990158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>39</v>
+      </c>
+      <c r="D27">
+        <v>695797</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>5.6050830917638338E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6050830917638335</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>354425</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>5.3607956549340478E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3607956549340479</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>206268</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>5.3328679194058213E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3328679194058211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>218775</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>5.0279968003656729E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>5.0279968003656732</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>239824</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>5.0036693575288543E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>5.003669357528854</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>434170</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>4.8368150724370637E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>4.836815072437064</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>84247</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>4.7479435469512266E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7479435469512268</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>148350</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>4.7185709470845974E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>4.7185709470845971</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>180822</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>4.4242404132240542E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>4.4242404132240543</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>91850</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>4.3549265106151338E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>4.354926510615134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>75168</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>3.9910600255427843E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9910600255427844</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>263407</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>3.796406321775807E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>3.7964063217758071</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>147790</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>3.3831788348332092E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3831788348332092</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>196435</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>3.0544454908748441E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0544454908748442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>112055</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>2.6607420809663814E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6607420809663815</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>577212</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>2.5986985717552651E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>2.5986985717552651</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>116446</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>2.5763014616216958E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>2.5763014616216959</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>127998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>2.3437866216659635E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>2.3437866216659637</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>28</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>133573</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>1.4973085878134053E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4973085878134054</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>71544</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>80055</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>1.2491412154144025E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2491412154144026</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>150417</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>6.6481847131640709E-4</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>0.66481847131640714</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>278</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE7700A-3136-495F-BF2B-878EB2092195}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>158</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>6.0825845594745881E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>60.825845594745878</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>164</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>4.6898949921072498E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>46.8989499210725</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>71</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>3.0256412441777715E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>30.256412441777716</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>209244</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>2.2461814914645103E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>22.461814914645103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>63</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>2.1898190792332156E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>21.898190792332155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>2.1855694136845787E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>21.855694136845788</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>167794</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>2.1454879197110744E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>21.454879197110746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>195</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.0764583925656402E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>20.764583925656403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>342296</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>1.9281557482412882E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>19.281557482412882</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>1.6694237452762897E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>16.694237452762898</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>301185</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>1.6269070504839219E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>16.26907050483922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>92</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>1.5713870907134438E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>15.713870907134439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>51</v>
+      </c>
+      <c r="D14">
+        <v>519212</v>
+      </c>
+      <c r="E14">
         <f>100*C14/D14</f>
         <v>9.8225772902013047E-3</v>
       </c>
@@ -5622,46 +7064,46 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D15">
-        <v>454973</v>
+        <v>235836</v>
       </c>
       <c r="E15">
         <f>100*C15/D15</f>
-        <v>9.6709035481226356E-3</v>
+        <v>9.7525399006088975E-3</v>
       </c>
       <c r="F15" s="1">
         <f>E15*1000</f>
-        <v>9.6709035481226362</v>
+        <v>9.7525399006088982</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D16">
-        <v>235836</v>
+        <v>454973</v>
       </c>
       <c r="E16">
         <f>100*C16/D16</f>
-        <v>9.3285164266693806E-3</v>
+        <v>9.6709035481226356E-3</v>
       </c>
       <c r="F16" s="1">
         <f>E16*1000</f>
-        <v>9.3285164266693812</v>
+        <v>9.6709035481226362</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5672,18 +7114,18 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17">
         <v>270227</v>
       </c>
       <c r="E17">
         <f>100*C17/D17</f>
-        <v>9.2514811621340568E-3</v>
+        <v>9.6215404086194192E-3</v>
       </c>
       <c r="F17" s="1">
         <f>E17*1000</f>
-        <v>9.2514811621340574</v>
+        <v>9.6215404086194187</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5716,18 +7158,18 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>739575</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>8.7888314234526588E-3</v>
+        <v>8.9240442145826996E-3</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>8.7888314234526597</v>
+        <v>8.9240442145827004</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5760,128 +7202,128 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21">
         <v>742652</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>8.0791541664198031E-3</v>
+        <v>7.9445015969794742E-3</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>8.0791541664198032</v>
+        <v>7.9445015969794746</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D22">
-        <v>192518</v>
+        <v>583702</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>6.7526153398643242E-3</v>
+        <v>7.8807336620398769E-3</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>6.7526153398643238</v>
+        <v>7.8807336620398774</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D23">
-        <v>583702</v>
+        <v>192518</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>6.5101712860329416E-3</v>
+        <v>6.7526153398643242E-3</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>6.5101712860329419</v>
+        <v>6.7526153398643238</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C24">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="D24">
-        <v>683365</v>
+        <v>75168</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>6.4387260102580614E-3</v>
+        <v>6.6517667092379738E-3</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>6.438726010258061</v>
+        <v>6.6517667092379735</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D25">
-        <v>125851</v>
+        <v>683365</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>6.3567234269095996E-3</v>
+        <v>6.585060692309381E-3</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>6.3567234269095998</v>
+        <v>6.5850606923093808</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D26">
-        <v>190006</v>
+        <v>125851</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>5.7892908644990157E-3</v>
+        <v>6.3567234269095996E-3</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>5.7892908644990158</v>
+        <v>6.3567234269095998</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5892,106 +7334,106 @@
         <v>22</v>
       </c>
       <c r="C27">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D27">
         <v>695797</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>5.6050830917638338E-3</v>
+        <v>6.1799634088678165E-3</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>5.6050830917638335</v>
+        <v>6.1799634088678168</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
       <c r="C28">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D28">
-        <v>354425</v>
+        <v>218775</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>5.3607956549340478E-3</v>
+        <v>5.9421780367957949E-3</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>5.3607956549340479</v>
+        <v>5.942178036795795</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>11</v>
       </c>
       <c r="D29">
-        <v>206268</v>
+        <v>190006</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>5.3328679194058213E-3</v>
+        <v>5.7892908644990157E-3</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>5.3328679194058211</v>
+        <v>5.7892908644990158</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D30">
-        <v>218775</v>
+        <v>354425</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>5.0279968003656729E-3</v>
+        <v>5.6429427946674193E-3</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>5.0279968003656732</v>
+        <v>5.6429427946674195</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31">
-        <v>239824</v>
+        <v>206268</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>5.0036693575288543E-3</v>
+        <v>5.3328679194058213E-3</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>5.003669357528854</v>
+        <v>5.3328679194058211</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6002,282 +7444,282 @@
         <v>29</v>
       </c>
       <c r="C32">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D32">
         <v>434170</v>
       </c>
       <c r="E32">
         <f>100*C32/D32</f>
-        <v>4.8368150724370637E-3</v>
+        <v>5.0671395996959717E-3</v>
       </c>
       <c r="F32" s="1">
         <f>E32*1000</f>
-        <v>4.836815072437064</v>
+        <v>5.0671395996959721</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>84247</v>
+        <v>239824</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>4.7479435469512266E-3</v>
+        <v>5.0036693575288543E-3</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>4.7479435469512268</v>
+        <v>5.003669357528854</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>148350</v>
+        <v>84247</v>
       </c>
       <c r="E34">
         <f>100*C34/D34</f>
-        <v>4.7185709470845974E-3</v>
+        <v>4.7479435469512266E-3</v>
       </c>
       <c r="F34" s="1">
         <f>E34*1000</f>
-        <v>4.7185709470845971</v>
+        <v>4.7479435469512268</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C35">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35">
-        <v>180822</v>
+        <v>148350</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>4.4242404132240542E-3</v>
+        <v>4.7185709470845974E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>4.4242404132240543</v>
+        <v>4.7185709470845971</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
         <v>46</v>
       </c>
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
       <c r="C36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D36">
-        <v>91850</v>
+        <v>180822</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>4.3549265106151338E-3</v>
+        <v>4.4242404132240542E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>4.354926510615134</v>
+        <v>4.4242404132240543</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37">
-        <v>75168</v>
+        <v>91850</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>3.9910600255427843E-3</v>
+        <v>4.3549265106151338E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>3.9910600255427844</v>
+        <v>4.354926510615134</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C38">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D38">
-        <v>263407</v>
+        <v>116446</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>3.796406321775807E-3</v>
+        <v>4.2938357693694928E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>3.7964063217758071</v>
+        <v>4.2938357693694931</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>147790</v>
+        <v>263407</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>3.3831788348332092E-3</v>
+        <v>3.796406321775807E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>3.3831788348332092</v>
+        <v>3.7964063217758071</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40">
-        <v>196435</v>
+        <v>147790</v>
       </c>
       <c r="E40">
         <f>100*C40/D40</f>
-        <v>3.0544454908748441E-3</v>
+        <v>3.3831788348332092E-3</v>
       </c>
       <c r="F40" s="1">
         <f>E40*1000</f>
-        <v>3.0544454908748442</v>
+        <v>3.3831788348332092</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D41">
-        <v>112055</v>
+        <v>196435</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>2.6772567042969968E-3</v>
+        <v>3.0544454908748441E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>2.677256704296997</v>
+        <v>3.0544454908748442</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D42">
-        <v>75167</v>
+        <v>577212</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>2.6607420809663814E-3</v>
+        <v>2.7719451432056158E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>2.6607420809663815</v>
+        <v>2.7719451432056159</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C43">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>577212</v>
+        <v>112055</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>2.5986985717552651E-3</v>
+        <v>2.6772567042969968E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>2.5986985717552651</v>
+        <v>2.677256704296997</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44">
-        <v>116446</v>
+        <v>75167</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>2.5763014616216958E-3</v>
+        <v>2.6607420809663814E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>2.5763014616216959</v>
+        <v>2.6607420809663815</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6706,7 +8148,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -6720,7 +8162,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>278</v>
+        <v>365</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: 2020/4/12 and 2020/4/13 add.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6D4DFB-5519-4B2C-B722-8F10B2770C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2ED294-6CA9-486C-A2C9-87F1E27F9011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9030" yWindow="480" windowWidth="17070" windowHeight="12420" tabRatio="718" firstSheet="8" activeTab="12" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="12380" yWindow="760" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="11" activeTab="12" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,14 @@
     <sheet name="2020年4月10日" sheetId="11" r:id="rId11"/>
     <sheet name="2020年4月11日" sheetId="12" r:id="rId12"/>
     <sheet name="2020年4月12日" sheetId="13" r:id="rId13"/>
+    <sheet name="2020年4月13日" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'2020年4月10日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'2020年4月11日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'2020年4月12日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'2020年4月13日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -58,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -6054,11 +6056,11 @@
         <v>148350</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>4.7185709470845974E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>4.7185709470845971</v>
       </c>
     </row>
@@ -6744,7 +6746,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -6790,11 +6792,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>6.0825845594745881E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>60.825845594745878</v>
       </c>
     </row>
@@ -6812,11 +6814,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>4.6898949921072498E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>46.8989499210725</v>
       </c>
     </row>
@@ -6834,11 +6836,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>3.0256412441777715E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>30.256412441777716</v>
       </c>
     </row>
@@ -6856,11 +6858,11 @@
         <v>209244</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>2.2461814914645103E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>22.461814914645103</v>
       </c>
     </row>
@@ -6878,11 +6880,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.1898190792332156E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>21.898190792332155</v>
       </c>
     </row>
@@ -6900,11 +6902,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2.1855694136845787E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>21.855694136845788</v>
       </c>
     </row>
@@ -6922,11 +6924,11 @@
         <v>167794</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.1454879197110744E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>21.454879197110746</v>
       </c>
     </row>
@@ -6944,11 +6946,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.0764583925656402E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>20.764583925656403</v>
       </c>
     </row>
@@ -6966,11 +6968,11 @@
         <v>342296</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.9281557482412882E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>19.281557482412882</v>
       </c>
     </row>
@@ -6988,11 +6990,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.6694237452762897E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>16.694237452762898</v>
       </c>
     </row>
@@ -7010,11 +7012,11 @@
         <v>301185</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.6269070504839219E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>16.26907050483922</v>
       </c>
     </row>
@@ -7032,11 +7034,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.5713870907134438E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>15.713870907134439</v>
       </c>
     </row>
@@ -7054,11 +7056,11 @@
         <v>519212</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>9.8225772902013047E-3</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>9.8225772902013055</v>
       </c>
     </row>
@@ -7076,11 +7078,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>9.7525399006088975E-3</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>9.7525399006088982</v>
       </c>
     </row>
@@ -7098,11 +7100,11 @@
         <v>454973</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>9.6709035481226356E-3</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>9.6709035481226362</v>
       </c>
     </row>
@@ -7120,11 +7122,11 @@
         <v>270227</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>9.6215404086194192E-3</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>9.6215404086194187</v>
       </c>
     </row>
@@ -7142,6 +7144,1446 @@
         <v>54709</v>
       </c>
       <c r="E18">
+        <f t="shared" si="0"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>66</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>8.9240442145826996E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>8.9240442145827004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>83826</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>8.3506310691193655E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>8.3506310691193661</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>59</v>
+      </c>
+      <c r="D21">
+        <v>742652</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>7.9445015969794742E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>7.9445015969794746</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>46</v>
+      </c>
+      <c r="D22">
+        <v>583702</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>7.8807336620398769E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8807336620398774</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>192518</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>6.7526153398643242E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>6.7526153398643238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>75168</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>6.6517667092379738E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6517667092379735</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>683365</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>6.585060692309381E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5850606923093808</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>125851</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>6.3567234269095996E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>6.3567234269095998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>695797</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>6.1799634088678165E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>6.1799634088678168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>13</v>
+      </c>
+      <c r="D28">
+        <v>218775</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>5.9421780367957949E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>5.942178036795795</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>190006</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>5.7892908644990157E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7892908644990158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>354425</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>5.6429427946674193E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6429427946674195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>206268</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>5.3328679194058213E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3328679194058211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>22</v>
+      </c>
+      <c r="D32">
+        <v>434170</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>5.0671395996959717E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>5.0671395996959721</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>239824</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>5.0036693575288543E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>5.003669357528854</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>84247</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
+        <v>4.7479435469512266E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
+        <v>4.7479435469512268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>148350</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>4.7185709470845974E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>4.7185709470845971</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>180822</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>4.4242404132240542E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>4.4242404132240543</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>91850</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>4.3549265106151338E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>4.354926510615134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>116446</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>4.2938357693694928E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>4.2938357693694931</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>263407</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>3.796406321775807E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>3.7964063217758071</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>147790</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>3.3831788348332092E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3831788348332092</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>3.0544454908748441E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0544454908748442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>577212</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>2.7719451432056158E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7719451432056159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>112055</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>75167</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>2.6607420809663814E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6607420809663815</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>127998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>2.3437866216659635E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>2.3437866216659637</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>28</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>133573</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>1.4973085878134053E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4973085878134054</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>71544</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>80055</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>1.2491412154144025E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2491412154144026</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>150417</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>6.6481847131640709E-4</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>0.66481847131640714</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>52</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>365</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA044CB7-7C99-41D1-BD9D-1303CF3D17D2}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>163</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>6.2750714126225182E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>62.750714126225184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>177</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>5.0616549609938E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>50.616549609937998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>72</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>3.0682559095887258E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>30.682559095887257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>287695</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>2.5026503762665322E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>25.026503762665321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>167794</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>2.3242785796869971E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>23.24278579686997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>2.2827058320705598E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>22.8270583207056</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>209244</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>2.2461814914645103E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>22.461814914645103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>205</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.1829434383382369E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>21.82943438338237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>67</v>
+      </c>
+      <c r="D10">
+        <v>342296</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>1.957370229275247E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>19.573702292752468</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>1.8211895403014069E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>18.211895403014069</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>97</v>
+      </c>
+      <c r="D12">
+        <v>585470</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>1.6567885630348268E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>16.567885630348268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>301185</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>1.6269070504839219E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>16.26907050483922</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>1.0361658901590144E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>10.361658901590143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>52</v>
+      </c>
+      <c r="D15">
+        <v>519212</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>1.0015176844911135E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>10.015176844911135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>235836</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>9.7525399006088975E-3</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>9.7525399006088982</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>9.6709035481226356E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>9.6709035481226362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>54709</v>
+      </c>
+      <c r="E18">
         <f>100*C18/D18</f>
         <v>9.1392641064541487E-3</v>
       </c>
@@ -7158,18 +8600,18 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19">
         <v>739575</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>8.9240442145826996E-3</v>
+        <v>9.0592570057127404E-3</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>8.9240442145827004</v>
+        <v>9.0592570057127411</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -7202,18 +8644,18 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21">
         <v>742652</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>7.9445015969794742E-3</v>
+        <v>8.0791541664198031E-3</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>7.9445015969794746</v>
+        <v>8.0791541664198032</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -7224,62 +8666,62 @@
         <v>18</v>
       </c>
       <c r="C22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22">
         <v>583702</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>7.8807336620398769E-3</v>
+        <v>8.0520539590407426E-3</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>7.8807336620398774</v>
+        <v>8.0520539590407427</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C23">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D23">
-        <v>192518</v>
+        <v>75168</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>6.7526153398643242E-3</v>
+        <v>7.9821200510855686E-3</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>6.7526153398643238</v>
+        <v>7.9821200510855688</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>75168</v>
+        <v>192518</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>6.6517667092379738E-3</v>
+        <v>7.2720472890846566E-3</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>6.6517667092379735</v>
+        <v>7.2720472890846564</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -7290,172 +8732,172 @@
         <v>20</v>
       </c>
       <c r="C25">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <v>683365</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>6.585060692309381E-3</v>
+        <v>6.7313953743607007E-3</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>6.5850606923093808</v>
+        <v>6.7313953743607007</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D26">
-        <v>125851</v>
+        <v>354425</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>6.3567234269095996E-3</v>
+        <v>6.4893842138675321E-3</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>6.3567234269095998</v>
+        <v>6.4893842138675319</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C27">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D27">
-        <v>695797</v>
+        <v>125851</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>6.1799634088678165E-3</v>
+        <v>6.3567234269095996E-3</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>6.1799634088678168</v>
+        <v>6.3567234269095998</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C28">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28">
-        <v>218775</v>
+        <v>190006</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>5.9421780367957949E-3</v>
+        <v>6.3155900339989263E-3</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>5.942178036795795</v>
+        <v>6.3155900339989266</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D29">
-        <v>190006</v>
+        <v>206268</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>5.7892908644990157E-3</v>
+        <v>6.3024802683886985E-3</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>5.7892908644990158</v>
+        <v>6.3024802683886989</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C30">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D30">
-        <v>354425</v>
+        <v>695797</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>5.6429427946674193E-3</v>
+        <v>6.1799634088678165E-3</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>5.6429427946674195</v>
+        <v>6.1799634088678168</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D31">
-        <v>206268</v>
+        <v>218775</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>5.3328679194058213E-3</v>
+        <v>5.9421780367957949E-3</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>5.3328679194058211</v>
+        <v>5.942178036795795</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C32">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D32">
-        <v>434170</v>
+        <v>91850</v>
       </c>
       <c r="E32">
         <f>100*C32/D32</f>
-        <v>5.0671395996959717E-3</v>
+        <v>5.4436581382689168E-3</v>
       </c>
       <c r="F32" s="1">
         <f>E32*1000</f>
-        <v>5.0671395996959721</v>
+        <v>5.4436581382689164</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -7466,194 +8908,194 @@
         <v>28</v>
       </c>
       <c r="C33">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>239824</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>5.0036693575288543E-3</v>
+        <v>5.4206418039895923E-3</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>5.003669357528854</v>
+        <v>5.4206418039895921</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D34">
-        <v>84247</v>
+        <v>263407</v>
       </c>
       <c r="E34">
         <f>100*C34/D34</f>
-        <v>4.7479435469512266E-3</v>
+        <v>5.3149688504861301E-3</v>
       </c>
       <c r="F34" s="1">
         <f>E34*1000</f>
-        <v>4.7479435469512268</v>
+        <v>5.3149688504861299</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D35">
-        <v>148350</v>
+        <v>434170</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>4.7185709470845974E-3</v>
+        <v>5.2974641269548798E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>4.7185709470845971</v>
+        <v>5.2974641269548801</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D36">
-        <v>180822</v>
+        <v>116446</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>4.4242404132240542E-3</v>
+        <v>5.1526029232433915E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>4.4242404132240543</v>
+        <v>5.1526029232433919</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
       <c r="D37">
-        <v>91850</v>
+        <v>84247</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>4.3549265106151338E-3</v>
+        <v>4.7479435469512266E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>4.354926510615134</v>
+        <v>4.7479435469512268</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D38">
-        <v>116446</v>
+        <v>147790</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>4.2938357693694928E-3</v>
+        <v>4.7364503687664927E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>4.2938357693694931</v>
+        <v>4.7364503687664925</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C39">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D39">
-        <v>263407</v>
+        <v>148350</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>3.796406321775807E-3</v>
+        <v>4.7185709470845974E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>3.7964063217758071</v>
+        <v>4.7185709470845971</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D40">
-        <v>147790</v>
+        <v>180822</v>
       </c>
       <c r="E40">
         <f>100*C40/D40</f>
-        <v>3.3831788348332092E-3</v>
+        <v>4.4242404132240542E-3</v>
       </c>
       <c r="F40" s="1">
         <f>E40*1000</f>
-        <v>3.3831788348332092</v>
+        <v>4.4242404132240543</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>196435</v>
+        <v>75167</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>3.0544454908748441E-3</v>
+        <v>3.9911131214495719E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>3.0544454908748442</v>
+        <v>3.9911131214495721</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -7664,62 +9106,62 @@
         <v>23</v>
       </c>
       <c r="C42">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D42">
         <v>577212</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>2.7719451432056158E-3</v>
+        <v>3.2916848575566689E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>2.7719451432056159</v>
+        <v>3.2916848575566688</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D43">
-        <v>112055</v>
+        <v>196435</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>2.6772567042969968E-3</v>
+        <v>3.0544454908748441E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>2.677256704296997</v>
+        <v>3.0544454908748442</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>75167</v>
+        <v>112055</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>2.6607420809663814E-3</v>
+        <v>2.6772567042969968E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>2.6607420809663815</v>
+        <v>2.677256704296997</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -7746,90 +9188,90 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>133573</v>
+        <v>150417</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>1.4973085878134053E-3</v>
+        <v>1.9944554139492213E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>1.4973085878134054</v>
+        <v>1.9944554139492212</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47">
-        <v>71544</v>
+        <v>133573</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>1.3977412501397742E-3</v>
+        <v>1.4973085878134053E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>1.3977412501397741</v>
+        <v>1.4973085878134054</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <v>80055</v>
+        <v>71544</v>
       </c>
       <c r="E48">
         <f>100*C48/D48</f>
-        <v>1.2491412154144025E-3</v>
+        <v>1.3977412501397742E-3</v>
       </c>
       <c r="F48" s="1">
         <f>E48*1000</f>
-        <v>1.2491412154144026</v>
+        <v>1.3977412501397741</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>150417</v>
+        <v>80055</v>
       </c>
       <c r="E49">
         <f>100*C49/D49</f>
-        <v>6.6481847131640709E-4</v>
+        <v>1.2491412154144025E-3</v>
       </c>
       <c r="F49" s="1">
         <f>E49*1000</f>
-        <v>0.66481847131640714</v>
+        <v>1.2491412154144026</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -8148,7 +9590,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -8162,7 +9604,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: 2020/4/13 and 2020/4/14 data added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2ED294-6CA9-486C-A2C9-87F1E27F9011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D76D860-B4DA-4191-9FFB-E9C36372ECC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="760" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="11" activeTab="12" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="14240" yWindow="1120" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="12" activeTab="14" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="2020年4月11日" sheetId="12" r:id="rId12"/>
     <sheet name="2020年4月12日" sheetId="13" r:id="rId13"/>
     <sheet name="2020年4月13日" sheetId="14" r:id="rId14"/>
+    <sheet name="2020年4月14日" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -34,6 +35,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'2020年4月11日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'2020年4月12日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'2020年4月13日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'2020年4月14日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -6745,7 +6747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE7700A-3136-495F-BF2B-878EB2092195}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -8232,11 +8234,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>6.2750714126225182E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>62.750714126225184</v>
       </c>
     </row>
@@ -8254,11 +8256,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>5.0616549609938E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>50.616549609937998</v>
       </c>
     </row>
@@ -8276,11 +8278,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>3.0682559095887258E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>30.682559095887257</v>
       </c>
     </row>
@@ -8298,11 +8300,11 @@
         <v>287695</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>2.5026503762665322E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>25.026503762665321</v>
       </c>
     </row>
@@ -8320,11 +8322,11 @@
         <v>167794</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.3242785796869971E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>23.24278579686997</v>
       </c>
     </row>
@@ -8342,11 +8344,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2.2827058320705598E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>22.8270583207056</v>
       </c>
     </row>
@@ -8364,11 +8366,11 @@
         <v>209244</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.2461814914645103E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>22.461814914645103</v>
       </c>
     </row>
@@ -8386,11 +8388,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.1829434383382369E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>21.82943438338237</v>
       </c>
     </row>
@@ -8408,11 +8410,11 @@
         <v>342296</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.957370229275247E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>19.573702292752468</v>
       </c>
     </row>
@@ -8430,11 +8432,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.8211895403014069E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>18.211895403014069</v>
       </c>
     </row>
@@ -8452,11 +8454,11 @@
         <v>585470</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.6567885630348268E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>16.567885630348268</v>
       </c>
     </row>
@@ -8474,11 +8476,11 @@
         <v>301185</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.6269070504839219E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>16.26907050483922</v>
       </c>
     </row>
@@ -8496,11 +8498,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>1.0361658901590144E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>10.361658901590143</v>
       </c>
     </row>
@@ -8518,11 +8520,11 @@
         <v>519212</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>1.0015176844911135E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>10.015176844911135</v>
       </c>
     </row>
@@ -8540,11 +8542,11 @@
         <v>235836</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>9.7525399006088975E-3</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>9.7525399006088982</v>
       </c>
     </row>
@@ -8562,11 +8564,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>9.6709035481226356E-3</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>9.6709035481226362</v>
       </c>
     </row>
@@ -8584,11 +8586,11 @@
         <v>54709</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -8606,11 +8608,11 @@
         <v>739575</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>9.0592570057127404E-3</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>9.0592570057127411</v>
       </c>
     </row>
@@ -8628,11 +8630,11 @@
         <v>83826</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>8.3506310691193655E-3</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>8.3506310691193661</v>
       </c>
     </row>
@@ -8650,11 +8652,11 @@
         <v>742652</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>8.0791541664198031E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>8.0791541664198032</v>
       </c>
     </row>
@@ -8672,11 +8674,11 @@
         <v>583702</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>8.0520539590407426E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>8.0520539590407427</v>
       </c>
     </row>
@@ -8694,11 +8696,11 @@
         <v>75168</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>7.9821200510855686E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>7.9821200510855688</v>
       </c>
     </row>
@@ -8716,11 +8718,11 @@
         <v>192518</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>7.2720472890846566E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>7.2720472890846564</v>
       </c>
     </row>
@@ -8738,11 +8740,11 @@
         <v>683365</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>6.7313953743607007E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>6.7313953743607007</v>
       </c>
     </row>
@@ -8760,11 +8762,11 @@
         <v>354425</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>6.4893842138675321E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>6.4893842138675319</v>
       </c>
     </row>
@@ -8782,11 +8784,11 @@
         <v>125851</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>6.3567234269095996E-3</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3567234269095998</v>
       </c>
     </row>
@@ -8804,11 +8806,11 @@
         <v>190006</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>6.3155900339989263E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3155900339989266</v>
       </c>
     </row>
@@ -8826,11 +8828,11 @@
         <v>206268</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>6.3024802683886985E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3024802683886989</v>
       </c>
     </row>
@@ -8848,11 +8850,11 @@
         <v>695797</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>6.1799634088678165E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>6.1799634088678168</v>
       </c>
     </row>
@@ -8870,11 +8872,11 @@
         <v>218775</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>5.9421780367957949E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>5.942178036795795</v>
       </c>
     </row>
@@ -8892,11 +8894,11 @@
         <v>91850</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>5.4436581382689168E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>5.4436581382689164</v>
       </c>
     </row>
@@ -8914,11 +8916,11 @@
         <v>239824</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>5.4206418039895923E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>5.4206418039895921</v>
       </c>
     </row>
@@ -8936,11 +8938,11 @@
         <v>263407</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>5.3149688504861301E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>5.3149688504861299</v>
       </c>
     </row>
@@ -8958,11 +8960,11 @@
         <v>434170</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>5.2974641269548798E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>5.2974641269548801</v>
       </c>
     </row>
@@ -8980,11 +8982,11 @@
         <v>116446</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>5.1526029232433915E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>5.1526029232433919</v>
       </c>
     </row>
@@ -9002,11 +9004,11 @@
         <v>84247</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>4.7479435469512266E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>4.7479435469512268</v>
       </c>
     </row>
@@ -9024,11 +9026,11 @@
         <v>147790</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>4.7364503687664927E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>4.7364503687664925</v>
       </c>
     </row>
@@ -9046,11 +9048,11 @@
         <v>148350</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>4.7185709470845974E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>4.7185709470845971</v>
       </c>
     </row>
@@ -9068,6 +9070,1446 @@
         <v>180822</v>
       </c>
       <c r="E40">
+        <f t="shared" si="2"/>
+        <v>4.4242404132240542E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>4.4242404132240543</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>75167</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>3.9911131214495719E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9911131214495721</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <v>19</v>
+      </c>
+      <c r="D42">
+        <v>577212</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>3.2916848575566689E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>3.2916848575566688</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>196435</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>3.0544454908748441E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0544454908748442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>112055</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>127998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>2.3437866216659635E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>2.3437866216659637</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>36</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>150417</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>1.9944554139492213E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>1.9944554139492212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>133573</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>1.4973085878134053E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4973085878134054</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>71544</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>80055</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>1.2491412154144025E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2491412154144026</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>58</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>367</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0279B1E0-9B95-47ED-88B1-8A73E544E7D2}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>168</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>6.4675582657704483E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>64.675582657704481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>180</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>5.1474457230445428E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>51.474457230445431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>3.4517878982873167E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>34.517878982873164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>3.0394412195906887E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>30.394412195906888</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>2.6416865082813396E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>26.416865082813395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>104</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>2.5255468780355131E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>25.25546878035513</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>234</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>2.4917500710787681E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>24.917500710787682</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>49</v>
+      </c>
+      <c r="D9">
+        <v>209244</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.3417636825906599E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>23.417636825906598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>2.0585354516327176E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>20.585354516327175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>70</v>
+      </c>
+      <c r="D11">
+        <v>342296</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>2.0450136723771238E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>20.450136723771237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>107</v>
+      </c>
+      <c r="D12">
+        <v>585470</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>1.8275915076775923E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>18.275915076775924</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>65891</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>1.8211895403014069E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>18.211895403014069</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>1.295207362698768E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>12.95207362698768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>1.102461032242745E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>11.024610322427449</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>519212</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>1.0785575063750453E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>10.785575063750453</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>46</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.0110490073037302E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>10.110490073037301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>739575</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>9.6001081702329037E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>9.6001081702329039</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>54709</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>67</v>
+      </c>
+      <c r="D20">
+        <v>742652</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>9.0217221525021145E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>9.0217221525021145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>583702</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>8.5660148500433433E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>8.5660148500433433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>354425</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>8.4644141920011285E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>8.4644141920011293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>83826</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>8.3506310691193655E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>8.3506310691193661</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>75168</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>7.9821200510855686E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>7.9821200510855688</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="D25">
+        <v>683365</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>7.3167341025659784E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>7.3167341025659782</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>14</v>
+      </c>
+      <c r="D26">
+        <v>192518</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>7.2720472890846566E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>7.2720472890846564</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>47</v>
+      </c>
+      <c r="D27">
+        <v>695797</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>6.7548437259717991E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>6.7548437259717993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>91850</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>125851</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>6.3567234269095996E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>6.3567234269095998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>190006</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>6.3155900339989263E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>6.3155900339989266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>206268</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>6.3024802683886985E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>6.3024802683886989</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>239824</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>6.2545866969110683E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>6.2545866969110682</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>116446</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>6.0113700771172902E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>6.0113700771172907</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>218775</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>5.9421780367957949E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>5.942178036795795</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>263407</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>5.6946094826637109E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>5.6946094826637106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>24</v>
+      </c>
+      <c r="D36">
+        <v>434170</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>5.5277886542137869E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>5.5277886542137873</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>147790</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>5.4130861357331349E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>5.4130861357331348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>148350</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>5.3926525109538256E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>5.3926525109538259</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>84247</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>4.7479435469512266E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>4.7479435469512268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>180822</v>
+      </c>
+      <c r="E40">
         <f>100*C40/D40</f>
         <v>4.4242404132240542E-3</v>
       </c>
@@ -9106,18 +10548,18 @@
         <v>23</v>
       </c>
       <c r="C42">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D42">
         <v>577212</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>3.2916848575566689E-3</v>
+        <v>3.4649314290070201E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>3.2916848575566688</v>
+        <v>3.4649314290070201</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -9166,46 +10608,46 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>127998</v>
+        <v>150417</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>2.3437866216659635E-3</v>
+        <v>2.6592738852656284E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>2.3437866216659637</v>
+        <v>2.6592738852656286</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46">
-        <v>150417</v>
+        <v>127998</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>1.9944554139492213E-3</v>
+        <v>2.3437866216659635E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>1.9944554139492212</v>
+        <v>2.3437866216659637</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -9590,7 +11032,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -9604,7 +11046,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: 2020/04/15 and 2020/04/16 data added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D76D860-B4DA-4191-9FFB-E9C36372ECC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C35AA4-BABE-46E4-A299-5C0B0DCD49BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14240" yWindow="1120" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="12" activeTab="14" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="12740" yWindow="920" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="13" activeTab="15" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="2020年4月12日" sheetId="13" r:id="rId13"/>
     <sheet name="2020年4月13日" sheetId="14" r:id="rId14"/>
     <sheet name="2020年4月14日" sheetId="15" r:id="rId15"/>
+    <sheet name="2020年4月15日" sheetId="16" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -36,6 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'2020年4月12日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'2020年4月13日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'2020年4月14日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'2020年4月15日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -8938,11 +8940,11 @@
         <v>263407</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>5.3149688504861301E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>5.3149688504861299</v>
       </c>
     </row>
@@ -9627,8 +9629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0279B1E0-9B95-47ED-88B1-8A73E544E7D2}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -9674,11 +9676,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>6.4675582657704483E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>64.675582657704481</v>
       </c>
     </row>
@@ -9696,11 +9698,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>5.1474457230445428E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>51.474457230445431</v>
       </c>
     </row>
@@ -9718,11 +9720,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>3.4517878982873167E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>34.517878982873164</v>
       </c>
     </row>
@@ -9740,11 +9742,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>3.0394412195906887E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>30.394412195906888</v>
       </c>
     </row>
@@ -9762,11 +9764,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.6416865082813396E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>26.416865082813395</v>
       </c>
     </row>
@@ -9784,11 +9786,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2.5255468780355131E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>25.25546878035513</v>
       </c>
     </row>
@@ -9806,11 +9808,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.4917500710787681E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>24.917500710787682</v>
       </c>
     </row>
@@ -9828,11 +9830,11 @@
         <v>209244</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.3417636825906599E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>23.417636825906598</v>
       </c>
     </row>
@@ -9850,11 +9852,11 @@
         <v>301185</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>2.0585354516327176E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>20.585354516327175</v>
       </c>
     </row>
@@ -9872,11 +9874,11 @@
         <v>342296</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>2.0450136723771238E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>20.450136723771237</v>
       </c>
     </row>
@@ -9894,11 +9896,11 @@
         <v>585470</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.8275915076775923E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>18.275915076775924</v>
       </c>
     </row>
@@ -9916,11 +9918,11 @@
         <v>65891</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.8211895403014069E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>18.211895403014069</v>
       </c>
     </row>
@@ -9938,11 +9940,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>1.295207362698768E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>12.95207362698768</v>
       </c>
     </row>
@@ -9960,11 +9962,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>1.102461032242745E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>11.024610322427449</v>
       </c>
     </row>
@@ -9982,11 +9984,11 @@
         <v>519212</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.0785575063750453E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>10.785575063750453</v>
       </c>
     </row>
@@ -10004,11 +10006,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.0110490073037302E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>10.110490073037301</v>
       </c>
     </row>
@@ -10026,11 +10028,11 @@
         <v>739575</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>9.6001081702329037E-3</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>9.6001081702329039</v>
       </c>
     </row>
@@ -10048,11 +10050,11 @@
         <v>54709</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -10070,11 +10072,11 @@
         <v>742652</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>9.0217221525021145E-3</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>9.0217221525021145</v>
       </c>
     </row>
@@ -10092,11 +10094,11 @@
         <v>583702</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>8.5660148500433433E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>8.5660148500433433</v>
       </c>
     </row>
@@ -10114,11 +10116,11 @@
         <v>354425</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>8.4644141920011285E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>8.4644141920011293</v>
       </c>
     </row>
@@ -10136,11 +10138,11 @@
         <v>83826</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>8.3506310691193655E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>8.3506310691193661</v>
       </c>
     </row>
@@ -10158,11 +10160,11 @@
         <v>75168</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>7.9821200510855686E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>7.9821200510855688</v>
       </c>
     </row>
@@ -10180,11 +10182,11 @@
         <v>683365</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>7.3167341025659784E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>7.3167341025659782</v>
       </c>
     </row>
@@ -10202,11 +10204,11 @@
         <v>192518</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>7.2720472890846566E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>7.2720472890846564</v>
       </c>
     </row>
@@ -10224,11 +10226,11 @@
         <v>695797</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>6.7548437259717991E-3</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>6.7548437259717993</v>
       </c>
     </row>
@@ -10246,11 +10248,11 @@
         <v>91850</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>6.5323897659226998E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>6.5323897659226997</v>
       </c>
     </row>
@@ -10268,11 +10270,11 @@
         <v>125851</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>6.3567234269095996E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3567234269095998</v>
       </c>
     </row>
@@ -10290,11 +10292,11 @@
         <v>190006</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>6.3155900339989263E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3155900339989266</v>
       </c>
     </row>
@@ -10312,11 +10314,11 @@
         <v>206268</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>6.3024802683886985E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>6.3024802683886989</v>
       </c>
     </row>
@@ -10334,11 +10336,11 @@
         <v>239824</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>6.2545866969110683E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>6.2545866969110682</v>
       </c>
     </row>
@@ -10356,11 +10358,11 @@
         <v>116446</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>6.0113700771172902E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>6.0113700771172907</v>
       </c>
     </row>
@@ -10378,11 +10380,11 @@
         <v>218775</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>5.9421780367957949E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>5.942178036795795</v>
       </c>
     </row>
@@ -10400,11 +10402,11 @@
         <v>263407</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>5.6946094826637109E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>5.6946094826637106</v>
       </c>
     </row>
@@ -10422,11 +10424,11 @@
         <v>434170</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>5.5277886542137869E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>5.5277886542137873</v>
       </c>
     </row>
@@ -10444,11 +10446,11 @@
         <v>147790</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>5.4130861357331349E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>5.4130861357331348</v>
       </c>
     </row>
@@ -10466,11 +10468,11 @@
         <v>148350</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>5.3926525109538256E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>5.3926525109538259</v>
       </c>
     </row>
@@ -10488,6 +10490,1446 @@
         <v>84247</v>
       </c>
       <c r="E39">
+        <f t="shared" si="2"/>
+        <v>4.7479435469512266E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>4.7479435469512268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>180822</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>4.4242404132240542E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>4.4242404132240543</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>75167</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>3.9911131214495719E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9911131214495721</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <v>20</v>
+      </c>
+      <c r="D42">
+        <v>577212</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>3.4649314290070201E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>3.4649314290070201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>196435</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>3.0544454908748441E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0544454908748442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>112055</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>36</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>150417</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>2.6592738852656284E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6592738852656286</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>37</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>127998</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>2.3437866216659635E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>2.3437866216659637</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>133573</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>1.4973085878134053E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4973085878134054</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>71544</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>80055</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>1.2491412154144025E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2491412154144026</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>60</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>371</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2174E841-C080-46E6-85BA-8F553C4992EC}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>172</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>6.6215477482887919E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>66.21547748288792</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>187</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>5.347624167829608E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>53.476241678296077</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>89</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>3.7927052215749525E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>37.927052215749526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>3.1586349929079702E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>31.586349929079702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>2.7807226402961471E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>27.807226402961472</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>243</v>
+      </c>
+      <c r="D7">
+        <v>939099</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>2.5875866122741054E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>25.875866122741055</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>104</v>
+      </c>
+      <c r="D8">
+        <v>411792</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>2.5255468780355131E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>25.25546878035513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>65891</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.4282527204018758E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>24.282527204018759</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <v>209244</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>2.3417636825906599E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>23.417636825906598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>77</v>
+      </c>
+      <c r="D11">
+        <v>342296</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>2.2495150396148363E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>22.495150396148361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>301185</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>2.1581420057439779E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>21.581420057439779</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>115</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>1.9642338633918049E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>19.642338633918047</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>1.3322132873473043E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>13.322132873473043</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>1.1872657270306484E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>11.872657270306483</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>57</v>
+      </c>
+      <c r="D16">
+        <v>519212</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>1.0978174618460282E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>10.978174618460281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="D17">
+        <v>742652</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.0772205555226405E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>10.772205555226405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>48</v>
+      </c>
+      <c r="D18">
+        <v>454973</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.0550076597951966E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>10.550076597951966</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>77</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.0411384917013149E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>10.411384917013148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>83826</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>9.5435783647078477E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>9.543578364707848</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>116446</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>9.4464386926128852E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>9.4464386926128849</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>54709</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>51</v>
+      </c>
+      <c r="D23">
+        <v>583702</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>8.7373351470442107E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>8.7373351470442113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>30</v>
+      </c>
+      <c r="D24">
+        <v>354425</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>8.4644141920011285E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>8.4644141920011293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>239824</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>8.3394489292147583E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>8.3394489292147576</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>192518</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>8.3109111875253223E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>8.3109111875253223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>147790</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>8.1196292035997028E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>8.1196292035997022</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>75168</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>7.9821200510855686E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>7.9821200510855688</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>263407</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>7.5928126435516139E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>7.5928126435516141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>52</v>
+      </c>
+      <c r="D30">
+        <v>695797</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>7.4734441223517781E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>7.4734441223517782</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>51</v>
+      </c>
+      <c r="D31">
+        <v>683365</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>7.463068784617298E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>7.4630687846172981</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>148350</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>6.740815638692282E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>6.7408156386922817</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>91850</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>125851</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>6.3567234269095996E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>6.3567234269095998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>12</v>
+      </c>
+      <c r="D35">
+        <v>190006</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>6.3155900339989263E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>6.3155900339989266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>206268</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>6.3024802683886985E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>6.3024802683886989</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>218775</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>5.9421780367957949E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>5.942178036795795</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>434170</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>5.758113181472695E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>5.7581131814726954</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>84247</v>
+      </c>
+      <c r="E39">
         <f>100*C39/D39</f>
         <v>4.7479435469512266E-3</v>
       </c>
@@ -10520,200 +11962,200 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>75167</v>
+        <v>196435</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>3.9911131214495719E-3</v>
+        <v>4.0725939878331254E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>3.9911131214495721</v>
+        <v>4.072593987833125</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C42">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>577212</v>
+        <v>75167</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>3.4649314290070201E-3</v>
+        <v>3.9911131214495719E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>3.4649314290070201</v>
+        <v>3.9911131214495721</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43">
-        <v>196435</v>
+        <v>127998</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>3.0544454908748441E-3</v>
+        <v>3.9063110361099388E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>3.0544454908748442</v>
+        <v>3.9063110361099387</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D44">
-        <v>112055</v>
+        <v>577212</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>2.6772567042969968E-3</v>
+        <v>3.6381780004573708E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>2.677256704296997</v>
+        <v>3.6381780004573709</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45">
-        <v>150417</v>
+        <v>112055</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>2.6592738852656284E-3</v>
+        <v>2.6772567042969968E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>2.6592738852656286</v>
+        <v>2.677256704296997</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D46">
-        <v>127998</v>
+        <v>150417</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>2.3437866216659635E-3</v>
+        <v>2.6592738852656284E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>2.3437866216659637</v>
+        <v>2.6592738852656286</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
       <c r="D47">
-        <v>133573</v>
+        <v>80055</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>1.4973085878134053E-3</v>
+        <v>2.498282430828805E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>1.4973085878134054</v>
+        <v>2.4982824308288052</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48">
-        <v>71544</v>
+        <v>133573</v>
       </c>
       <c r="E48">
         <f>100*C48/D48</f>
-        <v>1.3977412501397742E-3</v>
+        <v>1.4973085878134053E-3</v>
       </c>
       <c r="F48" s="1">
         <f>E48*1000</f>
-        <v>1.3977412501397741</v>
+        <v>1.4973085878134054</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>80055</v>
+        <v>71544</v>
       </c>
       <c r="E49">
         <f>100*C49/D49</f>
-        <v>1.2491412154144025E-3</v>
+        <v>1.3977412501397742E-3</v>
       </c>
       <c r="F49" s="1">
         <f>E49*1000</f>
-        <v>1.2491412154144026</v>
+        <v>1.3977412501397741</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -11032,7 +12474,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -11046,7 +12488,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: data 2020/04/16 and 2020/04/17 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C35AA4-BABE-46E4-A299-5C0B0DCD49BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1072B889-DB9E-4785-8BC7-932009C30B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12740" yWindow="920" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="13" activeTab="15" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="2510" yWindow="1390" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="14" activeTab="16" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="2020年4月13日" sheetId="14" r:id="rId14"/>
     <sheet name="2020年4月14日" sheetId="15" r:id="rId15"/>
     <sheet name="2020年4月15日" sheetId="16" r:id="rId16"/>
+    <sheet name="2020年4月16日" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -38,6 +39,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'2020年4月13日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'2020年4月14日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'2020年4月15日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'2020年4月16日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -10380,11 +10382,11 @@
         <v>218775</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>5.9421780367957949E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>5.942178036795795</v>
       </c>
     </row>
@@ -11069,7 +11071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2174E841-C080-46E6-85BA-8F553C4992EC}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -11116,11 +11118,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>6.6215477482887919E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>66.21547748288792</v>
       </c>
     </row>
@@ -11138,11 +11140,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>5.347624167829608E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>53.476241678296077</v>
       </c>
     </row>
@@ -11160,11 +11162,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>3.7927052215749525E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>37.927052215749526</v>
       </c>
     </row>
@@ -11182,11 +11184,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>3.1586349929079702E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>31.586349929079702</v>
       </c>
     </row>
@@ -11204,11 +11206,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.7807226402961471E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>27.807226402961472</v>
       </c>
     </row>
@@ -11226,11 +11228,11 @@
         <v>939099</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2.5875866122741054E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>25.875866122741055</v>
       </c>
     </row>
@@ -11248,11 +11250,11 @@
         <v>411792</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.5255468780355131E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>25.25546878035513</v>
       </c>
     </row>
@@ -11270,11 +11272,11 @@
         <v>65891</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.4282527204018758E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>24.282527204018759</v>
       </c>
     </row>
@@ -11292,11 +11294,11 @@
         <v>209244</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>2.3417636825906599E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>23.417636825906598</v>
       </c>
     </row>
@@ -11314,11 +11316,11 @@
         <v>342296</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>2.2495150396148363E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>22.495150396148361</v>
       </c>
     </row>
@@ -11336,11 +11338,11 @@
         <v>301185</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>2.1581420057439779E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>21.581420057439779</v>
       </c>
     </row>
@@ -11358,11 +11360,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.9642338633918049E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>19.642338633918047</v>
       </c>
     </row>
@@ -11380,11 +11382,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>1.3322132873473043E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>13.322132873473043</v>
       </c>
     </row>
@@ -11402,11 +11404,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>1.1872657270306484E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>11.872657270306483</v>
       </c>
     </row>
@@ -11424,11 +11426,11 @@
         <v>519212</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.0978174618460282E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>10.978174618460281</v>
       </c>
     </row>
@@ -11446,11 +11448,11 @@
         <v>742652</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.0772205555226405E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>10.772205555226405</v>
       </c>
     </row>
@@ -11468,11 +11470,11 @@
         <v>454973</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.0550076597951966E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>10.550076597951966</v>
       </c>
     </row>
@@ -11490,11 +11492,11 @@
         <v>739575</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.0411384917013149E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>10.411384917013148</v>
       </c>
     </row>
@@ -11512,11 +11514,11 @@
         <v>83826</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>9.5435783647078477E-3</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>9.543578364707848</v>
       </c>
     </row>
@@ -11534,11 +11536,11 @@
         <v>116446</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>9.4464386926128852E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>9.4464386926128849</v>
       </c>
     </row>
@@ -11556,11 +11558,11 @@
         <v>54709</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -11578,11 +11580,11 @@
         <v>583702</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>8.7373351470442107E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>8.7373351470442113</v>
       </c>
     </row>
@@ -11600,11 +11602,11 @@
         <v>354425</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>8.4644141920011285E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>8.4644141920011293</v>
       </c>
     </row>
@@ -11622,11 +11624,11 @@
         <v>239824</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>8.3394489292147583E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>8.3394489292147576</v>
       </c>
     </row>
@@ -11644,11 +11646,11 @@
         <v>192518</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>8.3109111875253223E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>8.3109111875253223</v>
       </c>
     </row>
@@ -11666,11 +11668,11 @@
         <v>147790</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>8.1196292035997028E-3</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>8.1196292035997022</v>
       </c>
     </row>
@@ -11688,11 +11690,11 @@
         <v>75168</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>7.9821200510855686E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>7.9821200510855688</v>
       </c>
     </row>
@@ -11710,11 +11712,11 @@
         <v>263407</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>7.5928126435516139E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>7.5928126435516141</v>
       </c>
     </row>
@@ -11732,11 +11734,11 @@
         <v>695797</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>7.4734441223517781E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>7.4734441223517782</v>
       </c>
     </row>
@@ -11754,11 +11756,11 @@
         <v>683365</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>7.463068784617298E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>7.4630687846172981</v>
       </c>
     </row>
@@ -11776,11 +11778,11 @@
         <v>148350</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>6.740815638692282E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>6.7408156386922817</v>
       </c>
     </row>
@@ -11798,11 +11800,11 @@
         <v>91850</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>6.5323897659226998E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>6.5323897659226997</v>
       </c>
     </row>
@@ -11820,11 +11822,11 @@
         <v>125851</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>6.3567234269095996E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>6.3567234269095998</v>
       </c>
     </row>
@@ -11842,11 +11844,11 @@
         <v>190006</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>6.3155900339989263E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>6.3155900339989266</v>
       </c>
     </row>
@@ -11864,11 +11866,11 @@
         <v>206268</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>6.3024802683886985E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>6.3024802683886989</v>
       </c>
     </row>
@@ -11886,11 +11888,11 @@
         <v>218775</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>5.9421780367957949E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>5.942178036795795</v>
       </c>
     </row>
@@ -11908,11 +11910,11 @@
         <v>434170</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>5.758113181472695E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>5.7581131814726954</v>
       </c>
     </row>
@@ -11930,11 +11932,11 @@
         <v>84247</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>4.7479435469512266E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>4.7479435469512268</v>
       </c>
     </row>
@@ -11952,11 +11954,11 @@
         <v>180822</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>4.4242404132240542E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>4.4242404132240543</v>
       </c>
     </row>
@@ -11974,11 +11976,11 @@
         <v>196435</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>4.0725939878331254E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>4.072593987833125</v>
       </c>
     </row>
@@ -11996,6 +11998,1446 @@
         <v>75167</v>
       </c>
       <c r="E42">
+        <f t="shared" si="2"/>
+        <v>3.9911131214495719E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9911131214495721</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>127998</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>3.9063110361099388E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9063110361099387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44">
+        <v>21</v>
+      </c>
+      <c r="D44">
+        <v>577212</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>3.6381780004573708E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>3.6381780004573709</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>30</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>112055</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>36</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>150417</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>2.6592738852656284E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6592738852656286</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>80055</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>2.498282430828805E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>2.4982824308288052</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>28</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>133573</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>1.4973085878134053E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4973085878134054</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>71544</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>377</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD947B9-62D7-431E-B63E-6F0974B79D10}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>179</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>6.8910293426958938E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>68.910293426958944</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>205</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>5.8623687401340621E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>58.623687401340618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>94</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>4.0057785486297251E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>40.057785486297249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>3.3374256528838936E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>33.374256528838934</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>83</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>2.8849997393072525E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>28.849997393072524</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>65891</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>2.7317843104521101E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>27.317843104521103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>111</v>
+      </c>
+      <c r="D8">
+        <v>411792</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>2.6955356102109803E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>26.955356102109803</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>247</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.6301806305831441E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>26.301806305831441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>53</v>
+      </c>
+      <c r="D10">
+        <v>209244</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>2.5329280648429583E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>25.329280648429584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>301185</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>2.357355113966499E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>23.573551139664989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>79</v>
+      </c>
+      <c r="D12">
+        <v>342296</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>2.3079440016827543E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>23.079440016827544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>2.0496353357131878E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>20.496353357131877</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>1.739278458481203E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>17.392784584812031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>1.5264845061822623E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>15.264845061822623</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>59</v>
+      </c>
+      <c r="D16">
+        <v>454973</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>1.2967802484982626E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>12.967802484982625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>88</v>
+      </c>
+      <c r="D17">
+        <v>742652</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.1849426110749045E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>11.849426110749045</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>519212</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.1363373727879942E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>11.363373727879942</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>83826</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.0736525660296328E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>10.736525660296328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>79</v>
+      </c>
+      <c r="D20">
+        <v>739575</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.0681810499273232E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>10.681810499273231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>354425</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>9.5930027509346129E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>9.5930027509346125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>116446</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>9.4464386926128852E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>9.4464386926128849</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>18</v>
+      </c>
+      <c r="D23">
+        <v>192518</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>9.3497750859659872E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>9.3497750859659874</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>239824</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>9.1733938221362325E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>9.1733938221362319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>54709</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>147790</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>8.7962649705663441E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>8.7962649705663445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>51</v>
+      </c>
+      <c r="D27">
+        <v>583702</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>8.7373351470442107E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>8.7373351470442113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>695797</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>8.4794846772837489E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>8.4794846772837484</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>57</v>
+      </c>
+      <c r="D29">
+        <v>683365</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>8.3410768769252158E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>8.3410768769252162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>75168</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>7.9821200510855686E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>7.9821200510855688</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>263407</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>7.5928126435516139E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>7.5928126435516141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>206268</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>7.2720926173715748E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>7.272092617371575</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>6.740815638692282E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>6.7408156386922817</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>91850</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>125851</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>6.3567234269095996E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>6.3567234269095998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>6.3155900339989263E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>6.3155900339989266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>26</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>5.988437708731603E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>5.9884377087316034</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>218775</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>5.9421780367957949E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>5.942178036795795</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39">
+        <v>9</v>
+      </c>
+      <c r="D39">
+        <v>180822</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>4.9772704648770611E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>4.9772704648770612</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>84247</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>4.7479435469512266E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>4.7479435469512268</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>9</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>4.5816682363122663E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>4.5816682363122663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
         <f>100*C42/D42</f>
         <v>3.9911131214495719E-3</v>
       </c>
@@ -12034,18 +13476,18 @@
         <v>23</v>
       </c>
       <c r="C44">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D44">
         <v>577212</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>3.6381780004573708E-3</v>
+        <v>3.811424571907722E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>3.6381780004573709</v>
+        <v>3.8114245719077222</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -12072,46 +13514,46 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D46">
-        <v>150417</v>
+        <v>80055</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>2.6592738852656284E-3</v>
+        <v>2.498282430828805E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>2.6592738852656286</v>
+        <v>2.4982824308288052</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47">
-        <v>80055</v>
+        <v>150417</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>2.498282430828805E-3</v>
+        <v>1.9944554139492213E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>2.4982824308288052</v>
+        <v>1.9944554139492212</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -12474,7 +13916,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -12488,7 +13930,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: 2020/04/17 and 2020/04/18 data added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1072B889-DB9E-4785-8BC7-932009C30B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4738453-AF1A-4892-B1FB-7263F960B8FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2510" yWindow="1390" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="14" activeTab="16" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="718" firstSheet="9" activeTab="17" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="2020年4月14日" sheetId="15" r:id="rId15"/>
     <sheet name="2020年4月15日" sheetId="16" r:id="rId16"/>
     <sheet name="2020年4月16日" sheetId="17" r:id="rId17"/>
+    <sheet name="2020年4月17日" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -40,6 +41,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'2020年4月14日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'2020年4月15日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'2020年4月16日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'2020年4月17日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -3871,7 +3873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCADD9F-D6A4-429E-83CC-3643BB01A3B4}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -11822,11 +11824,11 @@
         <v>125851</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>6.3567234269095996E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>6.3567234269095998</v>
       </c>
     </row>
@@ -12511,7 +12513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD947B9-62D7-431E-B63E-6F0974B79D10}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -12558,11 +12560,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>6.8910293426958938E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>68.910293426958944</v>
       </c>
     </row>
@@ -12580,11 +12582,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>5.8623687401340621E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>58.623687401340618</v>
       </c>
     </row>
@@ -12602,11 +12604,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>4.0057785486297251E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>40.057785486297249</v>
       </c>
     </row>
@@ -12624,11 +12626,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>3.3374256528838936E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>33.374256528838934</v>
       </c>
     </row>
@@ -12646,11 +12648,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.8849997393072525E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>28.849997393072524</v>
       </c>
     </row>
@@ -12668,11 +12670,11 @@
         <v>65891</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2.7317843104521101E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>27.317843104521103</v>
       </c>
     </row>
@@ -12690,11 +12692,11 @@
         <v>411792</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.6955356102109803E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>26.955356102109803</v>
       </c>
     </row>
@@ -12712,11 +12714,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.6301806305831441E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>26.301806305831441</v>
       </c>
     </row>
@@ -12734,11 +12736,11 @@
         <v>209244</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>2.5329280648429583E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>25.329280648429584</v>
       </c>
     </row>
@@ -12756,11 +12758,11 @@
         <v>301185</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>2.357355113966499E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>23.573551139664989</v>
       </c>
     </row>
@@ -12778,11 +12780,11 @@
         <v>342296</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>2.3079440016827543E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>23.079440016827544</v>
       </c>
     </row>
@@ -12800,11 +12802,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>2.0496353357131878E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>20.496353357131877</v>
       </c>
     </row>
@@ -12822,11 +12824,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>1.739278458481203E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>17.392784584812031</v>
       </c>
     </row>
@@ -12844,11 +12846,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>1.5264845061822623E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>15.264845061822623</v>
       </c>
     </row>
@@ -12866,11 +12868,11 @@
         <v>454973</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.2967802484982626E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>12.967802484982625</v>
       </c>
     </row>
@@ -12888,11 +12890,11 @@
         <v>742652</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.1849426110749045E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>11.849426110749045</v>
       </c>
     </row>
@@ -12910,11 +12912,11 @@
         <v>519212</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.1363373727879942E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>11.363373727879942</v>
       </c>
     </row>
@@ -12932,11 +12934,11 @@
         <v>83826</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.0736525660296328E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>10.736525660296328</v>
       </c>
     </row>
@@ -12954,11 +12956,11 @@
         <v>739575</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.0681810499273232E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>10.681810499273231</v>
       </c>
     </row>
@@ -12976,11 +12978,11 @@
         <v>354425</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>9.5930027509346129E-3</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>9.5930027509346125</v>
       </c>
     </row>
@@ -12998,11 +13000,11 @@
         <v>116446</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>9.4464386926128852E-3</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>9.4464386926128849</v>
       </c>
     </row>
@@ -13020,11 +13022,11 @@
         <v>192518</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>9.3497750859659872E-3</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>9.3497750859659874</v>
       </c>
     </row>
@@ -13042,11 +13044,11 @@
         <v>239824</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>9.1733938221362325E-3</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1733938221362319</v>
       </c>
     </row>
@@ -13064,11 +13066,11 @@
         <v>54709</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -13086,11 +13088,11 @@
         <v>147790</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>8.7962649705663441E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>8.7962649705663445</v>
       </c>
     </row>
@@ -13108,11 +13110,11 @@
         <v>583702</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>8.7373351470442107E-3</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>8.7373351470442113</v>
       </c>
     </row>
@@ -13130,11 +13132,11 @@
         <v>695797</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>8.4794846772837489E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>8.4794846772837484</v>
       </c>
     </row>
@@ -13152,11 +13154,11 @@
         <v>683365</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>8.3410768769252158E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>8.3410768769252162</v>
       </c>
     </row>
@@ -13174,11 +13176,11 @@
         <v>75168</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>7.9821200510855686E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>7.9821200510855688</v>
       </c>
     </row>
@@ -13196,11 +13198,11 @@
         <v>263407</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>7.5928126435516139E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>7.5928126435516141</v>
       </c>
     </row>
@@ -13218,11 +13220,11 @@
         <v>206268</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>7.2720926173715748E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>7.272092617371575</v>
       </c>
     </row>
@@ -13240,11 +13242,11 @@
         <v>148350</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>6.740815638692282E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>6.7408156386922817</v>
       </c>
     </row>
@@ -13262,11 +13264,11 @@
         <v>91850</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>6.5323897659226998E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>6.5323897659226997</v>
       </c>
     </row>
@@ -13284,11 +13286,11 @@
         <v>125851</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>6.3567234269095996E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>6.3567234269095998</v>
       </c>
     </row>
@@ -13306,11 +13308,11 @@
         <v>190006</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>6.3155900339989263E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>6.3155900339989266</v>
       </c>
     </row>
@@ -13328,11 +13330,11 @@
         <v>434170</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>5.988437708731603E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>5.9884377087316034</v>
       </c>
     </row>
@@ -13350,11 +13352,11 @@
         <v>218775</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>5.9421780367957949E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>5.942178036795795</v>
       </c>
     </row>
@@ -13372,11 +13374,11 @@
         <v>180822</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>4.9772704648770611E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>4.9772704648770612</v>
       </c>
     </row>
@@ -13394,11 +13396,11 @@
         <v>84247</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>4.7479435469512266E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>4.7479435469512268</v>
       </c>
     </row>
@@ -13416,11 +13418,11 @@
         <v>196435</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>4.5816682363122663E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>4.5816682363122663</v>
       </c>
     </row>
@@ -13438,11 +13440,11 @@
         <v>75167</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>3.9911131214495719E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>3.9911131214495721</v>
       </c>
     </row>
@@ -13460,11 +13462,11 @@
         <v>127998</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>3.9063110361099388E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>3.9063110361099387</v>
       </c>
     </row>
@@ -13482,11 +13484,11 @@
         <v>577212</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>3.811424571907722E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>3.8114245719077222</v>
       </c>
     </row>
@@ -13504,11 +13506,11 @@
         <v>112055</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>2.6772567042969968E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>2.677256704296997</v>
       </c>
     </row>
@@ -13526,11 +13528,11 @@
         <v>80055</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>2.498282430828805E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>2.4982824308288052</v>
       </c>
     </row>
@@ -13548,11 +13550,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>1.9944554139492213E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>1.9944554139492212</v>
       </c>
     </row>
@@ -13570,11 +13572,11 @@
         <v>133573</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>1.4973085878134053E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>1.4973085878134054</v>
       </c>
     </row>
@@ -13592,11 +13594,11 @@
         <v>71544</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -13614,11 +13616,11 @@
         <v>57443</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13636,11 +13638,11 @@
         <v>32394</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13658,11 +13660,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13680,11 +13682,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13702,11 +13704,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13724,11 +13726,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13746,11 +13748,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13768,11 +13770,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13790,11 +13792,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13812,11 +13814,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13834,11 +13836,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13856,11 +13858,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13878,11 +13880,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13900,11 +13902,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13931,6 +13933,1446 @@
       </c>
       <c r="C65">
         <v>384</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B476F10-6476-4F38-9B49-4928118648F8}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>197</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>7.5839820140284425E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>75.839820140284431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>219</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>6.2627256297041939E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>62.627256297041939</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>105</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>4.4745398681502249E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>44.745398681502252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>3.4566194262011754E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>34.566194262011756</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>92</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>3.197831036340569E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>31.97831036340569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>123</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>2.9869448653689241E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>29.86944865368924</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>65891</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>2.8835501054772276E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>28.835501054772276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>259</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.7579626855102603E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>27.579626855102603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>79</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>2.6229725915965271E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>26.229725915965272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>209244</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>2.5329280648429583E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>25.329280648429584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>82</v>
+      </c>
+      <c r="D12">
+        <v>342296</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>2.3955874447846307E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>23.955874447846305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>127</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>2.1691973969631236E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>21.691973969631235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>1.7762843831297392E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>17.762843831297392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>39</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>1.6536915483641175E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>16.536915483641174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <v>454973</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>1.4066768797269289E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>14.066768797269289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>65</v>
+      </c>
+      <c r="D17">
+        <v>519212</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.2518971056138918E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>12.518971056138918</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>90</v>
+      </c>
+      <c r="D18">
+        <v>742652</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.2118731249629705E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>12.118731249629704</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>75168</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.1973180076628353E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>11.973180076628353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>147790</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.082617227146627E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>10.82617227146627</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>83826</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.0736525660296328E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>10.736525660296328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>79</v>
+      </c>
+      <c r="D22">
+        <v>739575</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.0681810499273232E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>10.681810499273231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>192518</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.0388638984406652E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>10.388638984406652</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>27</v>
+      </c>
+      <c r="D24">
+        <v>263407</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.0250297068794679E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>10.250297068794678</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>70</v>
+      </c>
+      <c r="D25">
+        <v>695797</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.0060405549319701E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>10.0604055493197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>354425</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>9.8751498906679835E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>9.8751498906679842</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>57</v>
+      </c>
+      <c r="D27">
+        <v>583702</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>9.765256929049412E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>9.7652569290494124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>239824</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>9.5903662685969705E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>9.5903662685969699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>683365</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>9.5117543333357729E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>9.511754333335773</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>116446</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>9.4464386926128852E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>9.4464386926128849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>54709</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <v>206268</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>8.7265111408458898E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>8.72651114084589</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>8.0889787664307385E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>8.0889787664307384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>180822</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>125851</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>7.1513138552732995E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>7.1513138552732993</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>6.841889203498837E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>6.8418892034988374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>91850</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>28</v>
+      </c>
+      <c r="D38">
+        <v>434170</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>6.4490867632494182E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>6.4490867632494187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>218775</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>5.9421780367957949E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>5.942178036795795</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>84247</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>5.9349294336890337E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>5.9349294336890335</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>75167</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>5.3214841619327628E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>5.3214841619327631</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>127998</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>4.6875732433319271E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>4.6875732433319275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>196435</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>4.5816682363122663E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>4.5816682363122663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44">
+        <v>23</v>
+      </c>
+      <c r="D44">
+        <v>577212</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>3.9846711433580732E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>3.984671143358073</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>32394</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>2.6592738852656284E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>2.6592738852656286</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>80055</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>2.498282430828805E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>2.4982824308288052</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>71544</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>57443</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>76</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>400</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: 2020/04/18 data and 2020/04/19 data added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4738453-AF1A-4892-B1FB-7263F960B8FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BA07A8-B5FF-4E69-94C2-69F41BFD7A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="718" firstSheet="9" activeTab="17" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="11400" yWindow="690" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="8" activeTab="18" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="2020年4月15日" sheetId="16" r:id="rId16"/>
     <sheet name="2020年4月16日" sheetId="17" r:id="rId17"/>
     <sheet name="2020年4月17日" sheetId="18" r:id="rId18"/>
+    <sheet name="2020年4月18日" sheetId="19" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -42,6 +43,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'2020年4月15日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'2020年4月16日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'2020年4月17日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'2020年4月18日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -13264,11 +13266,11 @@
         <v>91850</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>6.5323897659226998E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>6.5323897659226997</v>
       </c>
     </row>
@@ -13951,6 +13953,1446 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B476F10-6476-4F38-9B49-4928118648F8}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>197</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
+        <v>7.5839820140284425E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
+        <v>75.839820140284431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>219</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>6.2627256297041939E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
+        <v>62.627256297041939</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>105</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4.4745398681502249E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>44.745398681502252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>3.4566194262011754E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>34.566194262011756</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>92</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3.197831036340569E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>31.97831036340569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>123</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>2.9869448653689241E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>29.86944865368924</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>65891</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2.8835501054772276E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>28.835501054772276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>259</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2.7579626855102603E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>27.579626855102603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>79</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2.6229725915965271E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>26.229725915965272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>209244</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.5329280648429583E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>25.329280648429584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>82</v>
+      </c>
+      <c r="D12">
+        <v>342296</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2.3955874447846307E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>23.955874447846305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>127</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2.1691973969631236E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>21.691973969631235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>1.7762843831297392E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>17.762843831297392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>39</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1.6536915483641175E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>16.536915483641174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>64</v>
+      </c>
+      <c r="D16">
+        <v>454973</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.4066768797269289E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>14.066768797269289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>65</v>
+      </c>
+      <c r="D17">
+        <v>519212</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.2518971056138918E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>12.518971056138918</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>90</v>
+      </c>
+      <c r="D18">
+        <v>742652</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.2118731249629705E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>12.118731249629704</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>75168</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.1973180076628353E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>11.973180076628353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>147790</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1.082617227146627E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>10.82617227146627</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>83826</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.0736525660296328E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>10.736525660296328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>79</v>
+      </c>
+      <c r="D22">
+        <v>739575</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.0681810499273232E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>10.681810499273231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>192518</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.0388638984406652E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>10.388638984406652</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>27</v>
+      </c>
+      <c r="D24">
+        <v>263407</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.0250297068794679E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>10.250297068794678</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>70</v>
+      </c>
+      <c r="D25">
+        <v>695797</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.0060405549319701E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>10.0604055493197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>354425</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>9.8751498906679835E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>9.8751498906679842</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>57</v>
+      </c>
+      <c r="D27">
+        <v>583702</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>9.765256929049412E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>9.7652569290494124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>239824</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>9.5903662685969705E-3</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>9.5903662685969699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>683365</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>9.5117543333357729E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>9.511754333335773</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>116446</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>9.4464386926128852E-3</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4464386926128849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>54709</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <v>206268</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>8.7265111408458898E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>8.72651114084589</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>8.0889787664307385E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>8.0889787664307384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>180822</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>125851</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>7.1513138552732995E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1513138552732993</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>6.841889203498837E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>6.8418892034988374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>91850</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>28</v>
+      </c>
+      <c r="D38">
+        <v>434170</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>6.4490867632494182E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>6.4490867632494187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>218775</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>5.9421780367957949E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>5.942178036795795</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>84247</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>5.9349294336890337E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>5.9349294336890335</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>75167</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>5.3214841619327628E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3214841619327631</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>127998</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>4.6875732433319271E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6875732433319275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>196435</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>4.5816682363122663E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>4.5816682363122663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44">
+        <v>23</v>
+      </c>
+      <c r="D44">
+        <v>577212</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>3.9846711433580732E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>3.984671143358073</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>32394</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>2.6772567042969968E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>2.677256704296997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>2.6592738852656284E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6592738852656286</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>80055</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>2.498282430828805E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>2.4982824308288052</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>71544</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>57443</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>76</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>400</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BECCB3-37EB-4583-A175-894E90719EEE}">
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -13994,18 +15436,18 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="D2">
         <v>259758</v>
       </c>
       <c r="E2">
         <f>100*C2/D2</f>
-        <v>7.5839820140284425E-2</v>
+        <v>8.007453090953888E-2</v>
       </c>
       <c r="F2" s="1">
         <f>E2*1000</f>
-        <v>75.839820140284431</v>
+        <v>80.074530909538879</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14016,18 +15458,18 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="D3">
         <v>349688</v>
       </c>
       <c r="E3">
         <f>100*C3/D3</f>
-        <v>6.2627256297041939E-2</v>
+        <v>6.49150099517284E-2</v>
       </c>
       <c r="F3" s="1">
         <f>E3*1000</f>
-        <v>62.627256297041939</v>
+        <v>64.915009951728393</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14038,18 +15480,18 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D4">
         <v>234661</v>
       </c>
       <c r="E4">
         <f>100*C4/D4</f>
-        <v>4.4745398681502249E-2</v>
+        <v>4.8154571914378615E-2</v>
       </c>
       <c r="F4" s="1">
         <f>E4*1000</f>
-        <v>44.745398681502252</v>
+        <v>48.154571914378614</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14060,18 +15502,18 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>167794</v>
       </c>
       <c r="E5">
         <f>100*C5/D5</f>
-        <v>3.4566194262011754E-2</v>
+        <v>3.8737976328116618E-2</v>
       </c>
       <c r="F5" s="1">
         <f>E5*1000</f>
-        <v>34.566194262011756</v>
+        <v>38.737976328116616</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14082,18 +15524,18 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D6">
         <v>287695</v>
       </c>
       <c r="E6">
         <f>100*C6/D6</f>
-        <v>3.197831036340569E-2</v>
+        <v>3.2673491023479724E-2</v>
       </c>
       <c r="F6" s="1">
         <f>E6*1000</f>
-        <v>31.97831036340569</v>
+        <v>32.673491023479727</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14104,84 +15546,84 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D7">
         <v>411792</v>
       </c>
       <c r="E7">
         <f>100*C7/D7</f>
-        <v>2.9869448653689241E-2</v>
+        <v>3.156933597544391E-2</v>
       </c>
       <c r="F7" s="1">
         <f>E7*1000</f>
-        <v>29.86944865368924</v>
+        <v>31.569335975443909</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>19</v>
+        <v>277</v>
       </c>
       <c r="D8">
-        <v>65891</v>
+        <v>939099</v>
       </c>
       <c r="E8">
         <f>100*C8/D8</f>
-        <v>2.8835501054772276E-2</v>
+        <v>2.949635767900935E-2</v>
       </c>
       <c r="F8" s="1">
         <f>E8*1000</f>
-        <v>28.835501054772276</v>
+        <v>29.49635767900935</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>259</v>
+        <v>88</v>
       </c>
       <c r="D9">
-        <v>939099</v>
+        <v>301185</v>
       </c>
       <c r="E9">
         <f>100*C9/D9</f>
-        <v>2.7579626855102603E-2</v>
+        <v>2.9217922539303085E-2</v>
       </c>
       <c r="F9" s="1">
         <f>E9*1000</f>
-        <v>27.579626855102603</v>
+        <v>29.217922539303085</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>301185</v>
+        <v>65891</v>
       </c>
       <c r="E10">
         <f>100*C10/D10</f>
-        <v>2.6229725915965271E-2</v>
+        <v>2.8835501054772276E-2</v>
       </c>
       <c r="F10" s="1">
         <f>E10*1000</f>
-        <v>26.229725915965272</v>
+        <v>28.835501054772276</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14192,18 +15634,18 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D11">
         <v>209244</v>
       </c>
       <c r="E11">
         <f>100*C11/D11</f>
-        <v>2.5329280648429583E-2</v>
+        <v>2.6285102559691079E-2</v>
       </c>
       <c r="F11" s="1">
         <f>E11*1000</f>
-        <v>25.329280648429584</v>
+        <v>26.285102559691079</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14214,18 +15656,18 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D12">
         <v>342296</v>
       </c>
       <c r="E12">
         <f>100*C12/D12</f>
-        <v>2.3955874447846307E-2</v>
+        <v>2.4248019258185899E-2</v>
       </c>
       <c r="F12" s="1">
         <f>E12*1000</f>
-        <v>23.955874447846305</v>
+        <v>24.248019258185899</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14236,18 +15678,18 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D13">
         <v>585470</v>
       </c>
       <c r="E13">
         <f>100*C13/D13</f>
-        <v>2.1691973969631236E-2</v>
+        <v>2.2887594582130594E-2</v>
       </c>
       <c r="F13" s="1">
         <f>E13*1000</f>
-        <v>21.691973969631235</v>
+        <v>22.887594582130596</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14258,18 +15700,18 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>270227</v>
       </c>
       <c r="E14">
         <f>100*C14/D14</f>
-        <v>1.7762843831297392E-2</v>
+        <v>1.8873021570753476E-2</v>
       </c>
       <c r="F14" s="1">
         <f>E14*1000</f>
-        <v>17.762843831297392</v>
+        <v>18.873021570753476</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14280,18 +15722,18 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>235836</v>
       </c>
       <c r="E15">
         <f>100*C15/D15</f>
-        <v>1.6536915483641175E-2</v>
+        <v>1.7384962431520209E-2</v>
       </c>
       <c r="F15" s="1">
         <f>E15*1000</f>
-        <v>16.536915483641174</v>
+        <v>17.384962431520208</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14302,304 +15744,304 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>454973</v>
       </c>
       <c r="E16">
         <f>100*C16/D16</f>
-        <v>1.4066768797269289E-2</v>
+        <v>1.6924081209214611E-2</v>
       </c>
       <c r="F16" s="1">
         <f>E16*1000</f>
-        <v>14.066768797269289</v>
+        <v>16.924081209214613</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="D17">
-        <v>519212</v>
+        <v>742652</v>
       </c>
       <c r="E17">
         <f>100*C17/D17</f>
-        <v>1.2518971056138918E-2</v>
+        <v>1.3465256944033006E-2</v>
       </c>
       <c r="F17" s="1">
         <f>E17*1000</f>
-        <v>12.518971056138918</v>
+        <v>13.465256944033007</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D18">
-        <v>742652</v>
+        <v>519212</v>
       </c>
       <c r="E18">
         <f>100*C18/D18</f>
-        <v>1.2118731249629705E-2</v>
+        <v>1.3096769720268407E-2</v>
       </c>
       <c r="F18" s="1">
         <f>E18*1000</f>
-        <v>12.118731249629704</v>
+        <v>13.096769720268407</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D19">
-        <v>75168</v>
+        <v>147790</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>1.1973180076628353E-2</v>
+        <v>1.2856079572366196E-2</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>11.973180076628353</v>
+        <v>12.856079572366195</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D20">
-        <v>147790</v>
+        <v>354425</v>
       </c>
       <c r="E20">
         <f>100*C20/D20</f>
-        <v>1.082617227146627E-2</v>
+        <v>1.2414474148268321E-2</v>
       </c>
       <c r="F20" s="1">
         <f>E20*1000</f>
-        <v>10.82617227146627</v>
+        <v>12.414474148268321</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="D21">
-        <v>83826</v>
+        <v>739575</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>1.0736525660296328E-2</v>
+        <v>1.2169151201703681E-2</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>10.736525660296328</v>
+        <v>12.169151201703681</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C22">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="D22">
-        <v>739575</v>
+        <v>75168</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>1.0681810499273232E-2</v>
+        <v>1.1973180076628353E-2</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>10.681810499273231</v>
+        <v>11.973180076628353</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="D23">
-        <v>192518</v>
+        <v>695797</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>1.0388638984406652E-2</v>
+        <v>1.106644610425167E-2</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>10.388638984406652</v>
+        <v>11.066446104251671</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C24">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="D24">
-        <v>263407</v>
+        <v>583702</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>1.0250297068794679E-2</v>
+        <v>1.0964499008055481E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>10.250297068794678</v>
+        <v>10.96449900805548</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C25">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D25">
-        <v>695797</v>
+        <v>83826</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>1.0060405549319701E-2</v>
+        <v>1.0736525660296328E-2</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>10.0604055493197</v>
+        <v>10.736525660296328</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C26">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D26">
-        <v>354425</v>
+        <v>263407</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>9.8751498906679835E-3</v>
+        <v>1.062993770097226E-2</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>9.8751498906679842</v>
+        <v>10.62993770097226</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C27">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="D27">
-        <v>583702</v>
+        <v>192518</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>9.765256929049412E-3</v>
+        <v>1.0388638984406652E-2</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>9.7652569290494124</v>
+        <v>10.388638984406652</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D28">
-        <v>239824</v>
+        <v>683365</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>9.5903662685969705E-3</v>
+        <v>1.009709306154105E-2</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>9.5903662685969699</v>
+        <v>10.097093061541051</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C29">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="D29">
-        <v>683365</v>
+        <v>239824</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>9.5117543333357729E-3</v>
+        <v>1.0007338715057709E-2</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>9.511754333335773</v>
+        <v>10.007338715057708</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14626,46 +16068,46 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D31">
-        <v>54709</v>
+        <v>206268</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>9.1392641064541487E-3</v>
+        <v>9.2113173153373275E-3</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>9.1392641064541493</v>
+        <v>9.2113173153373271</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D32">
-        <v>206268</v>
+        <v>54709</v>
       </c>
       <c r="E32">
         <f>100*C32/D32</f>
-        <v>8.7265111408458898E-3</v>
+        <v>9.1392641064541487E-3</v>
       </c>
       <c r="F32" s="1">
         <f>E32*1000</f>
-        <v>8.72651114084589</v>
+        <v>9.1392641064541493</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14676,18 +16118,18 @@
         <v>24</v>
       </c>
       <c r="C33">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>148350</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>8.0889787664307385E-3</v>
+        <v>8.7630603302999658E-3</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>8.0889787664307384</v>
+        <v>8.7630603302999663</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14736,68 +16178,68 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D36">
-        <v>190006</v>
+        <v>434170</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>6.841889203498837E-3</v>
+        <v>6.9097358177672343E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>6.8418892034988374</v>
+        <v>6.9097358177672339</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D37">
-        <v>91850</v>
+        <v>190006</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>6.5323897659226998E-3</v>
+        <v>6.841889203498837E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>6.5323897659226997</v>
+        <v>6.8418892034988374</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C38">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D38">
-        <v>434170</v>
+        <v>91850</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>6.4490867632494182E-3</v>
+        <v>6.5323897659226998E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>6.4490867632494187</v>
+        <v>6.5323897659226997</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -14846,156 +16288,156 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D41">
-        <v>75167</v>
+        <v>196435</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>5.3214841619327628E-3</v>
+        <v>5.5998167332705472E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>5.3214841619327631</v>
+        <v>5.5998167332705471</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>127998</v>
+        <v>75167</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>4.6875732433319271E-3</v>
+        <v>5.3214841619327628E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>4.6875732433319275</v>
+        <v>5.3214841619327631</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D43">
-        <v>196435</v>
+        <v>577212</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>4.5816682363122663E-3</v>
+        <v>5.1973971435105302E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>4.5816682363122663</v>
+        <v>5.1973971435105302</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C44">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D44">
-        <v>577212</v>
+        <v>127998</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>3.9846711433580732E-3</v>
+        <v>4.6875732433319271E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>3.984671143358073</v>
+        <v>4.6875732433319275</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D45">
-        <v>32394</v>
+        <v>112055</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>3.0869914181638576E-3</v>
+        <v>4.4620945071616614E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>3.0869914181638576</v>
+        <v>4.4620945071616616</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D46">
-        <v>112055</v>
+        <v>150417</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>2.6772567042969968E-3</v>
+        <v>3.3240923565820354E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>2.677256704296997</v>
+        <v>3.3240923565820353</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>150417</v>
+        <v>32394</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>2.6592738852656284E-3</v>
+        <v>3.0869914181638576E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>2.6592738852656286</v>
+        <v>3.0869914181638576</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -15358,7 +16800,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -15372,7 +16814,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: 2020/04/19 and 2020/04/20 data added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BA07A8-B5FF-4E69-94C2-69F41BFD7A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C18FD2-8CD9-4D37-87C4-76F3AAE601E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="690" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="8" activeTab="18" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="12820" yWindow="970" windowWidth="12710" windowHeight="12420" tabRatio="718" firstSheet="17" activeTab="19" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="2020年4月16日" sheetId="17" r:id="rId17"/>
     <sheet name="2020年4月17日" sheetId="18" r:id="rId18"/>
     <sheet name="2020年4月18日" sheetId="19" r:id="rId19"/>
+    <sheet name="2020年4月19日" sheetId="20" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -44,6 +45,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'2020年4月16日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'2020年4月17日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'2020年4月18日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'2020年4月19日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
@@ -70,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -14706,11 +14708,11 @@
         <v>180822</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -15395,8 +15397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BECCB3-37EB-4583-A175-894E90719EEE}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -15442,11 +15444,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>8.007453090953888E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>80.074530909538879</v>
       </c>
     </row>
@@ -15464,11 +15466,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>6.49150099517284E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>64.915009951728393</v>
       </c>
     </row>
@@ -15486,11 +15488,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>4.8154571914378615E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>48.154571914378614</v>
       </c>
     </row>
@@ -15508,11 +15510,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>3.8737976328116618E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>38.737976328116616</v>
       </c>
     </row>
@@ -15530,11 +15532,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>3.2673491023479724E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>32.673491023479727</v>
       </c>
     </row>
@@ -15552,11 +15554,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.156933597544391E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>31.569335975443909</v>
       </c>
     </row>
@@ -15574,11 +15576,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.949635767900935E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>29.49635767900935</v>
       </c>
     </row>
@@ -15596,11 +15598,11 @@
         <v>301185</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.9217922539303085E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>29.217922539303085</v>
       </c>
     </row>
@@ -15618,11 +15620,11 @@
         <v>65891</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>2.8835501054772276E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>28.835501054772276</v>
       </c>
     </row>
@@ -15640,11 +15642,11 @@
         <v>209244</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>2.6285102559691079E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>26.285102559691079</v>
       </c>
     </row>
@@ -15662,11 +15664,11 @@
         <v>342296</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>2.4248019258185899E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>24.248019258185899</v>
       </c>
     </row>
@@ -15684,11 +15686,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>2.2887594582130594E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>22.887594582130596</v>
       </c>
     </row>
@@ -15706,11 +15708,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>1.8873021570753476E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>18.873021570753476</v>
       </c>
     </row>
@@ -15728,11 +15730,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>1.7384962431520209E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>17.384962431520208</v>
       </c>
     </row>
@@ -15750,11 +15752,11 @@
         <v>454973</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.6924081209214611E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>16.924081209214613</v>
       </c>
     </row>
@@ -15772,11 +15774,11 @@
         <v>742652</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.3465256944033006E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>13.465256944033007</v>
       </c>
     </row>
@@ -15794,11 +15796,11 @@
         <v>519212</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.3096769720268407E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>13.096769720268407</v>
       </c>
     </row>
@@ -15816,11 +15818,11 @@
         <v>147790</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.2856079572366196E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>12.856079572366195</v>
       </c>
     </row>
@@ -15838,11 +15840,11 @@
         <v>354425</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.2414474148268321E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>12.414474148268321</v>
       </c>
     </row>
@@ -15860,11 +15862,11 @@
         <v>739575</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.2169151201703681E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>12.169151201703681</v>
       </c>
     </row>
@@ -15882,11 +15884,11 @@
         <v>75168</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.1973180076628353E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>11.973180076628353</v>
       </c>
     </row>
@@ -15904,11 +15906,11 @@
         <v>695797</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.106644610425167E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>11.066446104251671</v>
       </c>
     </row>
@@ -15926,11 +15928,11 @@
         <v>583702</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.0964499008055481E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>10.96449900805548</v>
       </c>
     </row>
@@ -15948,11 +15950,11 @@
         <v>83826</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.0736525660296328E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>10.736525660296328</v>
       </c>
     </row>
@@ -15970,11 +15972,11 @@
         <v>263407</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.062993770097226E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>10.62993770097226</v>
       </c>
     </row>
@@ -15992,11 +15994,11 @@
         <v>192518</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.0388638984406652E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>10.388638984406652</v>
       </c>
     </row>
@@ -16014,11 +16016,11 @@
         <v>683365</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.009709306154105E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>10.097093061541051</v>
       </c>
     </row>
@@ -16036,11 +16038,11 @@
         <v>239824</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.0007338715057709E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>10.007338715057708</v>
       </c>
     </row>
@@ -16058,11 +16060,11 @@
         <v>116446</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>9.4464386926128852E-3</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>9.4464386926128849</v>
       </c>
     </row>
@@ -16080,11 +16082,11 @@
         <v>206268</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>9.2113173153373275E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>9.2113173153373271</v>
       </c>
     </row>
@@ -16102,11 +16104,11 @@
         <v>54709</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -16124,11 +16126,11 @@
         <v>148350</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>8.7630603302999658E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>8.7630603302999663</v>
       </c>
     </row>
@@ -16146,11 +16148,11 @@
         <v>180822</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -16168,11 +16170,11 @@
         <v>125851</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>7.1513138552732995E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1513138552732993</v>
       </c>
     </row>
@@ -16190,11 +16192,11 @@
         <v>434170</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>6.9097358177672343E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>6.9097358177672339</v>
       </c>
     </row>
@@ -16212,11 +16214,11 @@
         <v>190006</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>6.841889203498837E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>6.8418892034988374</v>
       </c>
     </row>
@@ -16234,11 +16236,11 @@
         <v>91850</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>6.5323897659226998E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>6.5323897659226997</v>
       </c>
     </row>
@@ -16256,11 +16258,11 @@
         <v>218775</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>5.9421780367957949E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>5.942178036795795</v>
       </c>
     </row>
@@ -16278,11 +16280,11 @@
         <v>84247</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>5.9349294336890337E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>5.9349294336890335</v>
       </c>
     </row>
@@ -16300,11 +16302,11 @@
         <v>196435</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>5.5998167332705472E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>5.5998167332705471</v>
       </c>
     </row>
@@ -16322,11 +16324,11 @@
         <v>75167</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>5.3214841619327628E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>5.3214841619327631</v>
       </c>
     </row>
@@ -16344,11 +16346,11 @@
         <v>577212</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>5.1973971435105302E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>5.1973971435105302</v>
       </c>
     </row>
@@ -16366,11 +16368,11 @@
         <v>127998</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>4.6875732433319271E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>4.6875732433319275</v>
       </c>
     </row>
@@ -16388,11 +16390,11 @@
         <v>112055</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>4.4620945071616614E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>4.4620945071616616</v>
       </c>
     </row>
@@ -16410,11 +16412,11 @@
         <v>150417</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>3.3240923565820354E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>3.3240923565820353</v>
       </c>
     </row>
@@ -16432,11 +16434,11 @@
         <v>32394</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -16454,11 +16456,11 @@
         <v>80055</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>2.498282430828805E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>2.4982824308288052</v>
       </c>
     </row>
@@ -16476,11 +16478,11 @@
         <v>133573</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -16498,11 +16500,11 @@
         <v>71544</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -16520,11 +16522,11 @@
         <v>57443</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16542,11 +16544,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16564,11 +16566,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16586,11 +16588,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16608,11 +16610,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16630,11 +16632,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16652,11 +16654,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16674,11 +16676,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16696,11 +16698,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16718,11 +16720,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16740,11 +16742,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16762,11 +16764,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -16784,11 +16786,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -18250,6 +18252,1446 @@
       </c>
       <c r="C65">
         <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E706B4F-4B11-48E0-B700-265DBF77CE6D}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.58203125" customWidth="1"/>
+    <col min="5" max="5" width="27.25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>212</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>8.1614425734722315E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>81.614425734722317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>227</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>6.49150099517284E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>64.915009951728393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>118</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>5.028530518492634E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>50.285305184926344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>3.9929914061289436E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>39.929914061289438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>97</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>3.3716262013590785E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>33.716262013590786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>132</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>3.2055018067373819E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>32.055018067373823</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>293</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.1200118411370898E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>31.200118411370898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>88</v>
+      </c>
+      <c r="D9">
+        <v>301185</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>2.9217922539303085E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>29.217922539303085</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>65891</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>2.8835501054772276E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>28.835501054772276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>59</v>
+      </c>
+      <c r="D11">
+        <v>209244</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>2.8196746382214064E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>28.196746382214066</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>342296</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>2.629303293056302E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>26.293032930563019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>145</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>2.4766426973201017E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>24.766426973201018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>2.109337704966565E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>21.093377049665651</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>45</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>1.9081056327278276E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>19.081056327278276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>78</v>
+      </c>
+      <c r="D16">
+        <v>454973</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>1.7143874471671944E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>17.143874471671946</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>73</v>
+      </c>
+      <c r="D17">
+        <v>519212</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.4059767493817554E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>14.059767493817553</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>101</v>
+      </c>
+      <c r="D18">
+        <v>742652</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.3599909513473335E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>13.599909513473335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>75168</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.3303533418475948E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>13.303533418475947</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>96</v>
+      </c>
+      <c r="D20">
+        <v>739575</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.2980427948483926E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>12.980427948483927</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>147790</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.2856079572366196E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>12.856079572366195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>354425</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.2696621288001694E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>12.696621288001694</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>83826</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.1929472955884809E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>11.929472955884808</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>81</v>
+      </c>
+      <c r="D24">
+        <v>695797</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.1641326421355654E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>11.641326421355654</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+      <c r="D25">
+        <v>263407</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.1389218965327422E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>11.389218965327421</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>66</v>
+      </c>
+      <c r="D26">
+        <v>583702</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.1307139602057214E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>11.307139602057214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>239824</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.0424311161518447E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>10.424311161518446</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>192518</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.0388638984406652E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>10.388638984406652</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>116446</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>70</v>
+      </c>
+      <c r="D30">
+        <v>683365</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.0243427743592369E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>10.243427743592369</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>21</v>
+      </c>
+      <c r="D31">
+        <v>206268</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>1.0180929664320205E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>10.180929664320205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>148350</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>9.4371418941691949E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>9.4371418941691942</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>54709</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>125851</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>7.9459042836369995E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>7.9459042836369997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>180822</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>31</v>
+      </c>
+      <c r="D36">
+        <v>434170</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>7.1400603450261415E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>7.1400603450261411</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>190006</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>6.841889203498837E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>6.8418892034988374</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>91850</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <v>196435</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>6.1088909817496881E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>6.1088909817496884</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>218775</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>5.9421780367957949E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>5.942178036795795</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>84247</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>5.9349294336890337E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>5.9349294336890335</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <v>31</v>
+      </c>
+      <c r="D42">
+        <v>577212</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>5.3706437149608809E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>5.370643714960881</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>112055</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>5.3545134085939937E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>5.3545134085939941</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>75167</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>5.3214841619327628E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>5.3214841619327631</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>127998</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>4.6875732433319271E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>4.6875732433319275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>80055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>3.747423646243208E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>3.7474236462432078</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>3.3240923565820354E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>3.3240923565820353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>71544</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>57443</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>82</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>412</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised: 2020/04/21 and 2020/04/22 data added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27019ED1-5043-44D7-9667-B5EFB291D8C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A33B7-BE79-4A59-95FD-11091198002D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14712" yWindow="1656" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="14" activeTab="20" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="12936" yWindow="2556" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="15" activeTab="21" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="2020年4月18日" sheetId="19" r:id="rId19"/>
     <sheet name="2020年4月19日" sheetId="20" r:id="rId20"/>
     <sheet name="2020年4月20日" sheetId="21" r:id="rId21"/>
+    <sheet name="2020年4月21日" sheetId="22" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -49,6 +50,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'2020年4月19日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">'2020年4月20日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'2020年4月21日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -58,7 +60,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2020年4月8日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'2020年4月9日'!$B$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -19022,11 +19024,11 @@
         <v>125851</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>7.9459042836369995E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>7.9459042836369997</v>
       </c>
     </row>
@@ -19711,7 +19713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F846AD-1565-4AED-8DFE-67061A81FA9F}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -19758,11 +19760,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>8.2769346853609899E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>82.769346853609903</v>
       </c>
     </row>
@@ -19780,11 +19782,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>7.2922147743131022E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>72.922147743131021</v>
       </c>
     </row>
@@ -19802,11 +19804,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>5.0711451839035887E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>50.711451839035888</v>
       </c>
     </row>
@@ -19824,11 +19826,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>4.0525882927875845E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>40.525882927875841</v>
       </c>
     </row>
@@ -19846,11 +19848,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>3.5106623333738853E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>35.106623333738852</v>
       </c>
     </row>
@@ -19868,11 +19870,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.351206434316354E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>33.512064343163537</v>
       </c>
     </row>
@@ -19890,11 +19892,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.2477938960642064E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>32.477938960642064</v>
       </c>
     </row>
@@ -19912,11 +19914,11 @@
         <v>301185</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.9217922539303085E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>29.217922539303085</v>
       </c>
     </row>
@@ -19934,6 +19936,1446 @@
         <v>65891</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2.8835501054772276E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>28.835501054772276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>59</v>
+      </c>
+      <c r="D11">
+        <v>209244</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.8196746382214064E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>28.196746382214066</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>342296</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2.629303293056302E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>26.293032930563019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>146</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2.4937229917843785E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>24.937229917843787</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>2.2203554789121737E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>22.203554789121736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>46</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1.9505079801217795E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>19.505079801217796</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>454973</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.7583460996586611E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>17.583460996586609</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>112</v>
+      </c>
+      <c r="D17">
+        <v>742652</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.5081087777316966E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>15.081087777316966</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>75168</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+      <c r="D19">
+        <v>519212</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.4444966603237214E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>14.444966603237214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>354425</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1.3260915567468435E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>13.260915567468436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>83826</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.3122420251473289E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>13.12242025147329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>97</v>
+      </c>
+      <c r="D22">
+        <v>739575</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.3115640739613967E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>13.115640739613967</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>147790</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.2856079572366196E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>12.856079572366195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>263407</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.2148500229682583E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>12.148500229682583</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>206268</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.2120154362285957E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>12.120154362285957</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>84</v>
+      </c>
+      <c r="D26">
+        <v>695797</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.2072486659183642E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>12.072486659183642</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>583702</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.1821100493059815E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>11.821100493059815</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>21</v>
+      </c>
+      <c r="D28">
+        <v>192518</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.0908070933626985E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>10.908070933626986</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>239824</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.0841283607979185E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>10.841283607979184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>116446</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>70</v>
+      </c>
+      <c r="D31">
+        <v>683365</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.0243427743592369E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>10.243427743592369</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>148350</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>9.4371418941691949E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4371418941691942</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>54709</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>125851</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>7.9459042836369995E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>7.9459042836369997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>190006</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>7.3681883729987477E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>7.3681883729987474</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>180822</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>31</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>7.1400603450261415E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1400603450261411</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>196435</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>6.617965230228829E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>6.6179652302288288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>91850</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>218775</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>6.3992686550108559E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>6.3992686550108555</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>84247</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>5.9349294336890337E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>5.9349294336890335</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <v>33</v>
+      </c>
+      <c r="D42">
+        <v>577212</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>5.7171368578615833E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>5.7171368578615835</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>112055</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>5.3545134085939937E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3545134085939941</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>75167</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>5.3214841619327628E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3214841619327631</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>127998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>4.6875732433319271E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6875732433319275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>80055</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>3.747423646243208E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>3.7474236462432078</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>3.3240923565820354E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3240923565820353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>71544</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>57443</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>85</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>412</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D56539-4BF6-4E5E-AEC7-0806BEF90EDA}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>224</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>8.6234110210272635E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>86.234110210272632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>259</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>7.4066024570474245E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>74.066024570474241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>132</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>5.6251358342459971E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>56.251358342459973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>4.171782066104867E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>41.71782066104867</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>102</v>
+      </c>
+      <c r="D6">
+        <v>287695</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>3.5454213663775873E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>35.454213663775874</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>141</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>3.4240587481058397E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>34.240587481058398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>314</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.3436304372595434E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>33.436304372595437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>93</v>
+      </c>
+      <c r="D9">
+        <v>301185</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>3.087803177449076E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>30.878031774490761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>65891</v>
+      </c>
+      <c r="E10">
         <f>100*C10/D10</f>
         <v>2.8835501054772276E-2</v>
       </c>
@@ -19972,18 +21414,18 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D12">
         <v>342296</v>
       </c>
       <c r="E12">
         <f>100*C12/D12</f>
-        <v>2.629303293056302E-2</v>
+        <v>2.7169467361581788E-2</v>
       </c>
       <c r="F12" s="1">
         <f>E12*1000</f>
-        <v>26.293032930563019</v>
+        <v>27.169467361581788</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -19994,18 +21436,18 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D13">
         <v>585470</v>
       </c>
       <c r="E13">
         <f>100*C13/D13</f>
-        <v>2.4937229917843785E-2</v>
+        <v>2.6303653474985908E-2</v>
       </c>
       <c r="F13" s="1">
         <f>E13*1000</f>
-        <v>24.937229917843787</v>
+        <v>26.303653474985907</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -20016,18 +21458,18 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D14">
         <v>270227</v>
       </c>
       <c r="E14">
         <f>100*C14/D14</f>
-        <v>2.2203554789121737E-2</v>
+        <v>2.3683791775063186E-2</v>
       </c>
       <c r="F14" s="1">
         <f>E14*1000</f>
-        <v>22.203554789121736</v>
+        <v>23.683791775063188</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -20038,18 +21480,18 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>235836</v>
       </c>
       <c r="E15">
         <f>100*C15/D15</f>
-        <v>1.9505079801217795E-2</v>
+        <v>2.1201173696975866E-2</v>
       </c>
       <c r="F15" s="1">
         <f>E15*1000</f>
-        <v>19.505079801217796</v>
+        <v>21.201173696975864</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -20060,84 +21502,84 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D16">
         <v>454973</v>
       </c>
       <c r="E16">
         <f>100*C16/D16</f>
-        <v>1.7583460996586611E-2</v>
+        <v>1.7803254259043944E-2</v>
       </c>
       <c r="F16" s="1">
         <f>E16*1000</f>
-        <v>17.583460996586609</v>
+        <v>17.803254259043943</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="D17">
-        <v>742652</v>
+        <v>519212</v>
       </c>
       <c r="E17">
         <f>100*C17/D17</f>
-        <v>1.5081087777316966E-2</v>
+        <v>1.5600563931496191E-2</v>
       </c>
       <c r="F17" s="1">
         <f>E17*1000</f>
-        <v>15.081087777316966</v>
+        <v>15.60056393149619</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>11</v>
+        <v>114</v>
       </c>
       <c r="D18">
-        <v>75168</v>
+        <v>742652</v>
       </c>
       <c r="E18">
         <f>100*C18/D18</f>
-        <v>1.4633886760323542E-2</v>
+        <v>1.5350392916197627E-2</v>
       </c>
       <c r="F18" s="1">
         <f>E18*1000</f>
-        <v>14.633886760323543</v>
+        <v>15.350392916197627</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C19">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>519212</v>
+        <v>75168</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>1.4444966603237214E-2</v>
+        <v>1.4633886760323542E-2</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>14.444966603237214</v>
+        <v>14.633886760323543</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -20148,40 +21590,40 @@
         <v>16</v>
       </c>
       <c r="C20">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D20">
         <v>354425</v>
       </c>
       <c r="E20">
         <f>100*C20/D20</f>
-        <v>1.3260915567468435E-2</v>
+        <v>1.4389504126401919E-2</v>
       </c>
       <c r="F20" s="1">
         <f>E20*1000</f>
-        <v>13.260915567468436</v>
+        <v>14.389504126401919</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C21">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D21">
-        <v>83826</v>
+        <v>147790</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>1.3122420251473289E-2</v>
+        <v>1.4209351106299478E-2</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>13.12242025147329</v>
+        <v>14.209351106299478</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -20192,62 +21634,62 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D22">
         <v>739575</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>1.3115640739613967E-2</v>
+        <v>1.3521279113004089E-2</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>13.115640739613967</v>
+        <v>13.521279113004089</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>147790</v>
+        <v>83826</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>1.2856079572366196E-2</v>
+        <v>1.3122420251473289E-2</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>12.856079572366195</v>
+        <v>13.12242025147329</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C24">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D24">
-        <v>263407</v>
+        <v>583702</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>1.2148500229682583E-2</v>
+        <v>1.2849022275065016E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>12.148500229682583</v>
+        <v>12.849022275065016</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -20258,62 +21700,62 @@
         <v>37</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25">
         <v>206268</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>1.2120154362285957E-2</v>
+        <v>1.2604960536777397E-2</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>12.120154362285957</v>
+        <v>12.604960536777398</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C26">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D26">
-        <v>695797</v>
+        <v>263407</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>1.2072486659183642E-2</v>
+        <v>1.2528140861860163E-2</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>12.072486659183642</v>
+        <v>12.528140861860162</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="D27">
-        <v>583702</v>
+        <v>695797</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>1.1821100493059815E-2</v>
+        <v>1.2503646897011628E-2</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>11.821100493059815</v>
+        <v>12.503646897011629</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -20324,84 +21766,84 @@
         <v>25</v>
       </c>
       <c r="C28">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D28">
         <v>192518</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>1.0908070933626985E-2</v>
+        <v>1.1427502882847319E-2</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>10.908070933626986</v>
+        <v>11.427502882847319</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D29">
-        <v>239824</v>
+        <v>683365</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>1.0841283607979185E-2</v>
+        <v>1.1121435835900287E-2</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>10.841283607979184</v>
+        <v>11.121435835900288</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D30">
-        <v>116446</v>
+        <v>239824</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>1.0305205846486783E-2</v>
+        <v>1.0841283607979185E-2</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>10.305205846486784</v>
+        <v>10.841283607979184</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C31">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D31">
-        <v>683365</v>
+        <v>116446</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>1.0243427743592369E-2</v>
+        <v>1.0305205846486783E-2</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>10.243427743592369</v>
+        <v>10.305205846486784</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -20450,266 +21892,266 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D34">
-        <v>125851</v>
+        <v>190006</v>
       </c>
       <c r="E34">
         <f>100*C34/D34</f>
-        <v>7.9459042836369995E-3</v>
+        <v>8.420786711998569E-3</v>
       </c>
       <c r="F34" s="1">
         <f>E34*1000</f>
-        <v>7.9459042836369997</v>
+        <v>8.4207867119985682</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D35">
-        <v>190006</v>
+        <v>125851</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>7.3681883729987477E-3</v>
+        <v>7.9459042836369995E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>7.3681883729987474</v>
+        <v>7.9459042836369997</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D36">
-        <v>180822</v>
+        <v>434170</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>7.1893906714890887E-3</v>
+        <v>7.8310339268028648E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>7.1893906714890887</v>
+        <v>7.8310339268028644</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C37">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D37">
-        <v>434170</v>
+        <v>218775</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>7.1400603450261415E-3</v>
+        <v>7.770540509656039E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>7.1400603450261411</v>
+        <v>7.7705405096560387</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>13</v>
       </c>
       <c r="D38">
-        <v>196435</v>
+        <v>180822</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>6.617965230228829E-3</v>
+        <v>7.1893906714890887E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>6.6179652302288288</v>
+        <v>7.1893906714890887</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D39">
-        <v>91850</v>
+        <v>196435</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>6.5323897659226998E-3</v>
+        <v>6.617965230228829E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>6.5323897659226997</v>
+        <v>6.6179652302288288</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C40">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D40">
-        <v>218775</v>
+        <v>91850</v>
       </c>
       <c r="E40">
         <f>100*C40/D40</f>
-        <v>6.3992686550108559E-3</v>
+        <v>6.5323897659226998E-3</v>
       </c>
       <c r="F40" s="1">
         <f>E40*1000</f>
-        <v>6.3992686550108555</v>
+        <v>6.5323897659226997</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D41">
-        <v>84247</v>
+        <v>577212</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>5.9349294336890337E-3</v>
+        <v>6.0636300007622847E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>5.9349294336890335</v>
+        <v>6.0636300007622843</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C42">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D42">
-        <v>577212</v>
+        <v>84247</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>5.7171368578615833E-3</v>
+        <v>5.9349294336890337E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>5.7171368578615835</v>
+        <v>5.9349294336890335</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>112055</v>
+        <v>127998</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>5.3545134085939937E-3</v>
+        <v>5.4688354505539145E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>5.3545134085939941</v>
+        <v>5.4688354505539145</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D44">
-        <v>75167</v>
+        <v>112055</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>5.3214841619327628E-3</v>
+        <v>5.3545134085939937E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>5.3214841619327631</v>
+        <v>5.3545134085939941</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>127998</v>
+        <v>75167</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>4.6875732433319271E-3</v>
+        <v>5.3214841619327628E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>4.6875732433319275</v>
+        <v>5.3214841619327631</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -20802,46 +22244,46 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>71544</v>
+        <v>57443</v>
       </c>
       <c r="E50">
         <f>100*C50/D50</f>
-        <v>1.3977412501397742E-3</v>
+        <v>1.7408561530560731E-3</v>
       </c>
       <c r="F50" s="1">
         <f>E50*1000</f>
-        <v>1.3977412501397741</v>
+        <v>1.7408561530560731</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>57443</v>
+        <v>71544</v>
       </c>
       <c r="E51">
         <f>100*C51/D51</f>
-        <v>0</v>
+        <v>1.3977412501397742E-3</v>
       </c>
       <c r="F51" s="1">
         <f>E51*1000</f>
-        <v>0</v>
+        <v>1.3977412501397741</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -21116,7 +22558,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -21130,7 +22572,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Revised: data 2020/04/22 and 2020/04/23 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A33B7-BE79-4A59-95FD-11091198002D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26AEB0C-1F16-4D20-87E5-D7E7F9D4F988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12936" yWindow="2556" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="15" activeTab="21" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="8604" yWindow="1248" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="16" activeTab="22" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="2020年4月19日" sheetId="20" r:id="rId20"/>
     <sheet name="2020年4月20日" sheetId="21" r:id="rId21"/>
     <sheet name="2020年4月21日" sheetId="22" r:id="rId22"/>
+    <sheet name="2020年4月22日" sheetId="23" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -51,6 +52,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020年4月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">'2020年4月20日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'2020年4月21日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'2020年4月22日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -60,7 +62,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2020年4月8日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'2020年4月9日'!$B$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -76,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -20464,11 +20466,11 @@
         <v>125851</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>7.9459042836369995E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>7.9459042836369997</v>
       </c>
     </row>
@@ -21153,7 +21155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D56539-4BF6-4E5E-AEC7-0806BEF90EDA}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
@@ -21200,11 +21202,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>8.6234110210272635E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>86.234110210272632</v>
       </c>
     </row>
@@ -21222,11 +21224,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>7.4066024570474245E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>74.066024570474241</v>
       </c>
     </row>
@@ -21244,11 +21246,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>5.6251358342459971E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>56.251358342459973</v>
       </c>
     </row>
@@ -21266,11 +21268,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>4.171782066104867E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>41.71782066104867</v>
       </c>
     </row>
@@ -21288,11 +21290,11 @@
         <v>287695</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>3.5454213663775873E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>35.454213663775874</v>
       </c>
     </row>
@@ -21310,11 +21312,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.4240587481058397E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>34.240587481058398</v>
       </c>
     </row>
@@ -21332,11 +21334,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.3436304372595434E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>33.436304372595437</v>
       </c>
     </row>
@@ -21354,11 +21356,11 @@
         <v>301185</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>3.087803177449076E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>30.878031774490761</v>
       </c>
     </row>
@@ -21376,11 +21378,11 @@
         <v>65891</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>2.8835501054772276E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>28.835501054772276</v>
       </c>
     </row>
@@ -21398,11 +21400,11 @@
         <v>209244</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>2.8196746382214064E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>28.196746382214066</v>
       </c>
     </row>
@@ -21420,11 +21422,11 @@
         <v>342296</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>2.7169467361581788E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>27.169467361581788</v>
       </c>
     </row>
@@ -21442,11 +21444,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>2.6303653474985908E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>26.303653474985907</v>
       </c>
     </row>
@@ -21464,11 +21466,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>2.3683791775063186E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>23.683791775063188</v>
       </c>
     </row>
@@ -21486,11 +21488,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.1201173696975866E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>21.201173696975864</v>
       </c>
     </row>
@@ -21508,11 +21510,11 @@
         <v>454973</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.7803254259043944E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>17.803254259043943</v>
       </c>
     </row>
@@ -21530,11 +21532,11 @@
         <v>519212</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.5600563931496191E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>15.60056393149619</v>
       </c>
     </row>
@@ -21552,11 +21554,11 @@
         <v>742652</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.5350392916197627E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>15.350392916197627</v>
       </c>
     </row>
@@ -21574,11 +21576,11 @@
         <v>75168</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -21596,11 +21598,11 @@
         <v>354425</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.4389504126401919E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>14.389504126401919</v>
       </c>
     </row>
@@ -21618,11 +21620,11 @@
         <v>147790</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.4209351106299478E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>14.209351106299478</v>
       </c>
     </row>
@@ -21640,11 +21642,11 @@
         <v>739575</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.3521279113004089E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>13.521279113004089</v>
       </c>
     </row>
@@ -21662,6 +21664,1446 @@
         <v>83826</v>
       </c>
       <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.3122420251473289E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>13.12242025147329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>75</v>
+      </c>
+      <c r="D24">
+        <v>583702</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.2849022275065016E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>12.849022275065016</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <v>206268</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.2604960536777397E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>12.604960536777398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>263407</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.2528140861860163E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>12.528140861860162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>87</v>
+      </c>
+      <c r="D27">
+        <v>695797</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.2503646897011628E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>12.503646897011629</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>192518</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.1427502882847319E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>11.427502882847319</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>76</v>
+      </c>
+      <c r="D29">
+        <v>683365</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.1121435835900287E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>11.121435835900288</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>26</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.0841283607979185E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>10.841283607979184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>116446</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>148350</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>9.4371418941691949E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4371418941691942</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>54709</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>190006</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>8.420786711998569E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>8.4207867119985682</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>125851</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>7.9459042836369995E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>7.9459042836369997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <v>434170</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>7.8310339268028648E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>7.8310339268028644</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <v>218775</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>7.770540509656039E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>7.7705405096560387</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>180822</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>196435</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>6.617965230228829E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>6.6179652302288288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>91850</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41">
+        <v>35</v>
+      </c>
+      <c r="D41">
+        <v>577212</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>6.0636300007622847E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>6.0636300007622843</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>84247</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>5.9349294336890337E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>5.9349294336890335</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>127998</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>5.4688354505539145E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>5.4688354505539145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>112055</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>5.3545134085939937E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3545134085939941</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>75167</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>5.3214841619327628E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3214841619327631</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>80055</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>3.747423646243208E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>3.7474236462432078</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>3.3240923565820354E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3240923565820353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>86</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>421</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB60DDEC-59C3-4784-B4F2-24C2518820A4}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>238</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>9.1623742098414673E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>91.623742098414667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>260</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>7.4351993777310055E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>74.351993777310057</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>133</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>5.6677504996569518E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>56.677504996569517</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>73</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>4.3505727260807897E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>43.505727260807895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>136</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>3.9731694206184123E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>39.731694206184123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>102</v>
+      </c>
+      <c r="D7">
+        <v>287695</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>3.5454213663775873E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>35.454213663775874</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>145</v>
+      </c>
+      <c r="D8">
+        <v>411792</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.5211951664918209E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>35.21195166491821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>317</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>3.3755759509913226E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>33.755759509913226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>65891</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>3.3388474905525795E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>33.388474905525797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>96</v>
+      </c>
+      <c r="D11">
+        <v>301185</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>3.1874097315603367E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>31.874097315603368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>59</v>
+      </c>
+      <c r="D12">
+        <v>209244</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>2.8196746382214064E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>28.196746382214066</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>158</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>2.6986865253556973E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>26.986865253556974</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>270227</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>2.4793969514519273E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>24.793969514519272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>51</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.1625197170915381E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>21.625197170915381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>83</v>
+      </c>
+      <c r="D16">
+        <v>454973</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>1.824284078395861E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>18.242840783958609</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>519212</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.6370962150335507E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>16.370962150335508</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>121</v>
+      </c>
+      <c r="D18">
+        <v>742652</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.6292960902279937E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>16.292960902279937</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>53</v>
+      </c>
+      <c r="D19">
+        <v>354425</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.4953798405868661E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>14.95379840586866</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>109</v>
+      </c>
+      <c r="D20">
+        <v>739575</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.4738194233174459E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>14.738194233174459</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>75168</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>147790</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.4209351106299478E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>14.209351106299478</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>83826</v>
+      </c>
+      <c r="E23">
         <f>100*C23/D23</f>
         <v>1.3122420251473289E-2</v>
       </c>
@@ -21678,84 +23120,84 @@
         <v>18</v>
       </c>
       <c r="C24">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24">
         <v>583702</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>1.2849022275065016E-2</v>
+        <v>1.3020342572065883E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>12.849022275065016</v>
+        <v>13.020342572065884</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="D25">
-        <v>206268</v>
+        <v>695797</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>1.2604960536777397E-2</v>
+        <v>1.2934807134839615E-2</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>12.604960536777398</v>
+        <v>12.934807134839614</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C26">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D26">
-        <v>263407</v>
+        <v>206268</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>1.2528140861860163E-2</v>
+        <v>1.2604960536777397E-2</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>12.528140861860162</v>
+        <v>12.604960536777398</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C27">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="D27">
-        <v>695797</v>
+        <v>263407</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>1.2503646897011628E-2</v>
+        <v>1.2528140861860163E-2</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>12.503646897011629</v>
+        <v>12.528140861860162</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -21766,18 +23208,18 @@
         <v>25</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D28">
         <v>192518</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>1.1427502882847319E-2</v>
+        <v>1.194693483206765E-2</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>11.427502882847319</v>
+        <v>11.946934832067651</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -21788,18 +23230,18 @@
         <v>20</v>
       </c>
       <c r="C29">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D29">
         <v>683365</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>1.1121435835900287E-2</v>
+        <v>1.1267770517951607E-2</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>11.121435835900288</v>
+        <v>11.267770517951607</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -21810,18 +23252,18 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D30">
         <v>239824</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>1.0841283607979185E-2</v>
+        <v>1.1258256054439923E-2</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>10.841283607979184</v>
+        <v>11.258256054439922</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -21914,68 +23356,68 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D35">
-        <v>125851</v>
+        <v>218775</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>7.9459042836369995E-3</v>
+        <v>8.2276311278711E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>7.9459042836369997</v>
+        <v>8.2276311278710992</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C36">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D36">
-        <v>434170</v>
+        <v>125851</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>7.8310339268028648E-3</v>
+        <v>7.9459042836369995E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>7.8310339268028644</v>
+        <v>7.9459042836369997</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C37">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D37">
-        <v>218775</v>
+        <v>434170</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>7.770540509656039E-3</v>
+        <v>7.8310339268028648E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>7.7705405096560387</v>
+        <v>7.8310339268028644</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -22008,18 +23450,18 @@
         <v>31</v>
       </c>
       <c r="C39">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D39">
         <v>196435</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>6.617965230228829E-3</v>
+        <v>7.1270394787079699E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>6.6179652302288288</v>
+        <v>7.1270394787079701</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -22558,7 +24000,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -22572,7 +24014,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: data 2020/04/23 and 2020/04/24 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26AEB0C-1F16-4D20-87E5-D7E7F9D4F988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF78C164-B080-4620-873F-5668BBCCAC87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8604" yWindow="1248" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="16" activeTab="22" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="5676" yWindow="9372" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="17" activeTab="23" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="2020年4月20日" sheetId="21" r:id="rId21"/>
     <sheet name="2020年4月21日" sheetId="22" r:id="rId22"/>
     <sheet name="2020年4月22日" sheetId="23" r:id="rId23"/>
+    <sheet name="2020年4月23日" sheetId="24" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -53,6 +54,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">'2020年4月20日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'2020年4月21日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'2020年4月22日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'2020年4月23日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -78,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -21906,11 +21908,11 @@
         <v>190006</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>8.420786711998569E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>8.4207867119985682</v>
       </c>
     </row>
@@ -22595,7 +22597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB60DDEC-59C3-4784-B4F2-24C2518820A4}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -22630,24 +22632,1464 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>422</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>317</v>
+      </c>
+      <c r="D3">
+        <v>939099</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>3.3755759509913226E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>33.755759509913226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>260</v>
+      </c>
+      <c r="D4">
+        <v>349688</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>7.4351993777310055E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>74.351993777310057</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>238</v>
+      </c>
+      <c r="D5">
+        <v>259758</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>9.1623742098414673E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>91.623742098414667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>158</v>
+      </c>
+      <c r="D6">
+        <v>585470</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>2.6986865253556973E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>26.986865253556974</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>145</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>3.5211951664918209E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>35.21195166491821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>136</v>
+      </c>
+      <c r="D8">
+        <v>342296</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.9731694206184123E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>39.731694206184123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>133</v>
+      </c>
+      <c r="D9">
+        <v>234661</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>5.6677504996569518E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>56.677504996569517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>121</v>
+      </c>
+      <c r="D10">
+        <v>742652</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>1.6292960902279937E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>16.292960902279937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>109</v>
+      </c>
+      <c r="D11">
+        <v>739575</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>1.4738194233174459E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>14.738194233174459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>102</v>
+      </c>
+      <c r="D12">
+        <v>287695</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>3.5454213663775873E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>35.454213663775874</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>96</v>
+      </c>
+      <c r="D14">
+        <v>301185</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>3.1874097315603367E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>31.874097315603368</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+      <c r="D15">
+        <v>695797</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>1.2934807134839615E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>12.934807134839614</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>519212</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>1.6370962150335507E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>16.370962150335508</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>83</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.824284078395861E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>18.242840783958609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>77</v>
+      </c>
+      <c r="D18">
+        <v>683365</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.1267770517951607E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>11.267770517951607</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>76</v>
+      </c>
+      <c r="D19">
+        <v>583702</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.3020342572065883E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>13.020342572065884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>73</v>
+      </c>
+      <c r="D20">
+        <v>167794</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>4.3505727260807897E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>43.505727260807895</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>67</v>
+      </c>
+      <c r="D21">
+        <v>270227</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>2.4793969514519273E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>24.793969514519272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>59</v>
+      </c>
+      <c r="D22">
+        <v>209244</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>2.8196746382214064E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>28.196746382214066</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>354425</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.4953798405868661E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>14.95379840586866</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>51</v>
+      </c>
+      <c r="D24">
+        <v>235836</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>2.1625197170915381E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>21.625197170915381</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>35</v>
+      </c>
+      <c r="D25">
+        <v>577212</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>6.0636300007622847E-3</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>6.0636300007622843</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>434170</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>7.8310339268028648E-3</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>7.8310339268028644</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>263407</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.2528140861860163E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>12.528140861860162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>239824</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.1258256054439923E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>11.258256054439922</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>206268</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.2604960536777397E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>12.604960536777398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>23</v>
+      </c>
+      <c r="D30">
+        <v>192518</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.194693483206765E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>11.946934832067651</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>65891</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>3.3388474905525795E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>33.388474905525797</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32">
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>147790</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>1.4209351106299478E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>14.209351106299478</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <v>18</v>
+      </c>
+      <c r="D33">
+        <v>218775</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>8.2276311278711E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>8.2276311278710992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>190006</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>8.420786711998569E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>8.4207867119985682</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>148350</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>9.4371418941691949E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>9.4371418941691942</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>196435</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>7.1270394787079699E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>7.1270394787079701</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>180822</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>116446</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>75168</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>83826</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>1.3122420251473289E-2</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>13.12242025147329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>125851</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>7.9459042836369995E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>7.9459042836369997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>127998</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>5.4688354505539145E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>5.4688354505539145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>91850</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>112055</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>5.3545134085939937E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>5.3545134085939941</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>54709</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>84247</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>5.9349294336890337E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>5.9349294336890335</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>3.3240923565820354E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>3.3240923565820353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>75167</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>5.3214841619327628E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>5.3214841619327631</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>80055</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>3.747423646243208E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>3.7474236462432078</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>133573</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>32394</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>39</v>
+      </c>
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>57443</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>71544</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>17140</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>1990</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>4863</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>7244</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>344</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2594</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>1870</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>2270</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>337</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>7096</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>176</v>
+      </c>
+      <c r="E64">
+        <f>100*C64/D64</f>
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <f>E64*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>3055</v>
+      </c>
+      <c r="E65">
+        <f>100*C65/D65</f>
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
+        <f>E65*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="C2:C65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258BD623-49C9-4D4B-A187-22FB1D764F55}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D2">
         <v>259758</v>
       </c>
       <c r="E2">
         <f>100*C2/D2</f>
-        <v>9.1623742098414673E-2</v>
+        <v>9.3163636923598123E-2</v>
       </c>
       <c r="F2" s="1">
         <f>E2*1000</f>
-        <v>91.623742098414667</v>
+        <v>93.163636923598119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -22658,18 +24100,18 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D3">
         <v>349688</v>
       </c>
       <c r="E3">
         <f>100*C3/D3</f>
-        <v>7.4351993777310055E-2</v>
+        <v>7.6353778225160721E-2</v>
       </c>
       <c r="F3" s="1">
         <f>E3*1000</f>
-        <v>74.351993777310057</v>
+        <v>76.353778225160724</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -22680,18 +24122,18 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D4">
         <v>234661</v>
       </c>
       <c r="E4">
         <f>100*C4/D4</f>
-        <v>5.6677504996569518E-2</v>
+        <v>5.8808238267117244E-2</v>
       </c>
       <c r="F4" s="1">
         <f>E4*1000</f>
-        <v>56.677504996569517</v>
+        <v>58.808238267117247</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -22702,18 +24144,18 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5">
         <v>167794</v>
       </c>
       <c r="E5">
         <f>100*C5/D5</f>
-        <v>4.3505727260807897E-2</v>
+        <v>4.4101696127394306E-2</v>
       </c>
       <c r="F5" s="1">
         <f>E5*1000</f>
-        <v>43.505727260807895</v>
+        <v>44.101696127394305</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -22724,62 +24166,62 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D6">
         <v>342296</v>
       </c>
       <c r="E6">
         <f>100*C6/D6</f>
-        <v>3.9731694206184123E-2</v>
+        <v>4.2360997499240424E-2</v>
       </c>
       <c r="F6" s="1">
         <f>E6*1000</f>
-        <v>39.731694206184123</v>
+        <v>42.360997499240426</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="D7">
-        <v>287695</v>
+        <v>411792</v>
       </c>
       <c r="E7">
         <f>100*C7/D7</f>
-        <v>3.5454213663775873E-2</v>
+        <v>3.6426156894742975E-2</v>
       </c>
       <c r="F7" s="1">
         <f>E7*1000</f>
-        <v>35.454213663775874</v>
+        <v>36.426156894742974</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
       <c r="C8">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="D8">
-        <v>411792</v>
+        <v>287695</v>
       </c>
       <c r="E8">
         <f>100*C8/D8</f>
-        <v>3.5211951664918209E-2</v>
+        <v>3.5801803993812893E-2</v>
       </c>
       <c r="F8" s="1">
         <f>E8*1000</f>
-        <v>35.21195166491821</v>
+        <v>35.801803993812896</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -22790,62 +24232,62 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="D9">
         <v>939099</v>
       </c>
       <c r="E9">
         <f>100*C9/D9</f>
-        <v>3.3755759509913226E-2</v>
+        <v>3.4714124921866596E-2</v>
       </c>
       <c r="F9" s="1">
         <f>E9*1000</f>
-        <v>33.755759509913226</v>
+        <v>34.714124921866599</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="D10">
-        <v>65891</v>
+        <v>301185</v>
       </c>
       <c r="E10">
         <f>100*C10/D10</f>
-        <v>3.3388474905525795E-2</v>
+        <v>3.4530272091903645E-2</v>
       </c>
       <c r="F10" s="1">
         <f>E10*1000</f>
-        <v>33.388474905525797</v>
+        <v>34.530272091903647</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <v>301185</v>
+        <v>65891</v>
       </c>
       <c r="E11">
         <f>100*C11/D11</f>
-        <v>3.1874097315603367E-2</v>
+        <v>3.3388474905525795E-2</v>
       </c>
       <c r="F11" s="1">
         <f>E11*1000</f>
-        <v>31.874097315603368</v>
+        <v>33.388474905525797</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -22856,18 +24298,18 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>209244</v>
       </c>
       <c r="E12">
         <f>100*C12/D12</f>
-        <v>2.8196746382214064E-2</v>
+        <v>2.8674657337844814E-2</v>
       </c>
       <c r="F12" s="1">
         <f>E12*1000</f>
-        <v>28.196746382214066</v>
+        <v>28.674657337844813</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -22878,18 +24320,18 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D13">
         <v>585470</v>
       </c>
       <c r="E13">
         <f>100*C13/D13</f>
-        <v>2.6986865253556973E-2</v>
+        <v>2.749927408748527E-2</v>
       </c>
       <c r="F13" s="1">
         <f>E13*1000</f>
-        <v>26.986865253556974</v>
+        <v>27.499274087485269</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -22900,18 +24342,18 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D14">
         <v>270227</v>
       </c>
       <c r="E14">
         <f>100*C14/D14</f>
-        <v>2.4793969514519273E-2</v>
+        <v>2.738438423991681E-2</v>
       </c>
       <c r="F14" s="1">
         <f>E14*1000</f>
-        <v>24.793969514519272</v>
+        <v>27.384384239916809</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -22922,18 +24364,18 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>235836</v>
       </c>
       <c r="E15">
         <f>100*C15/D15</f>
-        <v>2.1625197170915381E-2</v>
+        <v>2.2473244118794415E-2</v>
       </c>
       <c r="F15" s="1">
         <f>E15*1000</f>
-        <v>21.625197170915381</v>
+        <v>22.473244118794415</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -22944,18 +24386,18 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D16">
         <v>454973</v>
       </c>
       <c r="E16">
         <f>100*C16/D16</f>
-        <v>1.824284078395861E-2</v>
+        <v>1.9122013833787938E-2</v>
       </c>
       <c r="F16" s="1">
         <f>E16*1000</f>
-        <v>18.242840783958609</v>
+        <v>19.122013833787939</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -22966,18 +24408,18 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D17">
         <v>519212</v>
       </c>
       <c r="E17">
         <f>100*C17/D17</f>
-        <v>1.6370962150335507E-2</v>
+        <v>1.6948760814464996E-2</v>
       </c>
       <c r="F17" s="1">
         <f>E17*1000</f>
-        <v>16.370962150335508</v>
+        <v>16.948760814464997</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -22988,216 +24430,216 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D18">
         <v>742652</v>
       </c>
       <c r="E18">
         <f>100*C18/D18</f>
-        <v>1.6292960902279937E-2</v>
+        <v>1.6831571180041256E-2</v>
       </c>
       <c r="F18" s="1">
         <f>E18*1000</f>
-        <v>16.292960902279937</v>
+        <v>16.831571180041255</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="D19">
-        <v>354425</v>
+        <v>739575</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>1.4953798405868661E-2</v>
+        <v>1.6225534935604909E-2</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>14.95379840586866</v>
+        <v>16.225534935604909</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C20">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>739575</v>
+        <v>147790</v>
       </c>
       <c r="E20">
         <f>100*C20/D20</f>
-        <v>1.4738194233174459E-2</v>
+        <v>1.5562622640232763E-2</v>
       </c>
       <c r="F20" s="1">
         <f>E20*1000</f>
-        <v>14.738194233174459</v>
+        <v>15.562622640232762</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D21">
-        <v>75168</v>
+        <v>354425</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>1.4633886760323542E-2</v>
+        <v>1.5518092685335402E-2</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>14.633886760323543</v>
+        <v>15.518092685335402</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>147790</v>
+        <v>75168</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>1.4209351106299478E-2</v>
+        <v>1.4633886760323542E-2</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>14.209351106299478</v>
+        <v>14.633886760323543</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C23">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D23">
-        <v>83826</v>
+        <v>263407</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>1.3122420251473289E-2</v>
+        <v>1.4046703390570486E-2</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>13.12242025147329</v>
+        <v>14.046703390570487</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="D24">
-        <v>583702</v>
+        <v>695797</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>1.3020342572065883E-2</v>
+        <v>1.3797127610495589E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>13.020342572065884</v>
+        <v>13.79712761049559</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C25">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D25">
-        <v>695797</v>
+        <v>583702</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>1.2934807134839615E-2</v>
+        <v>1.3191662869066749E-2</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>12.934807134839614</v>
+        <v>13.191662869066748</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C26">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D26">
-        <v>206268</v>
+        <v>83826</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>1.2604960536777397E-2</v>
+        <v>1.3122420251473289E-2</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>12.604960536777398</v>
+        <v>13.12242025147329</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
         <v>27</v>
       </c>
-      <c r="C27">
-        <v>33</v>
-      </c>
       <c r="D27">
-        <v>263407</v>
+        <v>206268</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>1.2528140861860163E-2</v>
+        <v>1.3089766711268835E-2</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>12.528140861860162</v>
+        <v>13.089766711268835</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -23208,62 +24650,62 @@
         <v>25</v>
       </c>
       <c r="C28">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D28">
         <v>192518</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>1.194693483206765E-2</v>
+        <v>1.2466366781287984E-2</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>11.946934832067651</v>
+        <v>12.466366781287984</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C29">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="D29">
-        <v>683365</v>
+        <v>239824</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>1.1267770517951607E-2</v>
+        <v>1.2092200947361399E-2</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>11.267770517951607</v>
+        <v>12.092200947361398</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C30">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="D30">
-        <v>239824</v>
+        <v>683365</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>1.1258256054439923E-2</v>
+        <v>1.1706774564105566E-2</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>11.258256054439922</v>
+        <v>11.706774564105565</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -23312,90 +24754,90 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D33">
-        <v>54709</v>
+        <v>218775</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>9.1392641064541487E-3</v>
+        <v>9.141812364301222E-3</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>9.1392641064541493</v>
+        <v>9.1418123643012219</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C34">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D34">
-        <v>190006</v>
+        <v>54709</v>
       </c>
       <c r="E34">
         <f>100*C34/D34</f>
-        <v>8.420786711998569E-3</v>
+        <v>9.1392641064541487E-3</v>
       </c>
       <c r="F34" s="1">
         <f>E34*1000</f>
-        <v>8.4207867119985682</v>
+        <v>9.1392641064541493</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C35">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D35">
-        <v>218775</v>
+        <v>125851</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>8.2276311278711E-3</v>
+        <v>8.7404947120006994E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>8.2276311278710992</v>
+        <v>8.7404947120007002</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C36">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D36">
-        <v>125851</v>
+        <v>190006</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>7.9459042836369995E-3</v>
+        <v>8.420786711998569E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>7.9459042836369997</v>
+        <v>8.4207867119985682</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -23422,134 +24864,134 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D38">
-        <v>180822</v>
+        <v>127998</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>7.1893906714890887E-3</v>
+        <v>7.8126220722198776E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>7.1893906714890887</v>
+        <v>7.8126220722198774</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C39">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39">
-        <v>196435</v>
+        <v>180822</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>7.1270394787079699E-3</v>
+        <v>7.1893906714890887E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>7.1270394787079701</v>
+        <v>7.1893906714890887</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D40">
-        <v>91850</v>
+        <v>196435</v>
       </c>
       <c r="E40">
         <f>100*C40/D40</f>
-        <v>6.5323897659226998E-3</v>
+        <v>7.1270394787079699E-3</v>
       </c>
       <c r="F40" s="1">
         <f>E40*1000</f>
-        <v>6.5323897659226997</v>
+        <v>7.1270394787079701</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C41">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D41">
-        <v>577212</v>
+        <v>84247</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>6.0636300007622847E-3</v>
+        <v>7.1219153204268399E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>6.0636300007622843</v>
+        <v>7.1219153204268402</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D42">
-        <v>84247</v>
+        <v>91850</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>5.9349294336890337E-3</v>
+        <v>6.5323897659226998E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>5.9349294336890335</v>
+        <v>6.5323897659226997</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D43">
-        <v>127998</v>
+        <v>577212</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>5.4688354505539145E-3</v>
+        <v>6.0636300007622847E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>5.4688354505539145</v>
+        <v>6.0636300007622843</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -23604,18 +25046,18 @@
         <v>53</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D46">
         <v>80055</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>3.747423646243208E-3</v>
+        <v>4.9965648616576101E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>3.7474236462432078</v>
+        <v>4.9965648616576104</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -24000,7 +25442,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -24014,7 +25456,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>422</v>
+        <v>437</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Revised: data 2020/04/24 and 2020/04/25 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF78C164-B080-4620-873F-5668BBCCAC87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC2DE30-FD31-49B8-9B76-EDD5C1478777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="9372" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="17" activeTab="23" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="16884" yWindow="552" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="18" activeTab="24" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="2020年4月21日" sheetId="22" r:id="rId22"/>
     <sheet name="2020年4月22日" sheetId="23" r:id="rId23"/>
     <sheet name="2020年4月23日" sheetId="24" r:id="rId24"/>
+    <sheet name="2020年4月24日" sheetId="25" r:id="rId25"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -55,6 +56,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'2020年4月21日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'2020年4月22日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'2020年4月23日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">'2020年4月24日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -80,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -22598,7 +22600,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -22632,536 +22634,552 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>422</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
+        <v>238</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>9.1623742098414673E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>91.623742098414667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="D3">
-        <v>939099</v>
+        <v>349688</v>
       </c>
       <c r="E3">
         <f>100*C3/D3</f>
-        <v>3.3755759509913226E-2</v>
+        <v>7.4351993777310055E-2</v>
       </c>
       <c r="F3" s="1">
         <f>E3*1000</f>
-        <v>33.755759509913226</v>
+        <v>74.351993777310057</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>260</v>
+        <v>133</v>
       </c>
       <c r="D4">
-        <v>349688</v>
+        <v>234661</v>
       </c>
       <c r="E4">
         <f>100*C4/D4</f>
-        <v>7.4351993777310055E-2</v>
+        <v>5.6677504996569518E-2</v>
       </c>
       <c r="F4" s="1">
         <f>E4*1000</f>
-        <v>74.351993777310057</v>
+        <v>56.677504996569517</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>238</v>
+        <v>73</v>
       </c>
       <c r="D5">
-        <v>259758</v>
+        <v>167794</v>
       </c>
       <c r="E5">
         <f>100*C5/D5</f>
-        <v>9.1623742098414673E-2</v>
+        <v>4.3505727260807897E-2</v>
       </c>
       <c r="F5" s="1">
         <f>E5*1000</f>
-        <v>91.623742098414667</v>
+        <v>43.505727260807895</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="D6">
-        <v>585470</v>
+        <v>342296</v>
       </c>
       <c r="E6">
         <f>100*C6/D6</f>
-        <v>2.6986865253556973E-2</v>
+        <v>3.9731694206184123E-2</v>
       </c>
       <c r="F6" s="1">
         <f>E6*1000</f>
-        <v>26.986865253556974</v>
+        <v>39.731694206184123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
       <c r="C7">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="D7">
-        <v>411792</v>
+        <v>287695</v>
       </c>
       <c r="E7">
         <f>100*C7/D7</f>
-        <v>3.5211951664918209E-2</v>
+        <v>3.5454213663775873E-2</v>
       </c>
       <c r="F7" s="1">
         <f>E7*1000</f>
-        <v>35.21195166491821</v>
+        <v>35.454213663775874</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D8">
-        <v>342296</v>
+        <v>411792</v>
       </c>
       <c r="E8">
         <f>100*C8/D8</f>
-        <v>3.9731694206184123E-2</v>
+        <v>3.5211951664918209E-2</v>
       </c>
       <c r="F8" s="1">
         <f>E8*1000</f>
-        <v>39.731694206184123</v>
+        <v>35.21195166491821</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>133</v>
+        <v>317</v>
       </c>
       <c r="D9">
-        <v>234661</v>
+        <v>939099</v>
       </c>
       <c r="E9">
         <f>100*C9/D9</f>
-        <v>5.6677504996569518E-2</v>
+        <v>3.3755759509913226E-2</v>
       </c>
       <c r="F9" s="1">
         <f>E9*1000</f>
-        <v>56.677504996569517</v>
+        <v>33.755759509913226</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="D10">
-        <v>742652</v>
+        <v>65891</v>
       </c>
       <c r="E10">
         <f>100*C10/D10</f>
-        <v>1.6292960902279937E-2</v>
+        <v>3.3388474905525795E-2</v>
       </c>
       <c r="F10" s="1">
         <f>E10*1000</f>
-        <v>16.292960902279937</v>
+        <v>33.388474905525797</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D11">
-        <v>739575</v>
+        <v>301185</v>
       </c>
       <c r="E11">
         <f>100*C11/D11</f>
-        <v>1.4738194233174459E-2</v>
+        <v>3.1874097315603367E-2</v>
       </c>
       <c r="F11" s="1">
         <f>E11*1000</f>
-        <v>14.738194233174459</v>
+        <v>31.874097315603368</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D12">
-        <v>287695</v>
+        <v>209244</v>
       </c>
       <c r="E12">
         <f>100*C12/D12</f>
-        <v>3.5454213663775873E-2</v>
+        <v>2.8196746382214064E-2</v>
       </c>
       <c r="F12" s="1">
         <f>E12*1000</f>
-        <v>35.454213663775874</v>
+        <v>28.196746382214066</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s">
-        <v>69</v>
+        <v>158</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>2.6986865253556973E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>26.986865253556974</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="D14">
-        <v>301185</v>
+        <v>270227</v>
       </c>
       <c r="E14">
         <f>100*C14/D14</f>
-        <v>3.1874097315603367E-2</v>
+        <v>2.4793969514519273E-2</v>
       </c>
       <c r="F14" s="1">
         <f>E14*1000</f>
-        <v>31.874097315603368</v>
+        <v>24.793969514519272</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="D15">
-        <v>695797</v>
+        <v>235836</v>
       </c>
       <c r="E15">
         <f>100*C15/D15</f>
-        <v>1.2934807134839615E-2</v>
+        <v>2.1625197170915381E-2</v>
       </c>
       <c r="F15" s="1">
         <f>E15*1000</f>
-        <v>12.934807134839614</v>
+        <v>21.625197170915381</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D16">
-        <v>519212</v>
+        <v>454973</v>
       </c>
       <c r="E16">
         <f>100*C16/D16</f>
-        <v>1.6370962150335507E-2</v>
+        <v>1.824284078395861E-2</v>
       </c>
       <c r="F16" s="1">
         <f>E16*1000</f>
-        <v>16.370962150335508</v>
+        <v>18.242840783958609</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D17">
-        <v>454973</v>
+        <v>519212</v>
       </c>
       <c r="E17">
         <f>100*C17/D17</f>
-        <v>1.824284078395861E-2</v>
+        <v>1.6370962150335507E-2</v>
       </c>
       <c r="F17" s="1">
         <f>E17*1000</f>
-        <v>18.242840783958609</v>
+        <v>16.370962150335508</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="D18">
-        <v>683365</v>
+        <v>742652</v>
       </c>
       <c r="E18">
         <f>100*C18/D18</f>
-        <v>1.1267770517951607E-2</v>
+        <v>1.6292960902279937E-2</v>
       </c>
       <c r="F18" s="1">
         <f>E18*1000</f>
-        <v>11.267770517951607</v>
+        <v>16.292960902279937</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D19">
-        <v>583702</v>
+        <v>354425</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>1.3020342572065883E-2</v>
+        <v>1.4953798405868661E-2</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>13.020342572065884</v>
+        <v>14.95379840586866</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="D20">
-        <v>167794</v>
+        <v>739575</v>
       </c>
       <c r="E20">
         <f>100*C20/D20</f>
-        <v>4.3505727260807897E-2</v>
+        <v>1.4738194233174459E-2</v>
       </c>
       <c r="F20" s="1">
         <f>E20*1000</f>
-        <v>43.505727260807895</v>
+        <v>14.738194233174459</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>270227</v>
+        <v>75168</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>2.4793969514519273E-2</v>
+        <v>1.4633886760323542E-2</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>24.793969514519272</v>
+        <v>14.633886760323543</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C22">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>209244</v>
+        <v>147790</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>2.8196746382214064E-2</v>
+        <v>1.4209351106299478E-2</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>28.196746382214066</v>
+        <v>14.209351106299478</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C23">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>354425</v>
+        <v>83826</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>1.4953798405868661E-2</v>
+        <v>1.3122420251473289E-2</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>14.95379840586866</v>
+        <v>13.12242025147329</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C24">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="D24">
-        <v>235836</v>
+        <v>583702</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>2.1625197170915381E-2</v>
+        <v>1.3020342572065883E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>21.625197170915381</v>
+        <v>13.020342572065884</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="D25">
-        <v>577212</v>
+        <v>695797</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>6.0636300007622847E-3</v>
+        <v>1.2934807134839615E-2</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>6.0636300007622843</v>
+        <v>12.934807134839614</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C26">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D26">
-        <v>434170</v>
+        <v>206268</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>7.8310339268028648E-3</v>
+        <v>1.2604960536777397E-2</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>7.8310339268028644</v>
+        <v>12.604960536777398</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -23188,134 +23206,134 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C28">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D28">
-        <v>239824</v>
+        <v>192518</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>1.1258256054439923E-2</v>
+        <v>1.194693483206765E-2</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>11.258256054439922</v>
+        <v>11.946934832067651</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="D29">
-        <v>206268</v>
+        <v>683365</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>1.2604960536777397E-2</v>
+        <v>1.1267770517951607E-2</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>12.604960536777398</v>
+        <v>11.267770517951607</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30">
-        <v>23</v>
-      </c>
       <c r="D30">
-        <v>192518</v>
+        <v>239824</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>1.194693483206765E-2</v>
+        <v>1.1258256054439923E-2</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>11.946934832067651</v>
+        <v>11.258256054439922</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C31">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D31">
-        <v>65891</v>
+        <v>116446</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>3.3388474905525795E-2</v>
+        <v>1.0305205846486783E-2</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>33.388474905525797</v>
+        <v>10.305205846486784</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C32">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D32">
-        <v>147790</v>
+        <v>148350</v>
       </c>
       <c r="E32">
         <f>100*C32/D32</f>
-        <v>1.4209351106299478E-2</v>
+        <v>9.4371418941691949E-3</v>
       </c>
       <c r="F32" s="1">
         <f>E32*1000</f>
-        <v>14.209351106299478</v>
+        <v>9.4371418941691942</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C33">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D33">
-        <v>218775</v>
+        <v>54709</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>8.2276311278711E-3</v>
+        <v>9.1392641064541487E-3</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>8.2276311278710992</v>
+        <v>9.1392641064541493</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -23342,200 +23360,200 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C35">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D35">
-        <v>148350</v>
+        <v>218775</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>9.4371418941691949E-3</v>
+        <v>8.2276311278711E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>9.4371418941691942</v>
+        <v>8.2276311278710992</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D36">
-        <v>196435</v>
+        <v>125851</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>7.1270394787079699E-3</v>
+        <v>7.9459042836369995E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>7.1270394787079701</v>
+        <v>7.9459042836369997</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C37">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D37">
-        <v>180822</v>
+        <v>434170</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>7.1893906714890887E-3</v>
+        <v>7.8310339268028648E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>7.1893906714890887</v>
+        <v>7.8310339268028644</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C38">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38">
-        <v>116446</v>
+        <v>180822</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>1.0305205846486783E-2</v>
+        <v>7.1893906714890887E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>10.305205846486784</v>
+        <v>7.1893906714890887</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C39">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D39">
-        <v>75168</v>
+        <v>196435</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>1.4633886760323542E-2</v>
+        <v>7.1270394787079699E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>14.633886760323543</v>
+        <v>7.1270394787079701</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C40">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D40">
-        <v>83826</v>
+        <v>91850</v>
       </c>
       <c r="E40">
         <f>100*C40/D40</f>
-        <v>1.3122420251473289E-2</v>
+        <v>6.5323897659226998E-3</v>
       </c>
       <c r="F40" s="1">
         <f>E40*1000</f>
-        <v>13.12242025147329</v>
+        <v>6.5323897659226997</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D41">
-        <v>125851</v>
+        <v>577212</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>7.9459042836369995E-3</v>
+        <v>6.0636300007622847E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>7.9459042836369997</v>
+        <v>6.0636300007622843</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D42">
-        <v>127998</v>
+        <v>84247</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>5.4688354505539145E-3</v>
+        <v>5.9349294336890337E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>5.4688354505539145</v>
+        <v>5.9349294336890335</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>91850</v>
+        <v>127998</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>6.5323897659226998E-3</v>
+        <v>5.4688354505539145E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>6.5323897659226997</v>
+        <v>5.4688354505539145</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -23562,46 +23580,46 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>54709</v>
+        <v>75167</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>9.1392641064541487E-3</v>
+        <v>5.3214841619327628E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>9.1392641064541493</v>
+        <v>5.3214841619327631</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>84247</v>
+        <v>80055</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>5.9349294336890337E-3</v>
+        <v>3.747423646243208E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>5.9349294336890335</v>
+        <v>3.7474236462432078</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -23628,148 +23646,148 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D48">
-        <v>75167</v>
+        <v>32394</v>
       </c>
       <c r="E48">
         <f>100*C48/D48</f>
-        <v>5.3214841619327628E-3</v>
+        <v>3.0869914181638576E-3</v>
       </c>
       <c r="F48" s="1">
         <f>E48*1000</f>
-        <v>5.3214841619327631</v>
+        <v>3.0869914181638576</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C49">
         <v>3</v>
       </c>
       <c r="D49">
-        <v>80055</v>
+        <v>133573</v>
       </c>
       <c r="E49">
         <f>100*C49/D49</f>
-        <v>3.747423646243208E-3</v>
+        <v>2.2459628817201082E-3</v>
       </c>
       <c r="F49" s="1">
         <f>E49*1000</f>
-        <v>3.7474236462432078</v>
+        <v>2.2459628817201081</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>133573</v>
+        <v>57443</v>
       </c>
       <c r="E50">
         <f>100*C50/D50</f>
-        <v>2.2459628817201082E-3</v>
+        <v>1.7408561530560731E-3</v>
       </c>
       <c r="F50" s="1">
         <f>E50*1000</f>
-        <v>2.2459628817201081</v>
+        <v>1.7408561530560731</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>32394</v>
+        <v>71544</v>
       </c>
       <c r="E51">
         <f>100*C51/D51</f>
-        <v>3.0869914181638576E-3</v>
+        <v>1.3977412501397742E-3</v>
       </c>
       <c r="F51" s="1">
         <f>E51*1000</f>
-        <v>3.0869914181638576</v>
+        <v>1.3977412501397741</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>57443</v>
+        <v>17140</v>
       </c>
       <c r="E52">
         <f>100*C52/D52</f>
-        <v>1.7408561530560731E-3</v>
+        <v>0</v>
       </c>
       <c r="F52" s="1">
         <f>E52*1000</f>
-        <v>1.7408561530560731</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>71544</v>
+        <v>1990</v>
       </c>
       <c r="E53">
         <f>100*C53/D53</f>
-        <v>1.3977412501397742E-3</v>
+        <v>0</v>
       </c>
       <c r="F53" s="1">
         <f>E53*1000</f>
-        <v>1.3977412501397741</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>17140</v>
+        <v>4863</v>
       </c>
       <c r="E54">
         <f>100*C54/D54</f>
@@ -23782,16 +23800,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>1990</v>
+        <v>7244</v>
       </c>
       <c r="E55">
         <f>100*C55/D55</f>
@@ -23804,16 +23822,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>4863</v>
+        <v>344</v>
       </c>
       <c r="E56">
         <f>100*C56/D56</f>
@@ -23826,16 +23844,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>7244</v>
+        <v>2594</v>
       </c>
       <c r="E57">
         <f>100*C57/D57</f>
@@ -23848,16 +23866,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>344</v>
+        <v>1870</v>
       </c>
       <c r="E58">
         <f>100*C58/D58</f>
@@ -23870,16 +23888,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>2594</v>
+        <v>2270</v>
       </c>
       <c r="E59">
         <f>100*C59/D59</f>
@@ -23892,16 +23910,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>1870</v>
+        <v>337</v>
       </c>
       <c r="E60">
         <f>100*C60/D60</f>
@@ -23914,16 +23932,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>2270</v>
+        <v>7096</v>
       </c>
       <c r="E61">
         <f>100*C61/D61</f>
@@ -23936,16 +23954,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>337</v>
+        <v>176</v>
       </c>
       <c r="E62">
         <f>100*C62/D62</f>
@@ -23958,16 +23976,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>7096</v>
+        <v>3055</v>
       </c>
       <c r="E63">
         <f>100*C63/D63</f>
@@ -23980,52 +23998,36 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>176</v>
-      </c>
-      <c r="E64">
-        <f>100*C64/D64</f>
-        <v>0</v>
-      </c>
-      <c r="F64" s="1">
-        <f>E64*1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+        <v>422</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C65">
-        <v>0</v>
-      </c>
-      <c r="D65">
-        <v>3055</v>
-      </c>
-      <c r="E65">
-        <f>100*C65/D65</f>
-        <v>0</v>
-      </c>
-      <c r="F65" s="1">
-        <f>E65*1000</f>
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
-    <sortCondition descending="1" ref="C2:C65"/>
+    <sortCondition descending="1" ref="F2:F65"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24037,7 +24039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258BD623-49C9-4D4B-A187-22FB1D764F55}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -24084,11 +24086,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>9.3163636923598123E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>93.163636923598119</v>
       </c>
     </row>
@@ -24106,11 +24108,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>7.6353778225160721E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>76.353778225160724</v>
       </c>
     </row>
@@ -24128,11 +24130,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>5.8808238267117244E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>58.808238267117247</v>
       </c>
     </row>
@@ -24150,11 +24152,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>4.4101696127394306E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>44.101696127394305</v>
       </c>
     </row>
@@ -24172,11 +24174,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>4.2360997499240424E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>42.360997499240426</v>
       </c>
     </row>
@@ -24194,11 +24196,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.6426156894742975E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>36.426156894742974</v>
       </c>
     </row>
@@ -24216,11 +24218,11 @@
         <v>287695</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.5801803993812893E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>35.801803993812896</v>
       </c>
     </row>
@@ -24238,11 +24240,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>3.4714124921866596E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>34.714124921866599</v>
       </c>
     </row>
@@ -24260,11 +24262,11 @@
         <v>301185</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>3.4530272091903645E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>34.530272091903647</v>
       </c>
     </row>
@@ -24282,11 +24284,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>3.3388474905525795E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>33.388474905525797</v>
       </c>
     </row>
@@ -24304,11 +24306,11 @@
         <v>209244</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>2.8674657337844814E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>28.674657337844813</v>
       </c>
     </row>
@@ -24326,11 +24328,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>2.749927408748527E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>27.499274087485269</v>
       </c>
     </row>
@@ -24348,11 +24350,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>2.738438423991681E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>27.384384239916809</v>
       </c>
     </row>
@@ -24370,11 +24372,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.2473244118794415E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>22.473244118794415</v>
       </c>
     </row>
@@ -24392,11 +24394,11 @@
         <v>454973</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.9122013833787938E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>19.122013833787939</v>
       </c>
     </row>
@@ -24414,11 +24416,11 @@
         <v>519212</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.6948760814464996E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>16.948760814464997</v>
       </c>
     </row>
@@ -24436,11 +24438,11 @@
         <v>742652</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.6831571180041256E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>16.831571180041255</v>
       </c>
     </row>
@@ -24458,11 +24460,11 @@
         <v>739575</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.6225534935604909E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>16.225534935604909</v>
       </c>
     </row>
@@ -24480,11 +24482,11 @@
         <v>147790</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.5562622640232763E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>15.562622640232762</v>
       </c>
     </row>
@@ -24502,11 +24504,11 @@
         <v>354425</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.5518092685335402E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>15.518092685335402</v>
       </c>
     </row>
@@ -24524,11 +24526,11 @@
         <v>75168</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -24546,11 +24548,11 @@
         <v>263407</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.4046703390570486E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>14.046703390570487</v>
       </c>
     </row>
@@ -24568,11 +24570,11 @@
         <v>695797</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.3797127610495589E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>13.79712761049559</v>
       </c>
     </row>
@@ -24590,11 +24592,11 @@
         <v>583702</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.3191662869066749E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>13.191662869066748</v>
       </c>
     </row>
@@ -24612,11 +24614,11 @@
         <v>83826</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.3122420251473289E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>13.12242025147329</v>
       </c>
     </row>
@@ -24634,11 +24636,11 @@
         <v>206268</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.3089766711268835E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>13.089766711268835</v>
       </c>
     </row>
@@ -24656,11 +24658,11 @@
         <v>192518</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.2466366781287984E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>12.466366781287984</v>
       </c>
     </row>
@@ -24678,11 +24680,11 @@
         <v>239824</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.2092200947361399E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>12.092200947361398</v>
       </c>
     </row>
@@ -24700,11 +24702,11 @@
         <v>683365</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.1706774564105566E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>11.706774564105565</v>
       </c>
     </row>
@@ -24722,6 +24724,1446 @@
         <v>116446</v>
       </c>
       <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>148350</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>9.4371418941691949E-3</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4371418941691942</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>218775</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>9.141812364301222E-3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>9.1418123643012219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>54709</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>125851</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>8.7404947120006994E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>8.7404947120007002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>16</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>8.420786711998569E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>8.4207867119985682</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>34</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>7.8310339268028648E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>7.8310339268028644</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>127998</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>7.8126220722198776E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>7.8126220722198774</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>180822</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>196435</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>7.1270394787079699E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1270394787079701</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>84247</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>91850</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>6.5323897659226998E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>6.5323897659226997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43">
+        <v>35</v>
+      </c>
+      <c r="D43">
+        <v>577212</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>6.0636300007622847E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>6.0636300007622843</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>112055</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>5.3545134085939937E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3545134085939941</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>75167</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>5.3214841619327628E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3214841619327631</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>80055</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>4.9965648616576101E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>4.9965648616576104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>3.3240923565820354E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3240923565820353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>105</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>437</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCA568-86EC-4316-9E72-763BED0A160B}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>251</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>9.6628400280260859E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>96.628400280260863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>279</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>7.9785408707190406E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>79.785408707190399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>142</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>6.051282488355543E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>60.512824883555432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>79</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>4.7081540460326352E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>47.081540460326352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>147</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>4.2945287119919601E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>42.945287119919598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>153</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>3.7154680032637839E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>37.154680032637842</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>104</v>
+      </c>
+      <c r="D8">
+        <v>287695</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.6149394323849914E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>36.149394323849911</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>338</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>3.5991945471137758E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>35.991945471137761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>108</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>3.5858359480053788E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>35.858359480053785</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>3.4906132855776963E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>34.90613285577696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>209244</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>3.0586301160367799E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>30.5863011603678</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>270227</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>2.8864621225858259E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>28.864621225858258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>165</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>2.8182485866056331E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>28.182485866056332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.2897267592733934E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>22.897267592733932</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.019788541604951E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>20.197885416049509</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>1.9781393621159937E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>19.781393621159935</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>138</v>
+      </c>
+      <c r="D18">
+        <v>739575</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.8659365175945644E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>18.659365175945645</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>93</v>
+      </c>
+      <c r="D19">
+        <v>519212</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.7911758588014144E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>17.911758588014145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>354425</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.6928828384002257E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>16.928828384002259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>147790</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.6239258407199406E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>16.239258407199404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>263407</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.5185625287103228E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>15.185625287103228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>75168</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>695797</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.4372007927599573E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>14.372007927599572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>81</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.3876944057070217E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>13.876944057070217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>206268</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.3574572885760272E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>13.574572885760272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>83826</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.3122420251473289E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>13.12242025147329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>86</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.2584782656413484E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>12.584782656413484</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>30</v>
+      </c>
+      <c r="D29">
+        <v>239824</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.2509173393822137E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>12.509173393822136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>192518</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.2466366781287984E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>12.466366781287984</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>116446</v>
+      </c>
+      <c r="E31">
         <f>100*C31/D31</f>
         <v>1.0305205846486783E-2</v>
       </c>
@@ -24732,178 +26174,178 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C32">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D32">
-        <v>148350</v>
+        <v>218775</v>
       </c>
       <c r="E32">
         <f>100*C32/D32</f>
-        <v>9.4371418941691949E-3</v>
+        <v>1.0055993600731346E-2</v>
       </c>
       <c r="F32" s="1">
         <f>E32*1000</f>
-        <v>9.4371418941691942</v>
+        <v>10.055993600731346</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C33">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>218775</v>
+        <v>125851</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>9.141812364301222E-3</v>
+        <v>9.5350851403643994E-3</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>9.1418123643012219</v>
+        <v>9.5350851403643997</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D34">
-        <v>54709</v>
+        <v>148350</v>
       </c>
       <c r="E34">
         <f>100*C34/D34</f>
-        <v>9.1392641064541487E-3</v>
+        <v>9.4371418941691949E-3</v>
       </c>
       <c r="F34" s="1">
         <f>E34*1000</f>
-        <v>9.1392641064541493</v>
+        <v>9.4371418941691942</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C35">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D35">
-        <v>125851</v>
+        <v>54709</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>8.7404947120006994E-3</v>
+        <v>9.1392641064541487E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>8.7404947120007002</v>
+        <v>9.1392641064541493</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
       <c r="C36">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D36">
-        <v>190006</v>
+        <v>91850</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>8.420786711998569E-3</v>
+        <v>8.7098530212302676E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>8.4207867119985682</v>
+        <v>8.7098530212302681</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
       <c r="C37">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D37">
-        <v>434170</v>
+        <v>190006</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>7.8310339268028648E-3</v>
+        <v>8.420786711998569E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>7.8310339268028644</v>
+        <v>8.4207867119985682</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C38">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D38">
-        <v>127998</v>
+        <v>434170</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>7.8126220722198776E-3</v>
+        <v>8.2916829813206808E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>7.8126220722198774</v>
+        <v>8.2916829813206814</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>180822</v>
+        <v>127998</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>7.1893906714890887E-3</v>
+        <v>7.8126220722198776E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>7.1893906714890887</v>
+        <v>7.8126220722198774</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -24914,150 +26356,150 @@
         <v>31</v>
       </c>
       <c r="C40">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D40">
         <v>196435</v>
       </c>
       <c r="E40">
         <f>100*C40/D40</f>
-        <v>7.1270394787079699E-3</v>
+        <v>7.6361137271871099E-3</v>
       </c>
       <c r="F40" s="1">
         <f>E40*1000</f>
-        <v>7.1270394787079701</v>
+        <v>7.6361137271871096</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D41">
-        <v>84247</v>
+        <v>180822</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>7.1219153204268399E-3</v>
+        <v>7.1893906714890887E-3</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>7.1219153204268402</v>
+        <v>7.1893906714890887</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C42">
         <v>6</v>
       </c>
       <c r="D42">
-        <v>91850</v>
+        <v>84247</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>6.5323897659226998E-3</v>
+        <v>7.1219153204268399E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>6.5323897659226997</v>
+        <v>7.1219153204268402</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="C43">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D43">
-        <v>577212</v>
+        <v>80055</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>6.0636300007622847E-3</v>
+        <v>6.245706077072013E-3</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>6.0636300007622843</v>
+        <v>6.245706077072013</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D44">
-        <v>112055</v>
+        <v>577212</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>5.3545134085939937E-3</v>
+        <v>6.2368765722126355E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>5.3545134085939941</v>
+        <v>6.2368765722126351</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D45">
-        <v>75167</v>
+        <v>112055</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>5.3214841619327628E-3</v>
+        <v>5.3545134085939937E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>5.3214841619327631</v>
+        <v>5.3545134085939941</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
         <v>48</v>
-      </c>
-      <c r="B46" t="s">
-        <v>53</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46">
-        <v>80055</v>
+        <v>75167</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>4.9965648616576101E-3</v>
+        <v>5.3214841619327628E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>4.9965648616576104</v>
+        <v>5.3214841619327631</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -25068,18 +26510,18 @@
         <v>44</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D47">
         <v>150417</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>3.3240923565820354E-3</v>
+        <v>3.9889108278984425E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>3.3240923565820353</v>
+        <v>3.9889108278984424</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -25442,7 +26884,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -25456,7 +26898,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
revised: data 2020/04/25 and 2020/04/26 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC2DE30-FD31-49B8-9B76-EDD5C1478777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009B1C7-FB52-445B-AE79-928DE77A575B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16884" yWindow="552" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="18" activeTab="24" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="7560" yWindow="4980" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="19" activeTab="25" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="2020年4月22日" sheetId="23" r:id="rId23"/>
     <sheet name="2020年4月23日" sheetId="24" r:id="rId24"/>
     <sheet name="2020年4月24日" sheetId="25" r:id="rId25"/>
+    <sheet name="2020年4月25日" sheetId="26" r:id="rId26"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -57,6 +58,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'2020年4月22日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'2020年4月23日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">'2020年4月24日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">'2020年4月25日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -82,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -22646,11 +22648,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>9.1623742098414673E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>91.623742098414667</v>
       </c>
     </row>
@@ -22668,11 +22670,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>7.4351993777310055E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>74.351993777310057</v>
       </c>
     </row>
@@ -22690,11 +22692,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>5.6677504996569518E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>56.677504996569517</v>
       </c>
     </row>
@@ -22712,11 +22714,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>4.3505727260807897E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>43.505727260807895</v>
       </c>
     </row>
@@ -22734,11 +22736,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>3.9731694206184123E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>39.731694206184123</v>
       </c>
     </row>
@@ -22756,11 +22758,11 @@
         <v>287695</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.5454213663775873E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>35.454213663775874</v>
       </c>
     </row>
@@ -22778,11 +22780,11 @@
         <v>411792</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.5211951664918209E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>35.21195166491821</v>
       </c>
     </row>
@@ -22800,11 +22802,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>3.3755759509913226E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>33.755759509913226</v>
       </c>
     </row>
@@ -22822,11 +22824,11 @@
         <v>65891</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>3.3388474905525795E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>33.388474905525797</v>
       </c>
     </row>
@@ -22844,11 +22846,11 @@
         <v>301185</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>3.1874097315603367E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>31.874097315603368</v>
       </c>
     </row>
@@ -22866,11 +22868,11 @@
         <v>209244</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>2.8196746382214064E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>28.196746382214066</v>
       </c>
     </row>
@@ -22888,11 +22890,11 @@
         <v>585470</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>2.6986865253556973E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>26.986865253556974</v>
       </c>
     </row>
@@ -22910,11 +22912,11 @@
         <v>270227</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>2.4793969514519273E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>24.793969514519272</v>
       </c>
     </row>
@@ -22932,11 +22934,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.1625197170915381E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>21.625197170915381</v>
       </c>
     </row>
@@ -22954,11 +22956,11 @@
         <v>454973</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.824284078395861E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>18.242840783958609</v>
       </c>
     </row>
@@ -22976,11 +22978,11 @@
         <v>519212</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.6370962150335507E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>16.370962150335508</v>
       </c>
     </row>
@@ -22998,11 +23000,11 @@
         <v>742652</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.6292960902279937E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>16.292960902279937</v>
       </c>
     </row>
@@ -23020,11 +23022,11 @@
         <v>354425</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.4953798405868661E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>14.95379840586866</v>
       </c>
     </row>
@@ -23042,11 +23044,11 @@
         <v>739575</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.4738194233174459E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>14.738194233174459</v>
       </c>
     </row>
@@ -23064,11 +23066,11 @@
         <v>75168</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -23086,11 +23088,11 @@
         <v>147790</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.4209351106299478E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>14.209351106299478</v>
       </c>
     </row>
@@ -23108,11 +23110,11 @@
         <v>83826</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.3122420251473289E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>13.12242025147329</v>
       </c>
     </row>
@@ -23130,11 +23132,11 @@
         <v>583702</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.3020342572065883E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>13.020342572065884</v>
       </c>
     </row>
@@ -23152,11 +23154,11 @@
         <v>695797</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.2934807134839615E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>12.934807134839614</v>
       </c>
     </row>
@@ -23174,11 +23176,11 @@
         <v>206268</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.2604960536777397E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>12.604960536777398</v>
       </c>
     </row>
@@ -23196,11 +23198,11 @@
         <v>263407</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.2528140861860163E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>12.528140861860162</v>
       </c>
     </row>
@@ -23218,11 +23220,11 @@
         <v>192518</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.194693483206765E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>11.946934832067651</v>
       </c>
     </row>
@@ -23240,11 +23242,11 @@
         <v>683365</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.1267770517951607E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>11.267770517951607</v>
       </c>
     </row>
@@ -23262,11 +23264,11 @@
         <v>239824</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.1258256054439923E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>11.258256054439922</v>
       </c>
     </row>
@@ -23284,11 +23286,11 @@
         <v>116446</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -23306,11 +23308,11 @@
         <v>148350</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>9.4371418941691949E-3</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>9.4371418941691942</v>
       </c>
     </row>
@@ -23328,11 +23330,11 @@
         <v>54709</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -23350,11 +23352,11 @@
         <v>190006</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>8.420786711998569E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>8.4207867119985682</v>
       </c>
     </row>
@@ -23372,11 +23374,11 @@
         <v>218775</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>8.2276311278711E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>8.2276311278710992</v>
       </c>
     </row>
@@ -23394,11 +23396,11 @@
         <v>125851</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>7.9459042836369995E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>7.9459042836369997</v>
       </c>
     </row>
@@ -23416,11 +23418,11 @@
         <v>434170</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>7.8310339268028648E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>7.8310339268028644</v>
       </c>
     </row>
@@ -23438,11 +23440,11 @@
         <v>180822</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -23460,11 +23462,11 @@
         <v>196435</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>7.1270394787079699E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1270394787079701</v>
       </c>
     </row>
@@ -23482,11 +23484,11 @@
         <v>91850</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>6.5323897659226998E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>6.5323897659226997</v>
       </c>
     </row>
@@ -23504,11 +23506,11 @@
         <v>577212</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>6.0636300007622847E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>6.0636300007622843</v>
       </c>
     </row>
@@ -23526,11 +23528,11 @@
         <v>84247</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>5.9349294336890337E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>5.9349294336890335</v>
       </c>
     </row>
@@ -23548,11 +23550,11 @@
         <v>127998</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>5.4688354505539145E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>5.4688354505539145</v>
       </c>
     </row>
@@ -23570,11 +23572,11 @@
         <v>112055</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>5.3545134085939937E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>5.3545134085939941</v>
       </c>
     </row>
@@ -23592,11 +23594,11 @@
         <v>75167</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>5.3214841619327628E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>5.3214841619327631</v>
       </c>
     </row>
@@ -23614,11 +23616,11 @@
         <v>80055</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>3.747423646243208E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>3.7474236462432078</v>
       </c>
     </row>
@@ -23636,11 +23638,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>3.3240923565820354E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>3.3240923565820353</v>
       </c>
     </row>
@@ -23658,11 +23660,11 @@
         <v>32394</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -23680,11 +23682,11 @@
         <v>133573</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -23702,11 +23704,11 @@
         <v>57443</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>1.7408561530560731E-3</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7408561530560731</v>
       </c>
     </row>
@@ -23724,11 +23726,11 @@
         <v>71544</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -23746,11 +23748,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23768,11 +23770,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23790,11 +23792,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23812,11 +23814,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23834,11 +23836,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23856,11 +23858,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23878,11 +23880,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23900,11 +23902,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23922,11 +23924,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23944,11 +23946,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23966,11 +23968,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -23988,11 +23990,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -24790,11 +24792,11 @@
         <v>54709</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -25479,7 +25481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCA568-86EC-4316-9E72-763BED0A160B}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -25526,11 +25528,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>9.6628400280260859E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>96.628400280260863</v>
       </c>
     </row>
@@ -25548,11 +25550,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>7.9785408707190406E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>79.785408707190399</v>
       </c>
     </row>
@@ -25570,11 +25572,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>6.051282488355543E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>60.512824883555432</v>
       </c>
     </row>
@@ -25592,11 +25594,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>4.7081540460326352E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>47.081540460326352</v>
       </c>
     </row>
@@ -25614,11 +25616,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>4.2945287119919601E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>42.945287119919598</v>
       </c>
     </row>
@@ -25636,11 +25638,11 @@
         <v>411792</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.7154680032637839E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>37.154680032637842</v>
       </c>
     </row>
@@ -25658,11 +25660,11 @@
         <v>287695</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.6149394323849914E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>36.149394323849911</v>
       </c>
     </row>
@@ -25680,11 +25682,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>3.5991945471137758E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>35.991945471137761</v>
       </c>
     </row>
@@ -25702,11 +25704,11 @@
         <v>301185</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>3.5858359480053788E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>35.858359480053785</v>
       </c>
     </row>
@@ -25724,11 +25726,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>3.4906132855776963E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>34.90613285577696</v>
       </c>
     </row>
@@ -25746,11 +25748,11 @@
         <v>209244</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>3.0586301160367799E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>30.5863011603678</v>
       </c>
     </row>
@@ -25768,11 +25770,11 @@
         <v>270227</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>2.8864621225858259E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>28.864621225858258</v>
       </c>
     </row>
@@ -25790,11 +25792,11 @@
         <v>585470</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>2.8182485866056331E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>28.182485866056332</v>
       </c>
     </row>
@@ -25812,11 +25814,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.2897267592733934E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>22.897267592733932</v>
       </c>
     </row>
@@ -25834,11 +25836,11 @@
         <v>742652</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>2.019788541604951E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>20.197885416049509</v>
       </c>
     </row>
@@ -25856,11 +25858,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.9781393621159937E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>19.781393621159935</v>
       </c>
     </row>
@@ -25878,11 +25880,11 @@
         <v>739575</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.8659365175945644E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>18.659365175945645</v>
       </c>
     </row>
@@ -25900,11 +25902,11 @@
         <v>519212</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.7911758588014144E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>17.911758588014145</v>
       </c>
     </row>
@@ -25922,11 +25924,11 @@
         <v>354425</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.6928828384002257E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>16.928828384002259</v>
       </c>
     </row>
@@ -25944,11 +25946,11 @@
         <v>147790</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.6239258407199406E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>16.239258407199404</v>
       </c>
     </row>
@@ -25966,11 +25968,11 @@
         <v>263407</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.5185625287103228E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>15.185625287103228</v>
       </c>
     </row>
@@ -25988,11 +25990,11 @@
         <v>75168</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -26010,11 +26012,11 @@
         <v>695797</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.4372007927599573E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>14.372007927599572</v>
       </c>
     </row>
@@ -26032,11 +26034,11 @@
         <v>583702</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.3876944057070217E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>13.876944057070217</v>
       </c>
     </row>
@@ -26054,11 +26056,11 @@
         <v>206268</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.3574572885760272E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>13.574572885760272</v>
       </c>
     </row>
@@ -26076,11 +26078,11 @@
         <v>83826</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.3122420251473289E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>13.12242025147329</v>
       </c>
     </row>
@@ -26098,11 +26100,11 @@
         <v>683365</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.2584782656413484E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>12.584782656413484</v>
       </c>
     </row>
@@ -26120,11 +26122,11 @@
         <v>239824</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.2509173393822137E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>12.509173393822136</v>
       </c>
     </row>
@@ -26142,11 +26144,11 @@
         <v>192518</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.2466366781287984E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>12.466366781287984</v>
       </c>
     </row>
@@ -26164,11 +26166,11 @@
         <v>116446</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -26186,11 +26188,11 @@
         <v>218775</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>1.0055993600731346E-2</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>10.055993600731346</v>
       </c>
     </row>
@@ -26208,11 +26210,11 @@
         <v>125851</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>9.5350851403643994E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>9.5350851403643997</v>
       </c>
     </row>
@@ -26230,11 +26232,11 @@
         <v>148350</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>9.4371418941691949E-3</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>9.4371418941691942</v>
       </c>
     </row>
@@ -26252,11 +26254,11 @@
         <v>54709</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -26274,11 +26276,11 @@
         <v>91850</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>8.7098530212302676E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>8.7098530212302681</v>
       </c>
     </row>
@@ -26296,11 +26298,11 @@
         <v>190006</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>8.420786711998569E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>8.4207867119985682</v>
       </c>
     </row>
@@ -26318,11 +26320,11 @@
         <v>434170</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>8.2916829813206808E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>8.2916829813206814</v>
       </c>
     </row>
@@ -26340,11 +26342,11 @@
         <v>127998</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>7.8126220722198776E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>7.8126220722198774</v>
       </c>
     </row>
@@ -26362,11 +26364,11 @@
         <v>196435</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>7.6361137271871099E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>7.6361137271871096</v>
       </c>
     </row>
@@ -26384,11 +26386,11 @@
         <v>180822</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -26406,11 +26408,11 @@
         <v>84247</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>7.1219153204268399E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1219153204268402</v>
       </c>
     </row>
@@ -26428,11 +26430,11 @@
         <v>80055</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>6.245706077072013E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>6.245706077072013</v>
       </c>
     </row>
@@ -26450,11 +26452,11 @@
         <v>577212</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>6.2368765722126355E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>6.2368765722126351</v>
       </c>
     </row>
@@ -26472,11 +26474,11 @@
         <v>112055</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>5.3545134085939937E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>5.3545134085939941</v>
       </c>
     </row>
@@ -26494,11 +26496,11 @@
         <v>75167</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>5.3214841619327628E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>5.3214841619327631</v>
       </c>
     </row>
@@ -26516,11 +26518,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>3.9889108278984425E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>3.9889108278984424</v>
       </c>
     </row>
@@ -26538,11 +26540,11 @@
         <v>32394</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -26560,11 +26562,11 @@
         <v>133573</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -26582,11 +26584,11 @@
         <v>57443</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>1.7408561530560731E-3</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7408561530560731</v>
       </c>
     </row>
@@ -26604,11 +26606,11 @@
         <v>71544</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -26626,11 +26628,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26648,11 +26650,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26670,11 +26672,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26692,11 +26694,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26714,11 +26716,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26736,11 +26738,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26758,11 +26760,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26780,11 +26782,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26802,11 +26804,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26824,11 +26826,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26846,11 +26848,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26868,11 +26870,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26908,6 +26910,1446 @@
   <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
     <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B538B7-B887-4BD9-A463-31F3778D7F18}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>251</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>9.6628400280260859E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>96.628400280260863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>282</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>8.0643316327697834E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>80.643316327697832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>145</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>6.1791264845884063E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>61.791264845884065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>79</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>4.7081540460326352E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>47.081540460326352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>148</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>4.3237431930259189E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>43.237431930259191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>109</v>
+      </c>
+      <c r="D7">
+        <v>287695</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>3.7887345974035001E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>37.887345974035</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>155</v>
+      </c>
+      <c r="D8">
+        <v>411792</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.7640362124567742E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>37.640362124567744</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>349</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>3.716328097463633E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>37.163280974636329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>109</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>3.619038132709132E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>36.190381327091323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>3.4906132855776963E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>34.90613285577696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>85</v>
+      </c>
+      <c r="D12">
+        <v>270227</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>3.1455035951255796E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>31.455035951255795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>3.1064212115998548E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>31.064212115998547</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>173</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>2.9548909423198457E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>29.548909423198456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>57</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.4169338014552486E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>24.169338014552487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>157</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.1140453402131821E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>21.140453402131822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>2.0440773408531936E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>20.440773408531935</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>147790</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.8945801475065971E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>18.94580147506597</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>140</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.8929790758205726E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>18.929790758205726</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>95</v>
+      </c>
+      <c r="D20">
+        <v>519212</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.8296957697433804E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>18.296957697433804</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>354425</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.7210975523735628E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>17.210975523735627</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>263407</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.7083828447991133E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>17.083828447991131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>102</v>
+      </c>
+      <c r="D23">
+        <v>695797</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.4659448086151564E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>14.659448086151563</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>75168</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>84</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.4390904948072818E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>14.390904948072818</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>83826</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.4315367547061772E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>14.315367547061772</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <v>206268</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.4059379060251712E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>14.059379060251713</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.3170121384618762E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>13.170121384618762</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <v>192518</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.2985798730508317E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>12.985798730508316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.2509173393822137E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>12.509173393822136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>125851</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>1.0329675568728099E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>10.329675568728099</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>116446</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>1.0111223458038422E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>10.111223458038422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>218775</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>1.0055993600731346E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>10.055993600731346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>91850</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>127998</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>9.3751464866638542E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>9.375146486663855</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>54709</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>39</v>
+      </c>
+      <c r="D38">
+        <v>434170</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>8.9826565630974041E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>8.9826565630974038</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39">
+        <v>17</v>
+      </c>
+      <c r="D39">
+        <v>190006</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>8.9470858814984788E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>8.9470858814984791</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>196435</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>80055</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>7.494847292486416E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>7.4948472924864156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42">
+        <v>13</v>
+      </c>
+      <c r="D42">
+        <v>180822</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>84247</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>75167</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>6.6518552024159537E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>6.6518552024159536</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>38</v>
+      </c>
+      <c r="D45">
+        <v>577212</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>6.5833697151133378E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>6.5833697151133377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>6.246932310026326E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>6.2469323100263257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>3.9889108278984425E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>3.9889108278984424</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>115</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>442</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
+    <sortCondition descending="1" ref="F2:F66"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revised: data 2020/04/26 and 2020/04/27 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009B1C7-FB52-445B-AE79-928DE77A575B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AF6783-E2DF-4A8D-9895-54CF290D0474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="4980" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="19" activeTab="25" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="7860" yWindow="3264" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="20" activeTab="26" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
     <sheet name="2020年4月23日" sheetId="24" r:id="rId24"/>
     <sheet name="2020年4月24日" sheetId="25" r:id="rId25"/>
     <sheet name="2020年4月25日" sheetId="26" r:id="rId26"/>
+    <sheet name="2020年4月26日" sheetId="27" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -59,6 +60,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'2020年4月23日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">'2020年4月24日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">'2020年4月25日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">'2020年4月26日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -84,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -23352,11 +23354,11 @@
         <v>190006</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>8.420786711998569E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>8.4207867119985682</v>
       </c>
     </row>
@@ -26232,11 +26234,11 @@
         <v>148350</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>9.4371418941691949E-3</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>9.4371418941691942</v>
       </c>
     </row>
@@ -26921,7 +26923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B538B7-B887-4BD9-A463-31F3778D7F18}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -26968,11 +26970,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>9.6628400280260859E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>96.628400280260863</v>
       </c>
     </row>
@@ -26990,11 +26992,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>8.0643316327697834E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>80.643316327697832</v>
       </c>
     </row>
@@ -27012,11 +27014,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>6.1791264845884063E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>61.791264845884065</v>
       </c>
     </row>
@@ -27034,11 +27036,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>4.7081540460326352E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>47.081540460326352</v>
       </c>
     </row>
@@ -27056,11 +27058,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>4.3237431930259189E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>43.237431930259191</v>
       </c>
     </row>
@@ -27078,11 +27080,11 @@
         <v>287695</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.7887345974035001E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>37.887345974035</v>
       </c>
     </row>
@@ -27100,11 +27102,11 @@
         <v>411792</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.7640362124567742E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>37.640362124567744</v>
       </c>
     </row>
@@ -27122,11 +27124,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>3.716328097463633E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>37.163280974636329</v>
       </c>
     </row>
@@ -27144,11 +27146,11 @@
         <v>301185</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>3.619038132709132E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>36.190381327091323</v>
       </c>
     </row>
@@ -27166,11 +27168,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>3.4906132855776963E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>34.90613285577696</v>
       </c>
     </row>
@@ -27188,11 +27190,11 @@
         <v>270227</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>3.1455035951255796E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>31.455035951255795</v>
       </c>
     </row>
@@ -27210,11 +27212,11 @@
         <v>209244</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>3.1064212115998548E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>31.064212115998547</v>
       </c>
     </row>
@@ -27232,11 +27234,11 @@
         <v>585470</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>2.9548909423198457E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>29.548909423198456</v>
       </c>
     </row>
@@ -27254,11 +27256,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.4169338014552486E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>24.169338014552487</v>
       </c>
     </row>
@@ -27276,11 +27278,11 @@
         <v>742652</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>2.1140453402131821E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>21.140453402131822</v>
       </c>
     </row>
@@ -27298,11 +27300,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>2.0440773408531936E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>20.440773408531935</v>
       </c>
     </row>
@@ -27320,11 +27322,11 @@
         <v>147790</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.8945801475065971E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>18.94580147506597</v>
       </c>
     </row>
@@ -27342,11 +27344,11 @@
         <v>739575</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.8929790758205726E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>18.929790758205726</v>
       </c>
     </row>
@@ -27364,11 +27366,11 @@
         <v>519212</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.8296957697433804E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>18.296957697433804</v>
       </c>
     </row>
@@ -27386,11 +27388,11 @@
         <v>354425</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.7210975523735628E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>17.210975523735627</v>
       </c>
     </row>
@@ -27408,11 +27410,11 @@
         <v>263407</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.7083828447991133E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>17.083828447991131</v>
       </c>
     </row>
@@ -27430,11 +27432,11 @@
         <v>695797</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.4659448086151564E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>14.659448086151563</v>
       </c>
     </row>
@@ -27452,11 +27454,11 @@
         <v>75168</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -27474,11 +27476,11 @@
         <v>583702</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.4390904948072818E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>14.390904948072818</v>
       </c>
     </row>
@@ -27496,11 +27498,11 @@
         <v>83826</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.4315367547061772E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>14.315367547061772</v>
       </c>
     </row>
@@ -27518,11 +27520,11 @@
         <v>206268</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.4059379060251712E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>14.059379060251713</v>
       </c>
     </row>
@@ -27540,11 +27542,11 @@
         <v>683365</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.3170121384618762E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>13.170121384618762</v>
       </c>
     </row>
@@ -27562,11 +27564,11 @@
         <v>192518</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.2985798730508317E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>12.985798730508316</v>
       </c>
     </row>
@@ -27584,11 +27586,11 @@
         <v>239824</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.2509173393822137E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>12.509173393822136</v>
       </c>
     </row>
@@ -27606,11 +27608,11 @@
         <v>125851</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>1.0329675568728099E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>10.329675568728099</v>
       </c>
     </row>
@@ -27628,11 +27630,11 @@
         <v>116446</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -27650,11 +27652,11 @@
         <v>148350</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>1.0111223458038422E-2</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>10.111223458038422</v>
       </c>
     </row>
@@ -27672,11 +27674,11 @@
         <v>218775</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>1.0055993600731346E-2</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>10.055993600731346</v>
       </c>
     </row>
@@ -27694,11 +27696,11 @@
         <v>91850</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>9.7985846488840497E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>9.7985846488840505</v>
       </c>
     </row>
@@ -27716,11 +27718,11 @@
         <v>127998</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>9.3751464866638542E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>9.375146486663855</v>
       </c>
     </row>
@@ -27738,11 +27740,11 @@
         <v>54709</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -27760,11 +27762,11 @@
         <v>434170</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>8.9826565630974041E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>8.9826565630974038</v>
       </c>
     </row>
@@ -27782,11 +27784,11 @@
         <v>190006</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>8.9470858814984788E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>8.9470858814984791</v>
       </c>
     </row>
@@ -27804,11 +27806,11 @@
         <v>196435</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>8.1451879756662508E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>8.14518797566625</v>
       </c>
     </row>
@@ -27826,11 +27828,11 @@
         <v>80055</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>7.494847292486416E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>7.4948472924864156</v>
       </c>
     </row>
@@ -27848,11 +27850,11 @@
         <v>180822</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -27870,11 +27872,11 @@
         <v>84247</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>7.1219153204268399E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1219153204268402</v>
       </c>
     </row>
@@ -27892,11 +27894,11 @@
         <v>75167</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>6.6518552024159537E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>6.6518552024159536</v>
       </c>
     </row>
@@ -27914,11 +27916,11 @@
         <v>577212</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>6.5833697151133378E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>6.5833697151133377</v>
       </c>
     </row>
@@ -27936,11 +27938,11 @@
         <v>112055</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>6.246932310026326E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>6.2469323100263257</v>
       </c>
     </row>
@@ -27958,11 +27960,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>3.9889108278984425E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>3.9889108278984424</v>
       </c>
     </row>
@@ -27980,11 +27982,11 @@
         <v>32394</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -28002,11 +28004,11 @@
         <v>133573</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -28024,11 +28026,11 @@
         <v>57443</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>1.7408561530560731E-3</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7408561530560731</v>
       </c>
     </row>
@@ -28046,11 +28048,11 @@
         <v>71544</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -28068,11 +28070,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28090,11 +28092,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28112,11 +28114,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28134,11 +28136,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28156,11 +28158,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28178,11 +28180,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28200,11 +28202,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28222,11 +28224,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28244,11 +28246,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28266,11 +28268,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28288,11 +28290,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28310,11 +28312,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -28350,6 +28352,1446 @@
   <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
     <sortCondition descending="1" ref="F2:F66"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B5E810-FF4A-4AAB-B791-4D14A934399B}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>261</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>0.10047813734321946</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>100.47813734321946</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>289</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>8.2645100775548486E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>82.645100775548485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>147</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>6.2643558154103149E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>62.643558154103147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>4.7677509326912761E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>47.677509326912762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>148</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>4.3237431930259189E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>43.237431930259191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>358</v>
+      </c>
+      <c r="D7">
+        <v>939099</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>3.81216463865897E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>38.121646386589703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>109</v>
+      </c>
+      <c r="D8">
+        <v>287695</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.7887345974035001E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>37.887345974035</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>156</v>
+      </c>
+      <c r="D9">
+        <v>411792</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>3.7883203170532696E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>37.883203170532695</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>109</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>3.619038132709132E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>36.190381327091323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>3.4906132855776963E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>34.90613285577696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>86</v>
+      </c>
+      <c r="D12">
+        <v>270227</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>3.1825095197741161E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>31.825095197741163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>3.1064212115998548E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>31.064212115998547</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>176</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>3.0061318257126754E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>30.061318257126754</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>59</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.501738496243152E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>25.017384962431521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>157</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.1140453402131821E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>21.140453402131822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>2.0440773408531936E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>20.440773408531935</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>101</v>
+      </c>
+      <c r="D18">
+        <v>519212</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>1.9452555025692781E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>19.452555025692781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19">
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <v>147790</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.8945801475065971E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>18.94580147506597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>140</v>
+      </c>
+      <c r="D20">
+        <v>739575</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.8929790758205726E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>18.929790758205726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>46</v>
+      </c>
+      <c r="D21">
+        <v>263407</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.7463469080168711E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>17.463469080168711</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>354425</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.7210975523735628E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>17.210975523735627</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>107</v>
+      </c>
+      <c r="D23">
+        <v>695797</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.5378048482531543E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>15.378048482531543</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>75168</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>85</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.4562225245073685E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>14.562225245073686</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>206268</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.454418523474315E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>14.54418523474315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>83826</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.4315367547061772E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>14.315367547061772</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.3170121384618762E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>13.170121384618762</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <v>192518</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.2985798730508317E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>12.985798730508316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>31</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.2926145840282875E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>12.926145840282874</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>125851</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>116446</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>1.0111223458038422E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>10.111223458038422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>218775</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>1.0055993600731346E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>10.055993600731346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>91850</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>54709</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>39</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>8.9826565630974041E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>8.9826565630974038</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <v>17</v>
+      </c>
+      <c r="D38">
+        <v>190006</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>8.9470858814984788E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>8.9470858814984791</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>127998</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>196435</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>75167</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>80055</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>7.494847292486416E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>7.4948472924864156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>84247</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>38</v>
+      </c>
+      <c r="D45">
+        <v>577212</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>6.5833697151133378E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>6.5833697151133377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>6.246932310026326E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>6.2469323100263257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>3.9889108278984425E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>3.9889108278984424</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>118</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>459</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revised: data 2020/04/27 and 2020/04/28 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AF6783-E2DF-4A8D-9895-54CF290D0474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F28A673-E52D-4F7E-BAB8-F814ADBD459B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="3264" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="20" activeTab="26" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="16404" yWindow="3036" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="21" activeTab="27" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,7 @@
     <sheet name="2020年4月24日" sheetId="25" r:id="rId25"/>
     <sheet name="2020年4月25日" sheetId="26" r:id="rId26"/>
     <sheet name="2020年4月26日" sheetId="27" r:id="rId27"/>
+    <sheet name="2020年4月27日" sheetId="28" r:id="rId28"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -61,6 +62,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">'2020年4月24日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">'2020年4月25日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">'2020年4月26日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">'2020年4月27日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -86,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -27674,11 +27676,11 @@
         <v>218775</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.0055993600731346E-2</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>10.055993600731346</v>
       </c>
     </row>
@@ -28363,7 +28365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B5E810-FF4A-4AAB-B791-4D14A934399B}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -28410,6 +28412,1446 @@
         <v>259758</v>
       </c>
       <c r="E2">
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
+        <v>0.10047813734321946</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
+        <v>100.47813734321946</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>289</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>8.2645100775548486E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
+        <v>82.645100775548485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>147</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6.2643558154103149E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>62.643558154103147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4.7677509326912761E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>47.677509326912762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>148</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4.3237431930259189E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>43.237431930259191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>358</v>
+      </c>
+      <c r="D7">
+        <v>939099</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3.81216463865897E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>38.121646386589703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>109</v>
+      </c>
+      <c r="D8">
+        <v>287695</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>3.7887345974035001E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>37.887345974035</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>156</v>
+      </c>
+      <c r="D9">
+        <v>411792</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3.7883203170532696E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>37.883203170532695</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>109</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3.619038132709132E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>36.190381327091323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3.4906132855776963E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>34.90613285577696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>86</v>
+      </c>
+      <c r="D12">
+        <v>270227</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3.1825095197741161E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>31.825095197741163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3.1064212115998548E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>31.064212115998547</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>176</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3.0061318257126754E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>30.061318257126754</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>59</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2.501738496243152E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>25.017384962431521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>157</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2.1140453402131821E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>21.140453402131822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2.0440773408531936E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>20.440773408531935</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>101</v>
+      </c>
+      <c r="D18">
+        <v>519212</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.9452555025692781E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>19.452555025692781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19">
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <v>147790</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.8945801475065971E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>18.94580147506597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>140</v>
+      </c>
+      <c r="D20">
+        <v>739575</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1.8929790758205726E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>18.929790758205726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>46</v>
+      </c>
+      <c r="D21">
+        <v>263407</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.7463469080168711E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>17.463469080168711</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>354425</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.7210975523735628E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>17.210975523735627</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>107</v>
+      </c>
+      <c r="D23">
+        <v>695797</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.5378048482531543E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>15.378048482531543</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>75168</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>85</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.4562225245073685E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>14.562225245073686</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>206268</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.454418523474315E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>14.54418523474315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>83826</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.4315367547061772E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>14.315367547061772</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.3170121384618762E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>13.170121384618762</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <v>192518</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.2985798730508317E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>12.985798730508316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>31</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.2926145840282875E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>12.926145840282874</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>125851</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>116446</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.0111223458038422E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>10.111223458038422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>218775</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>1.0055993600731346E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>10.055993600731346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>91850</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>54709</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>39</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>8.9826565630974041E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>8.9826565630974038</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <v>17</v>
+      </c>
+      <c r="D38">
+        <v>190006</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>8.9470858814984788E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>8.9470858814984791</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>127998</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>196435</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>75167</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>80055</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>7.494847292486416E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>7.4948472924864156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>84247</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>38</v>
+      </c>
+      <c r="D45">
+        <v>577212</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>6.5833697151133378E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>6.5833697151133377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>6.246932310026326E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>6.2469323100263257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>3.9889108278984425E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9889108278984424</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>118</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>459</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72046AEB-A0FE-400B-816D-2BEAC20AE159}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>261</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
         <f>100*C2/D2</f>
         <v>0.10047813734321946</v>
       </c>
@@ -28426,18 +29868,18 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="D3">
         <v>349688</v>
       </c>
       <c r="E3">
         <f>100*C3/D3</f>
-        <v>8.2645100775548486E-2</v>
+        <v>8.4646885223399138E-2</v>
       </c>
       <c r="F3" s="1">
         <f>E3*1000</f>
-        <v>82.645100775548485</v>
+        <v>84.646885223399138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -28448,18 +29890,18 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D4">
         <v>234661</v>
       </c>
       <c r="E4">
         <f>100*C4/D4</f>
-        <v>6.2643558154103149E-2</v>
+        <v>6.3495851462322242E-2</v>
       </c>
       <c r="F4" s="1">
         <f>E4*1000</f>
-        <v>62.643558154103147</v>
+        <v>63.495851462322243</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -28470,18 +29912,18 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D5">
         <v>167794</v>
       </c>
       <c r="E5">
         <f>100*C5/D5</f>
-        <v>4.7677509326912761E-2</v>
+        <v>5.0061384793258397E-2</v>
       </c>
       <c r="F5" s="1">
         <f>E5*1000</f>
-        <v>47.677509326912762</v>
+        <v>50.061384793258398</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -28492,62 +29934,62 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D6">
         <v>342296</v>
       </c>
       <c r="E6">
         <f>100*C6/D6</f>
-        <v>4.3237431930259189E-2</v>
+        <v>4.4113866361277961E-2</v>
       </c>
       <c r="F6" s="1">
         <f>E6*1000</f>
-        <v>43.237431930259191</v>
+        <v>44.113866361277964</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>358</v>
+        <v>115</v>
       </c>
       <c r="D7">
-        <v>939099</v>
+        <v>287695</v>
       </c>
       <c r="E7">
         <f>100*C7/D7</f>
-        <v>3.81216463865897E-2</v>
+        <v>3.9972887954257109E-2</v>
       </c>
       <c r="F7" s="1">
         <f>E7*1000</f>
-        <v>38.121646386589703</v>
+        <v>39.972887954257111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>109</v>
+        <v>366</v>
       </c>
       <c r="D8">
-        <v>287695</v>
+        <v>939099</v>
       </c>
       <c r="E8">
         <f>100*C8/D8</f>
-        <v>3.7887345974035001E-2</v>
+        <v>3.8973526752770472E-2</v>
       </c>
       <c r="F8" s="1">
         <f>E8*1000</f>
-        <v>37.887345974035</v>
+        <v>38.973526752770475</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -28624,18 +30066,18 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12">
         <v>270227</v>
       </c>
       <c r="E12">
         <f>100*C12/D12</f>
-        <v>3.1825095197741161E-2</v>
+        <v>3.219515444422652E-2</v>
       </c>
       <c r="F12" s="1">
         <f>E12*1000</f>
-        <v>31.825095197741163</v>
+        <v>32.195154444226517</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -28668,18 +30110,18 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D14">
         <v>585470</v>
       </c>
       <c r="E14">
         <f>100*C14/D14</f>
-        <v>3.0061318257126754E-2</v>
+        <v>3.0232121201769518E-2</v>
       </c>
       <c r="F14" s="1">
         <f>E14*1000</f>
-        <v>30.061318257126754</v>
+        <v>30.23212120176952</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -28882,24 +30324,24 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D24">
-        <v>75168</v>
+        <v>206268</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>1.4633886760323542E-2</v>
+        <v>1.5028991409234587E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>14.633886760323543</v>
+        <v>15.028991409234587</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -28910,40 +30352,40 @@
         <v>18</v>
       </c>
       <c r="C25">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D25">
         <v>583702</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>1.4562225245073685E-2</v>
+        <v>1.4733545542074553E-2</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>14.562225245073686</v>
+        <v>14.733545542074552</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C26">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D26">
-        <v>206268</v>
+        <v>75168</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>1.454418523474315E-2</v>
+        <v>1.4633886760323542E-2</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>14.54418523474315</v>
+        <v>14.633886760323543</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -29146,46 +30588,46 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D36">
-        <v>54709</v>
+        <v>434170</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>9.1392641064541487E-3</v>
+        <v>9.2129810903563113E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>9.1392641064541493</v>
+        <v>9.2129810903563119</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C37">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="D37">
-        <v>434170</v>
+        <v>54709</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>8.9826565630974041E-3</v>
+        <v>9.1392641064541487E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>8.9826565630974038</v>
+        <v>9.1392641064541493</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -29394,18 +30836,18 @@
         <v>44</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D47">
         <v>150417</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>3.9889108278984425E-3</v>
+        <v>4.6537292992148496E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>3.9889108278984424</v>
+        <v>4.6537292992148496</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -29768,7 +31210,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -29782,7 +31224,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Revised: data 20200428 and 20200429 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F28A673-E52D-4F7E-BAB8-F814ADBD459B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AC0ECC-A381-408A-B5BB-D05B7E8EF334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16404" yWindow="3036" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="21" activeTab="27" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="5400" yWindow="984" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="22" activeTab="28" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <sheet name="2020年4月25日" sheetId="26" r:id="rId26"/>
     <sheet name="2020年4月26日" sheetId="27" r:id="rId27"/>
     <sheet name="2020年4月27日" sheetId="28" r:id="rId28"/>
+    <sheet name="2020年4月28日" sheetId="29" r:id="rId29"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -63,6 +64,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">'2020年4月25日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">'2020年4月26日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">'2020年4月27日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">'2020年4月28日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -88,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -29116,11 +29118,11 @@
         <v>218775</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.0055993600731346E-2</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>10.055993600731346</v>
       </c>
     </row>
@@ -29805,8 +29807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72046AEB-A0FE-400B-816D-2BEAC20AE159}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -29852,11 +29854,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>0.10047813734321946</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>100.47813734321946</v>
       </c>
     </row>
@@ -29874,11 +29876,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>8.4646885223399138E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>84.646885223399138</v>
       </c>
     </row>
@@ -29896,11 +29898,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>6.3495851462322242E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>63.495851462322243</v>
       </c>
     </row>
@@ -29918,11 +29920,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>5.0061384793258397E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>50.061384793258398</v>
       </c>
     </row>
@@ -29940,11 +29942,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>4.4113866361277961E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>44.113866361277964</v>
       </c>
     </row>
@@ -29962,11 +29964,11 @@
         <v>287695</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.9972887954257109E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>39.972887954257111</v>
       </c>
     </row>
@@ -29984,11 +29986,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.8973526752770472E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>38.973526752770475</v>
       </c>
     </row>
@@ -30006,11 +30008,11 @@
         <v>411792</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>3.7883203170532696E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>37.883203170532695</v>
       </c>
     </row>
@@ -30028,11 +30030,11 @@
         <v>301185</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>3.619038132709132E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>36.190381327091323</v>
       </c>
     </row>
@@ -30050,11 +30052,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>3.4906132855776963E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>34.90613285577696</v>
       </c>
     </row>
@@ -30072,11 +30074,11 @@
         <v>270227</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>3.219515444422652E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>32.195154444226517</v>
       </c>
     </row>
@@ -30094,11 +30096,11 @@
         <v>209244</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>3.1064212115998548E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>31.064212115998547</v>
       </c>
     </row>
@@ -30116,11 +30118,11 @@
         <v>585470</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>3.0232121201769518E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>30.23212120176952</v>
       </c>
     </row>
@@ -30138,11 +30140,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.501738496243152E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>25.017384962431521</v>
       </c>
     </row>
@@ -30160,11 +30162,11 @@
         <v>742652</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>2.1140453402131821E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>21.140453402131822</v>
       </c>
     </row>
@@ -30182,11 +30184,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>2.0440773408531936E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>20.440773408531935</v>
       </c>
     </row>
@@ -30204,11 +30206,11 @@
         <v>519212</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.9452555025692781E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>19.452555025692781</v>
       </c>
     </row>
@@ -30226,11 +30228,11 @@
         <v>147790</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.8945801475065971E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>18.94580147506597</v>
       </c>
     </row>
@@ -30248,11 +30250,11 @@
         <v>739575</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.8929790758205726E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>18.929790758205726</v>
       </c>
     </row>
@@ -30270,11 +30272,11 @@
         <v>263407</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.7463469080168711E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>17.463469080168711</v>
       </c>
     </row>
@@ -30292,11 +30294,11 @@
         <v>354425</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.7210975523735628E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>17.210975523735627</v>
       </c>
     </row>
@@ -30314,11 +30316,11 @@
         <v>695797</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.5378048482531543E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>15.378048482531543</v>
       </c>
     </row>
@@ -30336,11 +30338,11 @@
         <v>206268</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.5028991409234587E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>15.028991409234587</v>
       </c>
     </row>
@@ -30358,11 +30360,11 @@
         <v>583702</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.4733545542074553E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>14.733545542074552</v>
       </c>
     </row>
@@ -30380,11 +30382,11 @@
         <v>75168</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -30402,11 +30404,11 @@
         <v>83826</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.4315367547061772E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>14.315367547061772</v>
       </c>
     </row>
@@ -30424,11 +30426,11 @@
         <v>683365</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.3170121384618762E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>13.170121384618762</v>
       </c>
     </row>
@@ -30446,11 +30448,11 @@
         <v>192518</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.2985798730508317E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>12.985798730508316</v>
       </c>
     </row>
@@ -30468,11 +30470,11 @@
         <v>239824</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.2926145840282875E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>12.926145840282874</v>
       </c>
     </row>
@@ -30490,11 +30492,11 @@
         <v>125851</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>1.1124265997091799E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>11.124265997091799</v>
       </c>
     </row>
@@ -30512,11 +30514,11 @@
         <v>116446</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -30534,11 +30536,11 @@
         <v>148350</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>1.0111223458038422E-2</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>10.111223458038422</v>
       </c>
     </row>
@@ -30556,11 +30558,11 @@
         <v>218775</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>1.0055993600731346E-2</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>10.055993600731346</v>
       </c>
     </row>
@@ -30578,11 +30580,11 @@
         <v>91850</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>9.7985846488840497E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>9.7985846488840505</v>
       </c>
     </row>
@@ -30600,11 +30602,11 @@
         <v>434170</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>9.2129810903563113E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>9.2129810903563119</v>
       </c>
     </row>
@@ -30622,11 +30624,11 @@
         <v>54709</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -30644,11 +30646,11 @@
         <v>190006</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>8.9470858814984788E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>8.9470858814984791</v>
       </c>
     </row>
@@ -30666,11 +30668,11 @@
         <v>127998</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>8.5938842794418668E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>8.5938842794418662</v>
       </c>
     </row>
@@ -30688,11 +30690,11 @@
         <v>196435</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>8.1451879756662508E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>8.14518797566625</v>
       </c>
     </row>
@@ -30710,11 +30712,11 @@
         <v>75167</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>7.9822262428991438E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>7.9822262428991442</v>
       </c>
     </row>
@@ -30732,11 +30734,11 @@
         <v>80055</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>7.494847292486416E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>7.4948472924864156</v>
       </c>
     </row>
@@ -30754,11 +30756,11 @@
         <v>180822</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -30776,11 +30778,11 @@
         <v>84247</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>7.1219153204268399E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1219153204268402</v>
       </c>
     </row>
@@ -30798,11 +30800,11 @@
         <v>577212</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>6.5833697151133378E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>6.5833697151133377</v>
       </c>
     </row>
@@ -30820,11 +30822,11 @@
         <v>112055</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>6.246932310026326E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>6.2469323100263257</v>
       </c>
     </row>
@@ -30842,11 +30844,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>4.6537292992148496E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>4.6537292992148496</v>
       </c>
     </row>
@@ -30864,11 +30866,11 @@
         <v>32394</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -30886,11 +30888,11 @@
         <v>133573</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -30908,11 +30910,11 @@
         <v>57443</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>1.7408561530560731E-3</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7408561530560731</v>
       </c>
     </row>
@@ -30930,11 +30932,11 @@
         <v>71544</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -30952,11 +30954,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -30974,11 +30976,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -30996,11 +30998,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31018,11 +31020,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31040,11 +31042,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31062,11 +31064,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31084,11 +31086,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31106,11 +31108,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31128,11 +31130,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31150,11 +31152,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31172,11 +31174,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31194,11 +31196,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -31234,6 +31236,1450 @@
   <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
     <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E20F37F-6586-4963-BCE1-1E5278A5D429}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>264</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>0.10163305846210703</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>101.63305846210703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>299</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>8.5504792843906566E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>85.504792843906571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>152</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>6.4774291424650882E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>64.774291424650883</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>87</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>5.1849291393017631E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>51.84929139301763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>152</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>4.4406011171617549E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>44.40601117161755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>377</v>
+      </c>
+      <c r="D7">
+        <v>939099</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>4.0144862256269044E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>40.144862256269043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>115</v>
+      </c>
+      <c r="D8">
+        <v>287695</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>3.9972887954257109E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>39.972887954257111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>161</v>
+      </c>
+      <c r="D9">
+        <v>411792</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>3.9097408400357463E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>39.097408400357466</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>116</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>3.8514534256354066E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>38.514534256354068</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>3.6423790806028138E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>36.423790806028137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>93</v>
+      </c>
+      <c r="D12">
+        <v>270227</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>3.4415509923138694E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>34.415509923138693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>3.1542123071629291E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>31.542123071629291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>182</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>3.1086135924983348E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>31.086135924983349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.5441408436371039E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>25.441408436371038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>162</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.1813716249333471E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>21.813716249333471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>95</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>2.0880359933446599E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>20.880359933446599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>104</v>
+      </c>
+      <c r="D18">
+        <v>519212</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>2.0030353689822269E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>20.03035368982227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>142</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.9200216340465807E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>19.200216340465808</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <v>354425</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.9186005501869226E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>19.186005501869225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>147790</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.8945801475065971E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>18.94580147506597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>49</v>
+      </c>
+      <c r="D22">
+        <v>263407</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.8602390976701456E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>18.602390976701457</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>111</v>
+      </c>
+      <c r="D23">
+        <v>695797</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.5952928799635526E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>15.952928799635526</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>31</v>
+      </c>
+      <c r="D24">
+        <v>206268</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.5028991409234587E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>15.028991409234587</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>86</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.4733545542074553E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>14.733545542074552</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>75168</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>83826</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.4315367547061772E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>14.315367547061772</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>95</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.390179479487536E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>13.901794794875361</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <v>192518</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.2985798730508317E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>12.985798730508316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>31</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.2926145840282875E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>12.926145840282874</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>125851</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>116446</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>1.0111223458038422E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>10.111223458038422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>218775</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>1.0055993600731346E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>10.055993600731346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>91850</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>9.4733850509983904E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>9.4733850509983899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>41</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>9.4433056176152202E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>9.4433056176152199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>54709</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>80055</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>8.743988507900818E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>8.7439885079008182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>127998</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>47</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>84247</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>39</v>
+      </c>
+      <c r="D45">
+        <v>577212</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>6.7566162865636886E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>6.7566162865636885</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>6.246932310026326E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>6.2469323100263257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>4.6537292992148496E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>4.6537292992148496</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>39</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52">
+        <v>487</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53">
+        <v>120</v>
+      </c>
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>17140</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>1990</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>4863</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>7244</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>344</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2594</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>1870</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>2270</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>337</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>7096</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>176</v>
+      </c>
+      <c r="E64">
+        <f>100*C64/D64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>3055</v>
+      </c>
+      <c r="E65">
+        <f>100*C65/D65</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E65">
+      <sortCondition descending="1" ref="C1"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
+    <sortCondition descending="1" ref="F2:F66"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revised: data 2020/04/29 and 2020/04/30 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AC0ECC-A381-408A-B5BB-D05B7E8EF334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC11CCF-CD97-4B7B-9A00-05F629E68178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="984" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="22" activeTab="28" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="16920" yWindow="1800" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="23" activeTab="29" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,8 @@
     <sheet name="2020年4月25日" sheetId="26" r:id="rId26"/>
     <sheet name="2020年4月26日" sheetId="27" r:id="rId27"/>
     <sheet name="2020年4月27日" sheetId="28" r:id="rId28"/>
-    <sheet name="2020年4月28日" sheetId="29" r:id="rId29"/>
+    <sheet name="2020年4月28日" sheetId="31" r:id="rId29"/>
+    <sheet name="2020年4月29日" sheetId="32" r:id="rId30"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -65,6 +66,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">'2020年4月26日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">'2020年4月27日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">'2020年4月28日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="29" hidden="1">'2020年4月29日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
@@ -90,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -30558,11 +30560,11 @@
         <v>218775</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.0055993600731346E-2</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>10.055993600731346</v>
       </c>
     </row>
@@ -31244,11 +31246,11 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E20F37F-6586-4963-BCE1-1E5278A5D429}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296B17B6-6827-4A4D-8468-49915CF5BC59}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -31282,222 +31284,222 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>264</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>259758</v>
+        <v>65891</v>
       </c>
       <c r="E2">
         <f>100*C2/D2</f>
-        <v>0.10163305846210703</v>
+        <v>3.6423790806028138E-2</v>
       </c>
       <c r="F2" s="1">
         <f>E2*1000</f>
-        <v>101.63305846210703</v>
+        <v>36.423790806028137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>299</v>
+        <v>87</v>
       </c>
       <c r="D3">
-        <v>349688</v>
+        <v>167794</v>
       </c>
       <c r="E3">
         <f>100*C3/D3</f>
-        <v>8.5504792843906566E-2</v>
+        <v>5.1849291393017631E-2</v>
       </c>
       <c r="F3" s="1">
         <f>E3*1000</f>
-        <v>85.504792843906571</v>
+        <v>51.84929139301763</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>152</v>
+        <v>264</v>
       </c>
       <c r="D4">
-        <v>234661</v>
+        <v>259758</v>
       </c>
       <c r="E4">
         <f>100*C4/D4</f>
-        <v>6.4774291424650882E-2</v>
+        <v>0.10163305846210703</v>
       </c>
       <c r="F4" s="1">
         <f>E4*1000</f>
-        <v>64.774291424650883</v>
+        <v>101.63305846210703</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>87</v>
+        <v>299</v>
       </c>
       <c r="D5">
-        <v>167794</v>
+        <v>349688</v>
       </c>
       <c r="E5">
         <f>100*C5/D5</f>
-        <v>5.1849291393017631E-2</v>
+        <v>8.5504792843906566E-2</v>
       </c>
       <c r="F5" s="1">
         <f>E5*1000</f>
-        <v>51.84929139301763</v>
+        <v>85.504792843906571</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="D6">
-        <v>342296</v>
+        <v>235836</v>
       </c>
       <c r="E6">
         <f>100*C6/D6</f>
-        <v>4.4406011171617549E-2</v>
+        <v>2.5441408436371039E-2</v>
       </c>
       <c r="F6" s="1">
         <f>E6*1000</f>
-        <v>44.40601117161755</v>
+        <v>25.441408436371038</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>377</v>
+        <v>66</v>
       </c>
       <c r="D7">
-        <v>939099</v>
+        <v>209244</v>
       </c>
       <c r="E7">
         <f>100*C7/D7</f>
-        <v>4.0144862256269044E-2</v>
+        <v>3.1542123071629291E-2</v>
       </c>
       <c r="F7" s="1">
         <f>E7*1000</f>
-        <v>40.144862256269043</v>
+        <v>31.542123071629291</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D8">
-        <v>287695</v>
+        <v>270227</v>
       </c>
       <c r="E8">
         <f>100*C8/D8</f>
-        <v>3.9972887954257109E-2</v>
+        <v>3.4415509923138694E-2</v>
       </c>
       <c r="F8" s="1">
         <f>E8*1000</f>
-        <v>39.972887954257111</v>
+        <v>34.415509923138693</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="D9">
-        <v>411792</v>
+        <v>519212</v>
       </c>
       <c r="E9">
         <f>100*C9/D9</f>
-        <v>3.9097408400357463E-2</v>
+        <v>2.0030353689822269E-2</v>
       </c>
       <c r="F9" s="1">
         <f>E9*1000</f>
-        <v>39.097408400357466</v>
+        <v>20.03035368982227</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="D10">
-        <v>301185</v>
+        <v>411792</v>
       </c>
       <c r="E10">
         <f>100*C10/D10</f>
-        <v>3.8514534256354066E-2</v>
+        <v>3.9097408400357463E-2</v>
       </c>
       <c r="F10" s="1">
         <f>E10*1000</f>
-        <v>38.514534256354068</v>
+        <v>39.097408400357466</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="D11">
-        <v>65891</v>
+        <v>287695</v>
       </c>
       <c r="E11">
         <f>100*C11/D11</f>
-        <v>3.6423790806028138E-2</v>
+        <v>3.9972887954257109E-2</v>
       </c>
       <c r="F11" s="1">
         <f>E11*1000</f>
-        <v>36.423790806028137</v>
+        <v>39.972887954257111</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -31505,532 +31507,532 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="D12">
-        <v>270227</v>
+        <v>739575</v>
       </c>
       <c r="E12">
         <f>100*C12/D12</f>
-        <v>3.4415509923138694E-2</v>
+        <v>1.9200216340465807E-2</v>
       </c>
       <c r="F12" s="1">
         <f>E12*1000</f>
-        <v>34.415509923138693</v>
+        <v>19.200216340465808</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>66</v>
+        <v>377</v>
       </c>
       <c r="D13">
-        <v>209244</v>
+        <v>939099</v>
       </c>
       <c r="E13">
         <f>100*C13/D13</f>
-        <v>3.1542123071629291E-2</v>
+        <v>4.0144862256269044E-2</v>
       </c>
       <c r="F13" s="1">
         <f>E13*1000</f>
-        <v>31.542123071629291</v>
+        <v>40.144862256269043</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D14">
-        <v>585470</v>
+        <v>234661</v>
       </c>
       <c r="E14">
         <f>100*C14/D14</f>
-        <v>3.1086135924983348E-2</v>
+        <v>6.4774291424650882E-2</v>
       </c>
       <c r="F14" s="1">
         <f>E14*1000</f>
-        <v>31.086135924983349</v>
+        <v>64.774291424650883</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="D15">
-        <v>235836</v>
+        <v>342296</v>
       </c>
       <c r="E15">
         <f>100*C15/D15</f>
-        <v>2.5441408436371039E-2</v>
+        <v>4.4406011171617549E-2</v>
       </c>
       <c r="F15" s="1">
         <f>E15*1000</f>
-        <v>25.441408436371038</v>
+        <v>44.40601117161755</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="D16">
-        <v>742652</v>
+        <v>585470</v>
       </c>
       <c r="E16">
         <f>100*C16/D16</f>
-        <v>2.1813716249333471E-2</v>
+        <v>3.1086135924983348E-2</v>
       </c>
       <c r="F16" s="1">
         <f>E16*1000</f>
-        <v>21.813716249333471</v>
+        <v>31.086135924983349</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="D17">
-        <v>454973</v>
+        <v>301185</v>
       </c>
       <c r="E17">
         <f>100*C17/D17</f>
-        <v>2.0880359933446599E-2</v>
+        <v>3.8514534256354066E-2</v>
       </c>
       <c r="F17" s="1">
         <f>E17*1000</f>
-        <v>20.880359933446599</v>
+        <v>38.514534256354068</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="D18">
-        <v>519212</v>
+        <v>354425</v>
       </c>
       <c r="E18">
         <f>100*C18/D18</f>
-        <v>2.0030353689822269E-2</v>
+        <v>1.9186005501869226E-2</v>
       </c>
       <c r="F18" s="1">
         <f>E18*1000</f>
-        <v>20.03035368982227</v>
+        <v>19.186005501869225</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="D19">
-        <v>739575</v>
+        <v>218775</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>1.9200216340465807E-2</v>
+        <v>1.0055993600731346E-2</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>19.200216340465808</v>
+        <v>10.055993600731346</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="D20">
-        <v>354425</v>
+        <v>583702</v>
       </c>
       <c r="E20">
         <f>100*C20/D20</f>
-        <v>1.9186005501869226E-2</v>
+        <v>1.4733545542074553E-2</v>
       </c>
       <c r="F20" s="1">
         <f>E20*1000</f>
-        <v>19.186005501869225</v>
+        <v>14.733545542074552</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C21">
-        <v>28</v>
+        <v>162</v>
       </c>
       <c r="D21">
-        <v>147790</v>
+        <v>742652</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>1.8945801475065971E-2</v>
+        <v>2.1813716249333471E-2</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>18.94580147506597</v>
+        <v>21.813716249333471</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D22">
-        <v>263407</v>
+        <v>683365</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>1.8602390976701456E-2</v>
+        <v>1.390179479487536E-2</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>18.602390976701457</v>
+        <v>13.901794794875361</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="D23">
-        <v>695797</v>
+        <v>454973</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>1.5952928799635526E-2</v>
+        <v>2.0880359933446599E-2</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>15.952928799635526</v>
+        <v>20.880359933446599</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="D24">
-        <v>206268</v>
+        <v>695797</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>1.5028991409234587E-2</v>
+        <v>1.5952928799635526E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>15.028991409234587</v>
+        <v>15.952928799635526</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C25">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="D25">
-        <v>583702</v>
+        <v>577212</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>1.4733545542074553E-2</v>
+        <v>6.7566162865636886E-3</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>14.733545542074552</v>
+        <v>6.7566162865636885</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D26">
-        <v>75168</v>
+        <v>180822</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>1.4633886760323542E-2</v>
+        <v>7.1893906714890887E-3</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>14.633886760323543</v>
+        <v>7.1893906714890887</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C27">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D27">
-        <v>83826</v>
+        <v>148350</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>1.4315367547061772E-2</v>
+        <v>1.0111223458038422E-2</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>14.315367547061772</v>
+        <v>10.111223458038422</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C28">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="D28">
-        <v>683365</v>
+        <v>192518</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>1.390179479487536E-2</v>
+        <v>1.2985798730508317E-2</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>13.901794794875361</v>
+        <v>12.985798730508316</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <v>192518</v>
+        <v>133573</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>1.2985798730508317E-2</v>
+        <v>2.2459628817201082E-3</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>12.985798730508316</v>
+        <v>2.2459628817201081</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
       <c r="C30">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D30">
-        <v>239824</v>
+        <v>263407</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>1.2926145840282875E-2</v>
+        <v>1.8602390976701456E-2</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>12.926145840282874</v>
+        <v>18.602390976701457</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C31">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D31">
-        <v>125851</v>
+        <v>112055</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>1.1124265997091799E-2</v>
+        <v>6.246932310026326E-3</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>11.124265997091799</v>
+        <v>6.2469323100263257</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C32">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D32">
-        <v>116446</v>
+        <v>239824</v>
       </c>
       <c r="E32">
         <f>100*C32/D32</f>
-        <v>1.0305205846486783E-2</v>
+        <v>1.2926145840282875E-2</v>
       </c>
       <c r="F32" s="1">
         <f>E32*1000</f>
-        <v>10.305205846486784</v>
+        <v>12.926145840282874</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C33">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D33">
-        <v>148350</v>
+        <v>434170</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>1.0111223458038422E-2</v>
+        <v>9.4433056176152202E-3</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>10.111223458038422</v>
+        <v>9.4433056176152199</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C34">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D34">
-        <v>218775</v>
+        <v>125851</v>
       </c>
       <c r="E34">
         <f>100*C34/D34</f>
-        <v>1.0055993600731346E-2</v>
+        <v>1.1124265997091799E-2</v>
       </c>
       <c r="F34" s="1">
         <f>E34*1000</f>
-        <v>10.055993600731346</v>
+        <v>11.124265997091799</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D35">
-        <v>91850</v>
+        <v>196435</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>9.7985846488840497E-3</v>
+        <v>8.1451879756662508E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>9.7985846488840505</v>
+        <v>8.14518797566625</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
@@ -32052,346 +32054,350 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C37">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D37">
-        <v>434170</v>
+        <v>150417</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>9.4433056176152202E-3</v>
+        <v>4.6537292992148496E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>9.4433056176152199</v>
+        <v>4.6537292992148496</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>54709</v>
+        <v>127998</v>
       </c>
       <c r="E38">
         <f>100*C38/D38</f>
-        <v>9.1392641064541487E-3</v>
+        <v>8.5938842794418668E-3</v>
       </c>
       <c r="F38" s="1">
         <f>E38*1000</f>
-        <v>9.1392641064541493</v>
+        <v>8.5938842794418662</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39">
-        <v>80055</v>
+        <v>75167</v>
       </c>
       <c r="E39">
         <f>100*C39/D39</f>
-        <v>8.743988507900818E-3</v>
+        <v>7.9822262428991438E-3</v>
       </c>
       <c r="F39" s="1">
         <f>E39*1000</f>
-        <v>8.7439885079008182</v>
+        <v>7.9822262428991442</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C40">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>127998</v>
+        <v>57443</v>
       </c>
       <c r="E40">
         <f>100*C40/D40</f>
-        <v>8.5938842794418668E-3</v>
+        <v>1.7408561530560731E-3</v>
       </c>
       <c r="F40" s="1">
         <f>E40*1000</f>
-        <v>8.5938842794418662</v>
+        <v>1.7408561530560731</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C41">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D41">
-        <v>196435</v>
+        <v>83826</v>
       </c>
       <c r="E41">
         <f>100*C41/D41</f>
-        <v>8.1451879756662508E-3</v>
+        <v>1.4315367547061772E-2</v>
       </c>
       <c r="F41" s="1">
         <f>E41*1000</f>
-        <v>8.14518797566625</v>
+        <v>14.315367547061772</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C42">
         <v>6</v>
       </c>
       <c r="D42">
-        <v>75167</v>
+        <v>84247</v>
       </c>
       <c r="E42">
         <f>100*C42/D42</f>
-        <v>7.9822262428991438E-3</v>
+        <v>7.1219153204268399E-3</v>
       </c>
       <c r="F42" s="1">
         <f>E42*1000</f>
-        <v>7.9822262428991442</v>
+        <v>7.1219153204268402</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C43">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D43">
-        <v>180822</v>
+        <v>75168</v>
       </c>
       <c r="E43">
         <f>100*C43/D43</f>
-        <v>7.1893906714890887E-3</v>
+        <v>1.4633886760323542E-2</v>
       </c>
       <c r="F43" s="1">
         <f>E43*1000</f>
-        <v>7.1893906714890887</v>
+        <v>14.633886760323543</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D44">
-        <v>84247</v>
+        <v>116446</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>7.1219153204268399E-3</v>
+        <v>1.0305205846486783E-2</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>7.1219153204268402</v>
+        <v>10.305205846486784</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C45">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>577212</v>
+        <v>71544</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>6.7566162865636886E-3</v>
+        <v>1.3977412501397742E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>6.7566162865636885</v>
+        <v>1.3977412501397741</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D46">
-        <v>112055</v>
+        <v>147790</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>6.246932310026326E-3</v>
+        <v>1.8945801475065971E-2</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>6.2469323100263257</v>
+        <v>18.94580147506597</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D47">
-        <v>150417</v>
+        <v>91850</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>4.6537292992148496E-3</v>
+        <v>9.7985846488840497E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>4.6537292992148496</v>
+        <v>9.7985846488840505</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D48">
-        <v>32394</v>
+        <v>54709</v>
       </c>
       <c r="E48">
         <f>100*C48/D48</f>
-        <v>3.0869914181638576E-3</v>
+        <v>9.1392641064541487E-3</v>
       </c>
       <c r="F48" s="1">
         <f>E48*1000</f>
-        <v>3.0869914181638576</v>
+        <v>9.1392641064541493</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>133573</v>
+        <v>80055</v>
       </c>
       <c r="E49">
         <f>100*C49/D49</f>
-        <v>2.2459628817201082E-3</v>
+        <v>8.743988507900818E-3</v>
       </c>
       <c r="F49" s="1">
         <f>E49*1000</f>
-        <v>2.2459628817201081</v>
+        <v>8.7439885079008182</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D50">
-        <v>57443</v>
+        <v>206268</v>
       </c>
       <c r="E50">
         <f>100*C50/D50</f>
-        <v>1.7408561530560731E-3</v>
+        <v>1.5028991409234587E-2</v>
       </c>
       <c r="F50" s="1">
         <f>E50*1000</f>
-        <v>1.7408561530560731</v>
+        <v>15.028991409234587</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>71544</v>
+        <v>32394</v>
       </c>
       <c r="E51">
         <f>100*C51/D51</f>
-        <v>1.3977412501397742E-3</v>
+        <v>3.0869914181638576E-3</v>
       </c>
       <c r="F51" s="1">
         <f>E51*1000</f>
-        <v>1.3977412501397741</v>
+        <v>3.0869914181638576</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C52">
-        <v>487</v>
-      </c>
-      <c r="D52" t="s">
-        <v>69</v>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
       </c>
       <c r="F52" s="1">
         <f>E52*1000</f>
@@ -32400,16 +32406,20 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C53">
-        <v>120</v>
-      </c>
-      <c r="D53" t="s">
-        <v>69</v>
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
       </c>
       <c r="F53" s="1">
         <f>E53*1000</f>
@@ -32421,13 +32431,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>17140</v>
+        <v>4863</v>
       </c>
       <c r="E54">
         <f>100*C54/D54</f>
@@ -32443,13 +32453,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>1990</v>
+        <v>7244</v>
       </c>
       <c r="E55">
         <f>100*C55/D55</f>
@@ -32465,13 +32475,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>4863</v>
+        <v>344</v>
       </c>
       <c r="E56">
         <f>100*C56/D56</f>
@@ -32487,13 +32497,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>7244</v>
+        <v>2594</v>
       </c>
       <c r="E57">
         <f>100*C57/D57</f>
@@ -32509,13 +32519,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>344</v>
+        <v>1870</v>
       </c>
       <c r="E58">
         <f>100*C58/D58</f>
@@ -32531,13 +32541,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>2594</v>
+        <v>2270</v>
       </c>
       <c r="E59">
         <f>100*C59/D59</f>
@@ -32553,13 +32563,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>1870</v>
+        <v>337</v>
       </c>
       <c r="E60">
         <f>100*C60/D60</f>
@@ -32575,13 +32585,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>2270</v>
+        <v>7096</v>
       </c>
       <c r="E61">
         <f>100*C61/D61</f>
@@ -32597,13 +32607,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>337</v>
+        <v>176</v>
       </c>
       <c r="E62">
         <f>100*C62/D62</f>
@@ -32619,13 +32629,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>7096</v>
+        <v>3055</v>
       </c>
       <c r="E63">
         <f>100*C63/D63</f>
@@ -32641,45 +32651,33 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>176</v>
-      </c>
-      <c r="E64">
-        <f>100*C64/D64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+        <v>120</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C65">
-        <v>0</v>
-      </c>
-      <c r="D65">
-        <v>3055</v>
-      </c>
-      <c r="E65">
-        <f>100*C65/D65</f>
-        <v>0</v>
+        <v>487</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E65">
-      <sortCondition descending="1" ref="C1"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
-    <sortCondition descending="1" ref="F2:F66"/>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition ref="A2:A65"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34112,6 +34110,1446 @@
       </c>
       <c r="D65" t="s">
         <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7326AB91-0302-4895-A718-77C6505B3ACD}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>266</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>0.10240300587469876</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>102.40300587469876</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>299</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>8.5504792843906566E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>85.504792843906571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>153</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>6.5200438078760428E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>65.200438078760428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>87</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>5.1849291393017631E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>51.84929139301763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>155</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>4.5282445602636313E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>45.282445602636315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>167</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>4.0554454676147184E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>40.554454676147181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>379</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>4.0357832347814232E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>40.357832347814231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>115</v>
+      </c>
+      <c r="D9">
+        <v>287695</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>3.9972887954257109E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>39.972887954257111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>116</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>3.8514534256354066E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>38.514534256354068</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>3.6423790806028138E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>36.423790806028137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>95</v>
+      </c>
+      <c r="D12">
+        <v>270227</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>3.5155628416109419E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>35.155628416109423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>3.1542123071629291E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>31.542123071629291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>183</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>3.1256938869626112E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>31.256938869626111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.5441408436371039E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>25.441408436371038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>162</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.1813716249333471E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>21.813716249333471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>96</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>2.1100153195903932E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>21.100153195903932</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>105</v>
+      </c>
+      <c r="D18">
+        <v>519212</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>2.0222953244532098E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>20.222953244532096</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>146</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>1.9741067504985971E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>19.741067504985971</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <v>354425</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>1.9186005501869226E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>19.186005501869225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>263407</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.8982031608879034E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>18.982031608879034</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>147790</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.8945801475065971E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>18.94580147506597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>113</v>
+      </c>
+      <c r="D23">
+        <v>695797</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.6240368958187517E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>16.240368958187517</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>206268</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.5998603758217465E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>15.998603758217465</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>89</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.5247506433077153E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>15.247506433077152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>75168</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>99</v>
+      </c>
+      <c r="D27">
+        <v>683365</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.4487133523080637E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>14.487133523080637</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>83826</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.4315367547061772E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>14.315367547061772</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>192518</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.3505230679728648E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>13.505230679728648</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.3343118286743613E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>13.343118286743612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>218775</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>1.2341446691806651E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>12.341446691806651</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>125851</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>1.0785305021907651E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>10.785305021907652</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>116446</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>91850</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>9.4733850509983904E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>9.4733850509983899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>41</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>9.4433056176152202E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>9.4433056176152199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>54709</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>80055</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>8.743988507900818E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>8.7439885079008182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>127998</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>84247</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>39</v>
+      </c>
+      <c r="D45">
+        <v>577212</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>6.7566162865636886E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>6.7566162865636885</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>6.246932310026326E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>6.2469323100263257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>4.6537292992148496E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>4.6537292992148496</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>487</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised: data 2020/04/30, 2020/05/01 and 2020/05/02 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC11CCF-CD97-4B7B-9A00-05F629E68178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DB64C-C6EC-40BA-9342-E8C6690A6022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="1800" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="23" activeTab="29" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="2160" yWindow="3156" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="25" activeTab="31" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,8 @@
     <sheet name="2020年4月27日" sheetId="28" r:id="rId28"/>
     <sheet name="2020年4月28日" sheetId="31" r:id="rId29"/>
     <sheet name="2020年4月29日" sheetId="32" r:id="rId30"/>
+    <sheet name="2020年4月30日" sheetId="33" r:id="rId31"/>
+    <sheet name="2020年5月1日" sheetId="34" r:id="rId32"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -68,6 +70,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">'2020年4月28日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="29" hidden="1">'2020年4月29日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020年4月2日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="30" hidden="1">'2020年4月30日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020年4月3日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020年4月4日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2020年4月5日'!$B$1:$E$1</definedName>
@@ -75,6 +78,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'2020年4月7日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2020年4月8日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'2020年4月9日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">'2020年5月1日'!$B$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -31296,11 +31300,11 @@
         <v>65891</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>3.6423790806028138E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>36.423790806028137</v>
       </c>
     </row>
@@ -31318,11 +31322,11 @@
         <v>167794</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>5.1849291393017631E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>51.84929139301763</v>
       </c>
     </row>
@@ -31340,11 +31344,11 @@
         <v>259758</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>0.10163305846210703</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>101.63305846210703</v>
       </c>
     </row>
@@ -31362,11 +31366,11 @@
         <v>349688</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>8.5504792843906566E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>85.504792843906571</v>
       </c>
     </row>
@@ -31384,11 +31388,11 @@
         <v>235836</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.5441408436371039E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>25.441408436371038</v>
       </c>
     </row>
@@ -31406,11 +31410,11 @@
         <v>209244</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>3.1542123071629291E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>31.542123071629291</v>
       </c>
     </row>
@@ -31428,11 +31432,11 @@
         <v>270227</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>3.4415509923138694E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>34.415509923138693</v>
       </c>
     </row>
@@ -31450,11 +31454,11 @@
         <v>519212</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.0030353689822269E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>20.03035368982227</v>
       </c>
     </row>
@@ -31472,11 +31476,11 @@
         <v>411792</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>3.9097408400357463E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>39.097408400357466</v>
       </c>
     </row>
@@ -31494,11 +31498,11 @@
         <v>287695</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>3.9972887954257109E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>39.972887954257111</v>
       </c>
     </row>
@@ -31516,11 +31520,11 @@
         <v>739575</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.9200216340465807E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>19.200216340465808</v>
       </c>
     </row>
@@ -31538,11 +31542,11 @@
         <v>939099</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>4.0144862256269044E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>40.144862256269043</v>
       </c>
     </row>
@@ -31560,11 +31564,11 @@
         <v>234661</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>6.4774291424650882E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>64.774291424650883</v>
       </c>
     </row>
@@ -31582,11 +31586,11 @@
         <v>342296</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>4.4406011171617549E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>44.40601117161755</v>
       </c>
     </row>
@@ -31604,11 +31608,11 @@
         <v>585470</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>3.1086135924983348E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>31.086135924983349</v>
       </c>
     </row>
@@ -31626,11 +31630,11 @@
         <v>301185</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>3.8514534256354066E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>38.514534256354068</v>
       </c>
     </row>
@@ -31648,11 +31652,11 @@
         <v>354425</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.9186005501869226E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>19.186005501869225</v>
       </c>
     </row>
@@ -31670,11 +31674,11 @@
         <v>218775</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.0055993600731346E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>10.055993600731346</v>
       </c>
     </row>
@@ -31692,11 +31696,11 @@
         <v>583702</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.4733545542074553E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>14.733545542074552</v>
       </c>
     </row>
@@ -31714,11 +31718,11 @@
         <v>742652</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>2.1813716249333471E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>21.813716249333471</v>
       </c>
     </row>
@@ -31736,11 +31740,11 @@
         <v>683365</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.390179479487536E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>13.901794794875361</v>
       </c>
     </row>
@@ -31758,11 +31762,11 @@
         <v>454973</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>2.0880359933446599E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>20.880359933446599</v>
       </c>
     </row>
@@ -31780,11 +31784,11 @@
         <v>695797</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.5952928799635526E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>15.952928799635526</v>
       </c>
     </row>
@@ -31802,11 +31806,11 @@
         <v>577212</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>6.7566162865636886E-3</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>6.7566162865636885</v>
       </c>
     </row>
@@ -31824,11 +31828,11 @@
         <v>180822</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -31846,11 +31850,11 @@
         <v>148350</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.0111223458038422E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>10.111223458038422</v>
       </c>
     </row>
@@ -31868,11 +31872,11 @@
         <v>192518</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.2985798730508317E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>12.985798730508316</v>
       </c>
     </row>
@@ -31890,11 +31894,11 @@
         <v>133573</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -31912,11 +31916,11 @@
         <v>263407</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.8602390976701456E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>18.602390976701457</v>
       </c>
     </row>
@@ -31934,11 +31938,11 @@
         <v>112055</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>6.246932310026326E-3</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>6.2469323100263257</v>
       </c>
     </row>
@@ -31956,11 +31960,11 @@
         <v>239824</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>1.2926145840282875E-2</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>12.926145840282874</v>
       </c>
     </row>
@@ -31978,11 +31982,11 @@
         <v>434170</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>9.4433056176152202E-3</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>9.4433056176152199</v>
       </c>
     </row>
@@ -32000,11 +32004,11 @@
         <v>125851</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>1.1124265997091799E-2</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>11.124265997091799</v>
       </c>
     </row>
@@ -32022,11 +32026,11 @@
         <v>196435</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>8.1451879756662508E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>8.14518797566625</v>
       </c>
     </row>
@@ -32044,11 +32048,11 @@
         <v>190006</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>9.4733850509983904E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>9.4733850509983899</v>
       </c>
     </row>
@@ -32066,11 +32070,11 @@
         <v>150417</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>4.6537292992148496E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>4.6537292992148496</v>
       </c>
     </row>
@@ -32088,11 +32092,11 @@
         <v>127998</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>8.5938842794418668E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>8.5938842794418662</v>
       </c>
     </row>
@@ -32110,11 +32114,11 @@
         <v>75167</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>7.9822262428991438E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>7.9822262428991442</v>
       </c>
     </row>
@@ -32132,11 +32136,11 @@
         <v>57443</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>1.7408561530560731E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7408561530560731</v>
       </c>
     </row>
@@ -32154,11 +32158,11 @@
         <v>83826</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>1.4315367547061772E-2</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>14.315367547061772</v>
       </c>
     </row>
@@ -32176,11 +32180,11 @@
         <v>84247</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>7.1219153204268399E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1219153204268402</v>
       </c>
     </row>
@@ -32198,11 +32202,11 @@
         <v>75168</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -32220,11 +32224,11 @@
         <v>116446</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -32242,11 +32246,11 @@
         <v>71544</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -32264,11 +32268,11 @@
         <v>147790</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>1.8945801475065971E-2</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>18.94580147506597</v>
       </c>
     </row>
@@ -32286,11 +32290,11 @@
         <v>91850</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>9.7985846488840497E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>9.7985846488840505</v>
       </c>
     </row>
@@ -32308,11 +32312,11 @@
         <v>54709</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -32330,11 +32334,11 @@
         <v>80055</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>8.743988507900818E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>8.7439885079008182</v>
       </c>
     </row>
@@ -32352,11 +32356,11 @@
         <v>206268</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>1.5028991409234587E-2</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>15.028991409234587</v>
       </c>
     </row>
@@ -32374,11 +32378,11 @@
         <v>32394</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -32396,11 +32400,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32418,11 +32422,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32440,11 +32444,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32462,11 +32466,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32484,11 +32488,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32506,11 +32510,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32528,11 +32532,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32550,11 +32554,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32572,11 +32576,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32594,11 +32598,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32616,11 +32620,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -32638,11 +32642,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -34127,7 +34131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7326AB91-0302-4895-A718-77C6505B3ACD}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -34174,11 +34178,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>0.10240300587469876</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>102.40300587469876</v>
       </c>
     </row>
@@ -34196,11 +34200,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>8.5504792843906566E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>85.504792843906571</v>
       </c>
     </row>
@@ -34218,6 +34222,1446 @@
         <v>234661</v>
       </c>
       <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6.5200438078760428E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>65.200438078760428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>87</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.1849291393017631E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>51.84929139301763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>155</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4.5282445602636313E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>45.282445602636315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>167</v>
+      </c>
+      <c r="D7">
+        <v>411792</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4.0554454676147184E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>40.554454676147181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>379</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4.0357832347814232E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>40.357832347814231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>115</v>
+      </c>
+      <c r="D9">
+        <v>287695</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3.9972887954257109E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>39.972887954257111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>116</v>
+      </c>
+      <c r="D10">
+        <v>301185</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3.8514534256354066E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>38.514534256354068</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3.6423790806028138E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>36.423790806028137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>95</v>
+      </c>
+      <c r="D12">
+        <v>270227</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3.5155628416109419E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>35.155628416109423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3.1542123071629291E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>31.542123071629291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>183</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3.1256938869626112E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>31.256938869626111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2.5441408436371039E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>25.441408436371038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>162</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2.1813716249333471E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>21.813716249333471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>96</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2.1100153195903932E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>21.100153195903932</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>105</v>
+      </c>
+      <c r="D18">
+        <v>519212</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2.0222953244532098E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>20.222953244532096</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>146</v>
+      </c>
+      <c r="D19">
+        <v>739575</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.9741067504985971E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>19.741067504985971</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <v>354425</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1.9186005501869226E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>19.186005501869225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>263407</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.8982031608879034E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>18.982031608879034</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>147790</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.8945801475065971E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>18.94580147506597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>113</v>
+      </c>
+      <c r="D23">
+        <v>695797</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.6240368958187517E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>16.240368958187517</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>206268</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.5998603758217465E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>15.998603758217465</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>89</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.5247506433077153E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>15.247506433077152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>75168</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>99</v>
+      </c>
+      <c r="D27">
+        <v>683365</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.4487133523080637E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>14.487133523080637</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>83826</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.4315367547061772E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>14.315367547061772</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>192518</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.3505230679728648E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>13.505230679728648</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.3343118286743613E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>13.343118286743612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>218775</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.2341446691806651E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>12.341446691806651</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>125851</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.0785305021907651E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>10.785305021907652</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>116446</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>91850</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>9.4733850509983904E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>9.4733850509983899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>41</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>9.4433056176152202E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>9.4433056176152199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>54709</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>80055</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>8.743988507900818E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>8.7439885079008182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>127998</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>84247</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>39</v>
+      </c>
+      <c r="D45">
+        <v>577212</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>6.7566162865636886E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>6.7566162865636885</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>6.246932310026326E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>6.2469323100263257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>4.6537292992148496E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6537292992148496</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>487</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2C5E09-4D4C-4D97-8CD3-E9C70574AA10}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>268</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>0.10317295328729048</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>103.17295328729048</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>304</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>8.6934638878085613E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>86.934638878085607</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>153</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
         <f>100*C4/D4</f>
         <v>6.5200438078760428E-2</v>
       </c>
@@ -34272,24 +35716,24 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
       <c r="C7">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="D7">
-        <v>411792</v>
+        <v>287695</v>
       </c>
       <c r="E7">
         <f>100*C7/D7</f>
-        <v>4.0554454676147184E-2</v>
+        <v>4.2058429934479225E-2</v>
       </c>
       <c r="F7" s="1">
         <f>E7*1000</f>
-        <v>40.554454676147181</v>
+        <v>42.058429934479221</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -34300,40 +35744,40 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="D8">
         <v>939099</v>
       </c>
       <c r="E8">
         <f>100*C8/D8</f>
-        <v>4.0357832347814232E-2</v>
+        <v>4.0890257576677219E-2</v>
       </c>
       <c r="F8" s="1">
         <f>E8*1000</f>
-        <v>40.357832347814231</v>
+        <v>40.890257576677222</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="D9">
-        <v>287695</v>
+        <v>411792</v>
       </c>
       <c r="E9">
         <f>100*C9/D9</f>
-        <v>3.9972887954257109E-2</v>
+        <v>4.0554454676147184E-2</v>
       </c>
       <c r="F9" s="1">
         <f>E9*1000</f>
-        <v>39.972887954257111</v>
+        <v>40.554454676147181</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -34476,18 +35920,18 @@
         <v>19</v>
       </c>
       <c r="C16">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D16">
         <v>742652</v>
       </c>
       <c r="E16">
         <f>100*C16/D16</f>
-        <v>2.1813716249333471E-2</v>
+        <v>2.2621631665975452E-2</v>
       </c>
       <c r="F16" s="1">
         <f>E16*1000</f>
-        <v>21.813716249333471</v>
+        <v>22.621631665975453</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -34498,18 +35942,1458 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D17">
         <v>454973</v>
       </c>
       <c r="E17">
         <f>100*C17/D17</f>
-        <v>2.1100153195903932E-2</v>
+        <v>2.1319946458361265E-2</v>
       </c>
       <c r="F17" s="1">
         <f>E17*1000</f>
-        <v>21.100153195903932</v>
+        <v>21.319946458361265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>54</v>
+      </c>
+      <c r="D18">
+        <v>263407</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>2.0500594137589357E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>20.500594137589356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>106</v>
+      </c>
+      <c r="D19">
+        <v>519212</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>2.041555279924193E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>20.415552799241929</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>148</v>
+      </c>
+      <c r="D20">
+        <v>739575</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>2.0011493087246052E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>20.011493087246052</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>68</v>
+      </c>
+      <c r="D21">
+        <v>354425</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>1.9186005501869226E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>19.186005501869225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>147790</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>1.8945801475065971E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>18.94580147506597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>34</v>
+      </c>
+      <c r="D23">
+        <v>206268</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>1.6483409932708904E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>16.483409932708906</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>113</v>
+      </c>
+      <c r="D24">
+        <v>695797</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.6240368958187517E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>16.240368958187517</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>91</v>
+      </c>
+      <c r="D25">
+        <v>583702</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.5590147027078886E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>15.590147027078887</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>104</v>
+      </c>
+      <c r="D26">
+        <v>683365</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.5218806933337235E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>15.218806933337236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>75168</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>83826</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.4315367547061772E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>14.315367547061772</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>192518</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.3505230679728648E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>13.505230679728648</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.3343118286743613E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>13.343118286743612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>218775</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>1.3255627928236773E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>13.255627928236773</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>125851</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>1.0785305021907651E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>10.785305021907652</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>116446</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>91850</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>18</v>
+      </c>
+      <c r="D36">
+        <v>190006</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>9.4733850509983904E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>9.4733850509983899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <v>41</v>
+      </c>
+      <c r="D37">
+        <v>434170</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>9.4433056176152202E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>9.4433056176152199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>54709</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>80055</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>8.743988507900818E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>8.7439885079008182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>127998</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>84247</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45">
+        <v>39</v>
+      </c>
+      <c r="D45">
+        <v>577212</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>6.7566162865636886E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>6.7566162865636885</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>112055</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>6.246932310026326E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>6.2469323100263257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>4.6537292992148496E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>4.6537292992148496</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>128</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>487</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB369B25-4702-4754-B080-393D1CF32ACD}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>270</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>0.1039429006998822</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>103.9429006998822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>311</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>8.8936423325936265E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>88.936423325936261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>154</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>6.5626584732869975E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>65.626584732869972</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>88</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>5.244526025960404E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>52.445260259604041</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>158</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>4.6158880033655085E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>46.158880033655088</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>123</v>
+      </c>
+      <c r="D7">
+        <v>287695</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>4.2753610594553258E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>42.753610594553258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>393</v>
+      </c>
+      <c r="D8">
+        <v>939099</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>4.1848622988630589E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>41.848622988630588</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>113</v>
+      </c>
+      <c r="D9">
+        <v>270227</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>4.1816694852845941E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>41.816694852845941</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>169</v>
+      </c>
+      <c r="D10">
+        <v>411792</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>4.1040136768077086E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>41.040136768077083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>65891</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>4.0976764656781656E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>40.976764656781654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>123</v>
+      </c>
+      <c r="D12">
+        <v>301185</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>4.0838687185616812E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>40.838687185616813</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>74</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>3.5365410716675268E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>35.365410716675271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>192</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>3.2794165371411006E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>32.794165371411005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.5865431910310554E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>25.865431910310555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>172</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.3160241943736771E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>23.160241943736771</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>2.1979326245733264E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>21.979326245733265</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -34520,40 +37404,40 @@
         <v>7</v>
       </c>
       <c r="C18">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D18">
         <v>519212</v>
       </c>
       <c r="E18">
         <f>100*C18/D18</f>
-        <v>2.0222953244532098E-2</v>
+        <v>2.1763749682210735E-2</v>
       </c>
       <c r="F18" s="1">
         <f>E18*1000</f>
-        <v>20.222953244532096</v>
+        <v>21.763749682210733</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C19">
-        <v>146</v>
+        <v>55</v>
       </c>
       <c r="D19">
-        <v>739575</v>
+        <v>263407</v>
       </c>
       <c r="E19">
         <f>100*C19/D19</f>
-        <v>1.9741067504985971E-2</v>
+        <v>2.0880234769766939E-2</v>
       </c>
       <c r="F19" s="1">
         <f>E19*1000</f>
-        <v>19.741067504985971</v>
+        <v>20.88023476976694</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -34564,40 +37448,40 @@
         <v>16</v>
       </c>
       <c r="C20">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D20">
         <v>354425</v>
       </c>
       <c r="E20">
         <f>100*C20/D20</f>
-        <v>1.9186005501869226E-2</v>
+        <v>2.087888834026945E-2</v>
       </c>
       <c r="F20" s="1">
         <f>E20*1000</f>
-        <v>19.186005501869225</v>
+        <v>20.878888340269448</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D21">
-        <v>263407</v>
+        <v>739575</v>
       </c>
       <c r="E21">
         <f>100*C21/D21</f>
-        <v>1.8982031608879034E-2</v>
+        <v>2.0687557042896258E-2</v>
       </c>
       <c r="F21" s="1">
         <f>E21*1000</f>
-        <v>18.982031608879034</v>
+        <v>20.687557042896259</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -34608,18 +37492,18 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>147790</v>
       </c>
       <c r="E22">
         <f>100*C22/D22</f>
-        <v>1.8945801475065971E-2</v>
+        <v>1.9622437242032612E-2</v>
       </c>
       <c r="F22" s="1">
         <f>E22*1000</f>
-        <v>18.94580147506597</v>
+        <v>19.622437242032611</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -34630,18 +37514,18 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D23">
         <v>695797</v>
       </c>
       <c r="E23">
         <f>100*C23/D23</f>
-        <v>1.6240368958187517E-2</v>
+        <v>1.6671529196015503E-2</v>
       </c>
       <c r="F23" s="1">
         <f>E23*1000</f>
-        <v>16.240368958187517</v>
+        <v>16.671529196015502</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -34652,62 +37536,62 @@
         <v>37</v>
       </c>
       <c r="C24">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D24">
         <v>206268</v>
       </c>
       <c r="E24">
         <f>100*C24/D24</f>
-        <v>1.5998603758217465E-2</v>
+        <v>1.6483409932708904E-2</v>
       </c>
       <c r="F24" s="1">
         <f>E24*1000</f>
-        <v>15.998603758217465</v>
+        <v>16.483409932708906</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="D25">
-        <v>583702</v>
+        <v>218775</v>
       </c>
       <c r="E25">
         <f>100*C25/D25</f>
-        <v>1.5247506433077153E-2</v>
+        <v>1.5998171637527141E-2</v>
       </c>
       <c r="F25" s="1">
         <f>E25*1000</f>
-        <v>15.247506433077152</v>
+        <v>15.998171637527141</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="D26">
-        <v>75168</v>
+        <v>583702</v>
       </c>
       <c r="E26">
         <f>100*C26/D26</f>
-        <v>1.4633886760323542E-2</v>
+        <v>1.5761467324079754E-2</v>
       </c>
       <c r="F26" s="1">
         <f>E26*1000</f>
-        <v>14.633886760323543</v>
+        <v>15.761467324079755</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -34718,18 +37602,18 @@
         <v>20</v>
       </c>
       <c r="C27">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D27">
         <v>683365</v>
       </c>
       <c r="E27">
         <f>100*C27/D27</f>
-        <v>1.4487133523080637E-2</v>
+        <v>1.5511476297439875E-2</v>
       </c>
       <c r="F27" s="1">
         <f>E27*1000</f>
-        <v>14.487133523080637</v>
+        <v>15.511476297439874</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -34740,40 +37624,40 @@
         <v>43</v>
       </c>
       <c r="C28">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>83826</v>
       </c>
       <c r="E28">
         <f>100*C28/D28</f>
-        <v>1.4315367547061772E-2</v>
+        <v>1.5508314842650252E-2</v>
       </c>
       <c r="F28" s="1">
         <f>E28*1000</f>
-        <v>14.315367547061772</v>
+        <v>15.508314842650252</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C29">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D29">
-        <v>192518</v>
+        <v>75168</v>
       </c>
       <c r="E29">
         <f>100*C29/D29</f>
-        <v>1.3505230679728648E-2</v>
+        <v>1.4633886760323542E-2</v>
       </c>
       <c r="F29" s="1">
         <f>E29*1000</f>
-        <v>13.505230679728648</v>
+        <v>14.633886760323543</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -34784,40 +37668,40 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D30">
         <v>239824</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>1.3343118286743613E-2</v>
+        <v>1.4177063179665089E-2</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>13.343118286743612</v>
+        <v>14.177063179665089</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C31">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31">
-        <v>218775</v>
+        <v>192518</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>1.2341446691806651E-2</v>
+        <v>1.3505230679728648E-2</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>12.341446691806651</v>
+        <v>13.505230679728648</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -34888,68 +37772,68 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="D35">
-        <v>91850</v>
+        <v>434170</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>9.7985846488840497E-3</v>
+        <v>9.9039546721330363E-3</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>9.7985846488840505</v>
+        <v>9.903954672133036</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
       <c r="C36">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D36">
-        <v>190006</v>
+        <v>91850</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>9.4733850509983904E-3</v>
+        <v>9.7985846488840497E-3</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>9.4733850509983899</v>
+        <v>9.7985846488840505</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
       <c r="C37">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>434170</v>
+        <v>190006</v>
       </c>
       <c r="E37">
         <f>100*C37/D37</f>
-        <v>9.4433056176152202E-3</v>
+        <v>9.4733850509983904E-3</v>
       </c>
       <c r="F37" s="1">
         <f>E37*1000</f>
-        <v>9.4433056176152199</v>
+        <v>9.4733850509983899</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -35086,68 +37970,68 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D44">
-        <v>84247</v>
+        <v>112055</v>
       </c>
       <c r="E44">
         <f>100*C44/D44</f>
-        <v>7.1219153204268399E-3</v>
+        <v>7.1393512114586591E-3</v>
       </c>
       <c r="F44" s="1">
         <f>E44*1000</f>
-        <v>7.1219153204268402</v>
+        <v>7.139351211458659</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C45">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D45">
-        <v>577212</v>
+        <v>84247</v>
       </c>
       <c r="E45">
         <f>100*C45/D45</f>
-        <v>6.7566162865636886E-3</v>
+        <v>7.1219153204268399E-3</v>
       </c>
       <c r="F45" s="1">
         <f>E45*1000</f>
-        <v>6.7566162865636885</v>
+        <v>7.1219153204268402</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D46">
-        <v>112055</v>
+        <v>577212</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>6.246932310026326E-3</v>
+        <v>6.7566162865636886E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>6.2469323100263257</v>
+        <v>6.7566162865636885</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -35158,18 +38042,18 @@
         <v>44</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D47">
         <v>150417</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>4.6537292992148496E-3</v>
+        <v>5.3185477705312567E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>4.6537292992148496</v>
+        <v>5.3185477705312572</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -35532,7 +38416,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -35546,7 +38430,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>487</v>
+        <v>527</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Revised: data 2020/05/03 and 2020/05/04 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DB64C-C6EC-40BA-9342-E8C6690A6022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8763B8-7BC2-4CDE-A2B9-7B3742F879F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="3156" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="25" activeTab="31" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="7116" yWindow="2436" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="27" activeTab="33" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -45,6 +45,8 @@
     <sheet name="2020年4月29日" sheetId="32" r:id="rId30"/>
     <sheet name="2020年4月30日" sheetId="33" r:id="rId31"/>
     <sheet name="2020年5月1日" sheetId="34" r:id="rId32"/>
+    <sheet name="2020年5月2日" sheetId="35" r:id="rId33"/>
+    <sheet name="2020年5月3日" sheetId="36" r:id="rId34"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -79,6 +81,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2020年4月8日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'2020年4月9日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">'2020年5月1日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">'2020年5月2日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">'2020年5月3日'!$B$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -96,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -32004,11 +32008,11 @@
         <v>125851</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.1124265997091799E-2</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>11.124265997091799</v>
       </c>
     </row>
@@ -34882,11 +34886,11 @@
         <v>116446</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -35618,11 +35622,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>0.10317295328729048</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>103.17295328729048</v>
       </c>
     </row>
@@ -35640,11 +35644,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>8.6934638878085613E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>86.934638878085607</v>
       </c>
     </row>
@@ -35662,11 +35666,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>6.5200438078760428E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>65.200438078760428</v>
       </c>
     </row>
@@ -35684,11 +35688,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>5.1849291393017631E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>51.84929139301763</v>
       </c>
     </row>
@@ -35706,11 +35710,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>4.5282445602636313E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>45.282445602636315</v>
       </c>
     </row>
@@ -35728,11 +35732,11 @@
         <v>287695</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>4.2058429934479225E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>42.058429934479221</v>
       </c>
     </row>
@@ -35750,11 +35754,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>4.0890257576677219E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>40.890257576677222</v>
       </c>
     </row>
@@ -35772,11 +35776,11 @@
         <v>411792</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>4.0554454676147184E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>40.554454676147181</v>
       </c>
     </row>
@@ -35794,11 +35798,11 @@
         <v>301185</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>3.8514534256354066E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>38.514534256354068</v>
       </c>
     </row>
@@ -35816,11 +35820,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>3.6423790806028138E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>36.423790806028137</v>
       </c>
     </row>
@@ -35838,11 +35842,11 @@
         <v>270227</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>3.5155628416109419E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>35.155628416109423</v>
       </c>
     </row>
@@ -35860,11 +35864,11 @@
         <v>209244</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>3.1542123071629291E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>31.542123071629291</v>
       </c>
     </row>
@@ -35882,11 +35886,11 @@
         <v>585470</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>3.1256938869626112E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>31.256938869626111</v>
       </c>
     </row>
@@ -35904,11 +35908,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.5441408436371039E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>25.441408436371038</v>
       </c>
     </row>
@@ -35926,11 +35930,11 @@
         <v>742652</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>2.2621631665975452E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>22.621631665975453</v>
       </c>
     </row>
@@ -35948,11 +35952,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>2.1319946458361265E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>21.319946458361265</v>
       </c>
     </row>
@@ -35970,11 +35974,11 @@
         <v>263407</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>2.0500594137589357E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>20.500594137589356</v>
       </c>
     </row>
@@ -35992,11 +35996,11 @@
         <v>519212</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>2.041555279924193E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>20.415552799241929</v>
       </c>
     </row>
@@ -36014,11 +36018,11 @@
         <v>739575</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>2.0011493087246052E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>20.011493087246052</v>
       </c>
     </row>
@@ -36036,11 +36040,11 @@
         <v>354425</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.9186005501869226E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>19.186005501869225</v>
       </c>
     </row>
@@ -36058,11 +36062,11 @@
         <v>147790</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.8945801475065971E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>18.94580147506597</v>
       </c>
     </row>
@@ -36080,11 +36084,11 @@
         <v>206268</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.6483409932708904E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>16.483409932708906</v>
       </c>
     </row>
@@ -36102,11 +36106,11 @@
         <v>695797</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.6240368958187517E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>16.240368958187517</v>
       </c>
     </row>
@@ -36124,11 +36128,11 @@
         <v>583702</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.5590147027078886E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>15.590147027078887</v>
       </c>
     </row>
@@ -36146,11 +36150,11 @@
         <v>683365</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.5218806933337235E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>15.218806933337236</v>
       </c>
     </row>
@@ -36168,11 +36172,11 @@
         <v>75168</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -36190,11 +36194,11 @@
         <v>83826</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.4315367547061772E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>14.315367547061772</v>
       </c>
     </row>
@@ -36212,11 +36216,11 @@
         <v>192518</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.3505230679728648E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>13.505230679728648</v>
       </c>
     </row>
@@ -36234,11 +36238,11 @@
         <v>239824</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.3343118286743613E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>13.343118286743612</v>
       </c>
     </row>
@@ -36256,11 +36260,11 @@
         <v>218775</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>1.3255627928236773E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>13.255627928236773</v>
       </c>
     </row>
@@ -36278,11 +36282,11 @@
         <v>125851</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>1.1124265997091799E-2</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>11.124265997091799</v>
       </c>
     </row>
@@ -36300,11 +36304,11 @@
         <v>148350</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>1.0785305021907651E-2</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>10.785305021907652</v>
       </c>
     </row>
@@ -36322,11 +36326,11 @@
         <v>116446</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -36344,11 +36348,11 @@
         <v>91850</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>9.7985846488840497E-3</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>9.7985846488840505</v>
       </c>
     </row>
@@ -36366,11 +36370,11 @@
         <v>190006</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>9.4733850509983904E-3</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>9.4733850509983899</v>
       </c>
     </row>
@@ -36388,11 +36392,11 @@
         <v>434170</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>9.4433056176152202E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>9.4433056176152199</v>
       </c>
     </row>
@@ -36410,11 +36414,11 @@
         <v>54709</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -36432,11 +36436,11 @@
         <v>80055</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>8.743988507900818E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>8.7439885079008182</v>
       </c>
     </row>
@@ -36454,11 +36458,11 @@
         <v>127998</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>8.5938842794418668E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>8.5938842794418662</v>
       </c>
     </row>
@@ -36476,11 +36480,11 @@
         <v>196435</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>8.1451879756662508E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>8.14518797566625</v>
       </c>
     </row>
@@ -36498,11 +36502,11 @@
         <v>75167</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>7.9822262428991438E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>7.9822262428991442</v>
       </c>
     </row>
@@ -36520,11 +36524,11 @@
         <v>180822</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -36542,11 +36546,11 @@
         <v>84247</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>7.1219153204268399E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1219153204268402</v>
       </c>
     </row>
@@ -36564,11 +36568,11 @@
         <v>577212</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>6.7566162865636886E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>6.7566162865636885</v>
       </c>
     </row>
@@ -36586,11 +36590,11 @@
         <v>112055</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>6.246932310026326E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>6.2469323100263257</v>
       </c>
     </row>
@@ -36608,11 +36612,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>4.6537292992148496E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>4.6537292992148496</v>
       </c>
     </row>
@@ -36630,11 +36634,11 @@
         <v>32394</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -36652,11 +36656,11 @@
         <v>133573</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -36674,11 +36678,11 @@
         <v>57443</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>1.7408561530560731E-3</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7408561530560731</v>
       </c>
     </row>
@@ -36696,11 +36700,11 @@
         <v>71544</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>1.3977412501397742E-3</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>1.3977412501397741</v>
       </c>
     </row>
@@ -36718,11 +36722,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36740,11 +36744,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36762,11 +36766,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36784,11 +36788,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36806,11 +36810,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36828,11 +36832,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36850,11 +36854,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36872,11 +36876,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36894,11 +36898,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36916,11 +36920,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36938,11 +36942,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -36960,11 +36964,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -37011,7 +37015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB369B25-4702-4754-B080-393D1CF32ACD}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -37058,11 +37062,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>0.1039429006998822</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>103.9429006998822</v>
       </c>
     </row>
@@ -37080,11 +37084,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>8.8936423325936265E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>88.936423325936261</v>
       </c>
     </row>
@@ -37102,11 +37106,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>6.5626584732869975E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>65.626584732869972</v>
       </c>
     </row>
@@ -37124,11 +37128,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>5.244526025960404E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>52.445260259604041</v>
       </c>
     </row>
@@ -37146,11 +37150,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>4.6158880033655085E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>46.158880033655088</v>
       </c>
     </row>
@@ -37168,11 +37172,11 @@
         <v>287695</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>4.2753610594553258E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>42.753610594553258</v>
       </c>
     </row>
@@ -37190,11 +37194,11 @@
         <v>939099</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>4.1848622988630589E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>41.848622988630588</v>
       </c>
     </row>
@@ -37212,11 +37216,11 @@
         <v>270227</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>4.1816694852845941E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>41.816694852845941</v>
       </c>
     </row>
@@ -37234,11 +37238,11 @@
         <v>411792</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>4.1040136768077086E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>41.040136768077083</v>
       </c>
     </row>
@@ -37256,11 +37260,11 @@
         <v>65891</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>4.0976764656781656E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>40.976764656781654</v>
       </c>
     </row>
@@ -37278,11 +37282,11 @@
         <v>301185</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>4.0838687185616812E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>40.838687185616813</v>
       </c>
     </row>
@@ -37300,11 +37304,11 @@
         <v>209244</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>3.5365410716675268E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>35.365410716675271</v>
       </c>
     </row>
@@ -37322,11 +37326,11 @@
         <v>585470</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>3.2794165371411006E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>32.794165371411005</v>
       </c>
     </row>
@@ -37344,11 +37348,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.5865431910310554E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>25.865431910310555</v>
       </c>
     </row>
@@ -37366,11 +37370,11 @@
         <v>742652</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>2.3160241943736771E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>23.160241943736771</v>
       </c>
     </row>
@@ -37388,11 +37392,11 @@
         <v>454973</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>2.1979326245733264E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>21.979326245733265</v>
       </c>
     </row>
@@ -37410,11 +37414,11 @@
         <v>519212</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>2.1763749682210735E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>21.763749682210733</v>
       </c>
     </row>
@@ -37432,11 +37436,11 @@
         <v>263407</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>2.0880234769766939E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>20.88023476976694</v>
       </c>
     </row>
@@ -37454,11 +37458,11 @@
         <v>354425</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>2.087888834026945E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>20.878888340269448</v>
       </c>
     </row>
@@ -37476,11 +37480,11 @@
         <v>739575</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>2.0687557042896258E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>20.687557042896259</v>
       </c>
     </row>
@@ -37498,11 +37502,11 @@
         <v>147790</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.9622437242032612E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>19.622437242032611</v>
       </c>
     </row>
@@ -37520,11 +37524,11 @@
         <v>695797</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.6671529196015503E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>16.671529196015502</v>
       </c>
     </row>
@@ -37542,11 +37546,11 @@
         <v>206268</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.6483409932708904E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>16.483409932708906</v>
       </c>
     </row>
@@ -37564,11 +37568,11 @@
         <v>218775</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.5998171637527141E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>15.998171637527141</v>
       </c>
     </row>
@@ -37586,11 +37590,11 @@
         <v>583702</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.5761467324079754E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>15.761467324079755</v>
       </c>
     </row>
@@ -37608,11 +37612,11 @@
         <v>683365</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.5511476297439875E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>15.511476297439874</v>
       </c>
     </row>
@@ -37630,11 +37634,11 @@
         <v>83826</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.5508314842650252E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>15.508314842650252</v>
       </c>
     </row>
@@ -37652,6 +37656,2886 @@
         <v>75168</v>
       </c>
       <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>34</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.4177063179665089E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>14.177063179665089</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31">
+        <v>192518</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.3505230679728648E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>13.505230679728648</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>125851</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>148350</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.0785305021907651E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>10.785305021907652</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>116446</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35">
+        <v>43</v>
+      </c>
+      <c r="D35">
+        <v>434170</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>9.9039546721330363E-3</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>9.903954672133036</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <v>91850</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>9.7985846488840497E-3</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>9.7985846488840505</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37">
+        <v>18</v>
+      </c>
+      <c r="D37">
+        <v>190006</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>9.4733850509983904E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>9.4733850509983899</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>54709</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>80055</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>8.743988507900818E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>8.7439885079008182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>127998</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>112055</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>7.1393512114586591E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>7.139351211458659</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>84247</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46">
+        <v>39</v>
+      </c>
+      <c r="D46">
+        <v>577212</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>6.7566162865636886E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>6.7566162865636885</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>5.3185477705312567E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3185477705312572</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>133573</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>57443</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>71544</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1.3977412501397742E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3977412501397741</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>134</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>527</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDEA8B03-8E08-43AE-B2EE-5E3B14F1C3A7}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>273</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
+        <v>0.10509782181876978</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
+        <v>105.09782181876979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>323</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>9.2368053807965964E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
+        <v>92.368053807965964</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>158</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6.7331171349308147E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>67.33117134930815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>89</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.3041229126190449E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>53.041229126190451</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>165</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4.8203893706032203E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>48.203893706032204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>126</v>
+      </c>
+      <c r="D7">
+        <v>287695</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4.3796381584664312E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>43.79638158466431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>116</v>
+      </c>
+      <c r="D8">
+        <v>270227</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4.2926872592302025E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>42.926872592302026</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>401</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>4.2700503354811369E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>42.700503354811367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>65891</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4.2494422607032824E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>42.494422607032824</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>170</v>
+      </c>
+      <c r="D11">
+        <v>411792</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>4.1282977814042041E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>41.282977814042042</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>301185</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4.1170709032654351E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>41.170709032654351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>75</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3.5843321672306014E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>35.843321672306011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>199</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3.3989785983910364E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>33.989785983910366</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>62</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2.6289455384250073E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>26.289455384250072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>183</v>
+      </c>
+      <c r="D16">
+        <v>742652</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2.4641420207580401E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>24.641420207580403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>109</v>
+      </c>
+      <c r="D17">
+        <v>454973</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2.3957465607849258E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>23.957465607849258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>177</v>
+      </c>
+      <c r="D18">
+        <v>739575</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2.3932664030017238E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>23.932664030017239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>63</v>
+      </c>
+      <c r="D19">
+        <v>263407</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>2.3917359827187585E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>23.917359827187585</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>119</v>
+      </c>
+      <c r="D20">
+        <v>519212</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>2.2919347010469712E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>22.919347010469711</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>74</v>
+      </c>
+      <c r="D21">
+        <v>354425</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>2.087888834026945E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>20.878888340269448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>147790</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.9622437242032612E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>19.622437242032611</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>218775</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.8283624728602444E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>18.283624728602444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>121</v>
+      </c>
+      <c r="D24">
+        <v>695797</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.7390129592395484E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>17.390129592395486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>83826</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.6701262138238731E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>16.701262138238732</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>206268</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.6483409932708904E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>16.483409932708906</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>95</v>
+      </c>
+      <c r="D27">
+        <v>583702</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.6275428215082353E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>16.275428215082353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>110</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.6096815025645153E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>16.096815025645153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>75168</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.4633886760323542E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>14.633886760323543</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>34</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.4177063179665089E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>14.177063179665089</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31">
+        <v>192518</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.3505230679728648E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>13.505230679728648</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>125851</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>54709</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.0967116927744979E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>10.967116927744978</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>91850</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <v>1.0887316276537834E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <v>10.887316276537833</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <v>148350</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>1.0785305021907651E-2</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="3"/>
+        <v>10.785305021907652</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>45</v>
+      </c>
+      <c r="D36">
+        <v>434170</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>1.0364603726650851E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="3"/>
+        <v>10.36460372665085</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>116446</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="3"/>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <v>190006</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>9.4733850509983904E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="3"/>
+        <v>9.4733850509983899</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>80055</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>8.743988507900818E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="3"/>
+        <v>8.7439885079008182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>127998</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="3"/>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="3"/>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>75167</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="3"/>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>180822</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>112055</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>7.1393512114586591E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="3"/>
+        <v>7.139351211458659</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>84247</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46">
+        <v>41</v>
+      </c>
+      <c r="D46">
+        <v>577212</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>7.1031094294643909E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="3"/>
+        <v>7.1031094294643911</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>5.9833662418476638E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="3"/>
+        <v>5.9833662418476639</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>71544</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.7954825002795484E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7954825002795483</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>133573</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>57443</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>142</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>542</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67AD094-15F2-4D87-B58C-323B49352121}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>285</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>0.1097175062943201</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>109.7175062943201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>329</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>9.4083869048980806E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>94.083869048980802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>160</v>
+      </c>
+      <c r="D4">
+        <v>234661</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>6.818346465752724E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>68.183464657527239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>89</v>
+      </c>
+      <c r="D5">
+        <v>167794</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>5.3041229126190449E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>53.041229126190451</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>166</v>
+      </c>
+      <c r="D6">
+        <v>342296</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>4.8496038516371798E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>48.496038516371797</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>65891</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>4.5529738507535174E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>45.529738507535171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>128</v>
+      </c>
+      <c r="D8">
+        <v>287695</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>4.4491562244738353E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>44.491562244738354</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>406</v>
+      </c>
+      <c r="D9">
+        <v>939099</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>4.3232928583674349E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>43.232928583674351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>116</v>
+      </c>
+      <c r="D10">
+        <v>270227</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>4.2926872592302025E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>42.926872592302026</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>174</v>
+      </c>
+      <c r="D11">
+        <v>411792</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>4.2254341997901852E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>42.254341997901854</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>301185</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>4.1170709032654351E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>41.170709032654351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>75</v>
+      </c>
+      <c r="D13">
+        <v>209244</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>3.5843321672306014E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>35.843321672306011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>202</v>
+      </c>
+      <c r="D14">
+        <v>585470</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>3.4502194817838658E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>34.502194817838657</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.6713478858189588E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>26.713478858189589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>191</v>
+      </c>
+      <c r="D16">
+        <v>739575</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.5825643105837813E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>25.825643105837813</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>187</v>
+      </c>
+      <c r="D17">
+        <v>742652</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>2.5180030485341721E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>25.180030485341721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>66</v>
+      </c>
+      <c r="D18">
+        <v>263407</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>2.5056281723720326E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>25.056281723720325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>126</v>
+      </c>
+      <c r="D19">
+        <v>519212</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>2.4267543893438517E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>24.267543893438518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>109</v>
+      </c>
+      <c r="D20">
+        <v>454973</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>2.3957465607849258E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>23.957465607849258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>75</v>
+      </c>
+      <c r="D21">
+        <v>354425</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>2.116103548000282E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>21.16103548000282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>218775</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>2.0569077819677751E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>20.569077819677752</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>17</v>
+      </c>
+      <c r="D23">
+        <v>83826</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>2.0280104025004176E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>20.280104025004174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>147790</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.9622437242032612E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>19.622437242032611</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>36</v>
+      </c>
+      <c r="D25">
+        <v>206268</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.745302228169178E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>17.45302228169178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>121</v>
+      </c>
+      <c r="D26">
+        <v>695797</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.7390129592395484E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>17.390129592395486</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>97</v>
+      </c>
+      <c r="D27">
+        <v>583702</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.6618068809084088E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>16.618068809084086</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>112</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.6389484389747792E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>16.389484389747793</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>75168</v>
+      </c>
+      <c r="E29">
         <f>100*C29/D29</f>
         <v>1.4633886760323542E-2</v>
       </c>
@@ -37668,18 +40552,18 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D30">
         <v>239824</v>
       </c>
       <c r="E30">
         <f>100*C30/D30</f>
-        <v>1.4177063179665089E-2</v>
+        <v>1.4594035626125825E-2</v>
       </c>
       <c r="F30" s="1">
         <f>E30*1000</f>
-        <v>14.177063179665089</v>
+        <v>14.594035626125825</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -37690,18 +40574,18 @@
         <v>25</v>
       </c>
       <c r="C31">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D31">
         <v>192518</v>
       </c>
       <c r="E31">
         <f>100*C31/D31</f>
-        <v>1.3505230679728648E-2</v>
+        <v>1.4024662628948982E-2</v>
       </c>
       <c r="F31" s="1">
         <f>E31*1000</f>
-        <v>13.505230679728648</v>
+        <v>14.024662628948981</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -37728,46 +40612,46 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D33">
-        <v>148350</v>
+        <v>91850</v>
       </c>
       <c r="E33">
         <f>100*C33/D33</f>
-        <v>1.0785305021907651E-2</v>
+        <v>1.0887316276537834E-2</v>
       </c>
       <c r="F33" s="1">
         <f>E33*1000</f>
-        <v>10.785305021907652</v>
+        <v>10.887316276537833</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C34">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D34">
-        <v>116446</v>
+        <v>148350</v>
       </c>
       <c r="E34">
         <f>100*C34/D34</f>
-        <v>1.0305205846486783E-2</v>
+        <v>1.0785305021907651E-2</v>
       </c>
       <c r="F34" s="1">
         <f>E34*1000</f>
-        <v>10.305205846486784</v>
+        <v>10.785305021907652</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -37778,40 +40662,40 @@
         <v>29</v>
       </c>
       <c r="C35">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D35">
         <v>434170</v>
       </c>
       <c r="E35">
         <f>100*C35/D35</f>
-        <v>9.9039546721330363E-3</v>
+        <v>1.0364603726650851E-2</v>
       </c>
       <c r="F35" s="1">
         <f>E35*1000</f>
-        <v>9.903954672133036</v>
+        <v>10.36460372665085</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D36">
-        <v>91850</v>
+        <v>116446</v>
       </c>
       <c r="E36">
         <f>100*C36/D36</f>
-        <v>9.7985846488840497E-3</v>
+        <v>1.0305205846486783E-2</v>
       </c>
       <c r="F36" s="1">
         <f>E36*1000</f>
-        <v>9.7985846488840505</v>
+        <v>10.305205846486784</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -38020,18 +40904,18 @@
         <v>23</v>
       </c>
       <c r="C46">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D46">
         <v>577212</v>
       </c>
       <c r="E46">
         <f>100*C46/D46</f>
-        <v>6.7566162865636886E-3</v>
+        <v>7.1031094294643909E-3</v>
       </c>
       <c r="F46" s="1">
         <f>E46*1000</f>
-        <v>6.7566162865636885</v>
+        <v>7.1031094294643911</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -38042,18 +40926,18 @@
         <v>44</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D47">
         <v>150417</v>
       </c>
       <c r="E47">
         <f>100*C47/D47</f>
-        <v>5.3185477705312567E-3</v>
+        <v>6.6481847131640709E-3</v>
       </c>
       <c r="F47" s="1">
         <f>E47*1000</f>
-        <v>5.3185477705312572</v>
+        <v>6.6481847131640706</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -38080,68 +40964,68 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49">
-        <v>133573</v>
+        <v>71544</v>
       </c>
       <c r="E49">
         <f>100*C49/D49</f>
-        <v>2.2459628817201082E-3</v>
+        <v>2.7954825002795484E-3</v>
       </c>
       <c r="F49" s="1">
         <f>E49*1000</f>
-        <v>2.2459628817201081</v>
+        <v>2.7954825002795483</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D50">
-        <v>57443</v>
+        <v>133573</v>
       </c>
       <c r="E50">
         <f>100*C50/D50</f>
-        <v>1.7408561530560731E-3</v>
+        <v>2.2459628817201082E-3</v>
       </c>
       <c r="F50" s="1">
         <f>E50*1000</f>
-        <v>1.7408561530560731</v>
+        <v>2.2459628817201081</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>71544</v>
+        <v>57443</v>
       </c>
       <c r="E51">
         <f>100*C51/D51</f>
-        <v>1.3977412501397742E-3</v>
+        <v>1.7408561530560731E-3</v>
       </c>
       <c r="F51" s="1">
         <f>E51*1000</f>
-        <v>1.3977412501397741</v>
+        <v>1.7408561530560731</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -38416,7 +41300,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D64" t="s">
         <v>69</v>
@@ -38430,7 +41314,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>527</v>
+        <v>547</v>
       </c>
       <c r="D65" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Revised: data 2020/05/04 and 2020/05/05 added.
</commit_message>
<xml_diff>
--- a/infected-person-number-population-ratio-20200401.xlsx
+++ b/infected-person-number-population-ratio-20200401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wakatono\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8763B8-7BC2-4CDE-A2B9-7B3742F879F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0861F20A-6AF1-4DF5-A3EB-FCC20325E17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7116" yWindow="2436" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="27" activeTab="33" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
+    <workbookView xWindow="17016" yWindow="1752" windowWidth="23040" windowHeight="12156" tabRatio="718" firstSheet="28" activeTab="34" xr2:uid="{2429BC5A-A61F-44D9-B931-3B703E1F67B3}"/>
   </bookViews>
   <sheets>
     <sheet name="2020年3月31日" sheetId="1" r:id="rId1"/>
@@ -47,6 +47,7 @@
     <sheet name="2020年5月1日" sheetId="34" r:id="rId32"/>
     <sheet name="2020年5月2日" sheetId="35" r:id="rId33"/>
     <sheet name="2020年5月3日" sheetId="36" r:id="rId34"/>
+    <sheet name="2020年5月4日" sheetId="37" r:id="rId35"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020年3月31日'!$B$1:$E$1</definedName>
@@ -83,6 +84,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">'2020年5月1日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">'2020年5月2日'!$B$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">'2020年5月3日'!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">'2020年5月4日'!$B$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -100,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2514" uniqueCount="100">
   <si>
     <t>千代田区</t>
   </si>
@@ -39206,11 +39208,11 @@
         <v>91850</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
+        <f t="shared" ref="E34:E63" si="2">100*C34/D34</f>
         <v>1.0887316276537834E-2</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
+        <f t="shared" ref="F34:F63" si="3">E34*1000</f>
         <v>10.887316276537833</v>
       </c>
     </row>
@@ -39895,7 +39897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67AD094-15F2-4D87-B58C-323B49352121}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -39942,11 +39944,11 @@
         <v>259758</v>
       </c>
       <c r="E2">
-        <f>100*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">100*C2/D2</f>
         <v>0.1097175062943201</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*1000</f>
+        <f t="shared" ref="F2:F33" si="1">E2*1000</f>
         <v>109.7175062943201</v>
       </c>
     </row>
@@ -39964,11 +39966,11 @@
         <v>349688</v>
       </c>
       <c r="E3">
-        <f>100*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>9.4083869048980806E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>E3*1000</f>
+        <f t="shared" si="1"/>
         <v>94.083869048980802</v>
       </c>
     </row>
@@ -39986,11 +39988,11 @@
         <v>234661</v>
       </c>
       <c r="E4">
-        <f>100*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>6.818346465752724E-2</v>
       </c>
       <c r="F4" s="1">
-        <f>E4*1000</f>
+        <f t="shared" si="1"/>
         <v>68.183464657527239</v>
       </c>
     </row>
@@ -40008,11 +40010,11 @@
         <v>167794</v>
       </c>
       <c r="E5">
-        <f>100*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>5.3041229126190449E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>E5*1000</f>
+        <f t="shared" si="1"/>
         <v>53.041229126190451</v>
       </c>
     </row>
@@ -40030,11 +40032,11 @@
         <v>342296</v>
       </c>
       <c r="E6">
-        <f>100*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>4.8496038516371798E-2</v>
       </c>
       <c r="F6" s="1">
-        <f>E6*1000</f>
+        <f t="shared" si="1"/>
         <v>48.496038516371797</v>
       </c>
     </row>
@@ -40052,11 +40054,11 @@
         <v>65891</v>
       </c>
       <c r="E7">
-        <f>100*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>4.5529738507535174E-2</v>
       </c>
       <c r="F7" s="1">
-        <f>E7*1000</f>
+        <f t="shared" si="1"/>
         <v>45.529738507535171</v>
       </c>
     </row>
@@ -40074,11 +40076,11 @@
         <v>287695</v>
       </c>
       <c r="E8">
-        <f>100*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>4.4491562244738353E-2</v>
       </c>
       <c r="F8" s="1">
-        <f>E8*1000</f>
+        <f t="shared" si="1"/>
         <v>44.491562244738354</v>
       </c>
     </row>
@@ -40096,11 +40098,11 @@
         <v>939099</v>
       </c>
       <c r="E9">
-        <f>100*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>4.3232928583674349E-2</v>
       </c>
       <c r="F9" s="1">
-        <f>E9*1000</f>
+        <f t="shared" si="1"/>
         <v>43.232928583674351</v>
       </c>
     </row>
@@ -40118,11 +40120,11 @@
         <v>270227</v>
       </c>
       <c r="E10">
-        <f>100*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>4.2926872592302025E-2</v>
       </c>
       <c r="F10" s="1">
-        <f>E10*1000</f>
+        <f t="shared" si="1"/>
         <v>42.926872592302026</v>
       </c>
     </row>
@@ -40140,11 +40142,11 @@
         <v>411792</v>
       </c>
       <c r="E11">
-        <f>100*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>4.2254341997901852E-2</v>
       </c>
       <c r="F11" s="1">
-        <f>E11*1000</f>
+        <f t="shared" si="1"/>
         <v>42.254341997901854</v>
       </c>
     </row>
@@ -40162,11 +40164,11 @@
         <v>301185</v>
       </c>
       <c r="E12">
-        <f>100*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>4.1170709032654351E-2</v>
       </c>
       <c r="F12" s="1">
-        <f>E12*1000</f>
+        <f t="shared" si="1"/>
         <v>41.170709032654351</v>
       </c>
     </row>
@@ -40184,11 +40186,11 @@
         <v>209244</v>
       </c>
       <c r="E13">
-        <f>100*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>3.5843321672306014E-2</v>
       </c>
       <c r="F13" s="1">
-        <f>E13*1000</f>
+        <f t="shared" si="1"/>
         <v>35.843321672306011</v>
       </c>
     </row>
@@ -40206,11 +40208,11 @@
         <v>585470</v>
       </c>
       <c r="E14">
-        <f>100*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>3.4502194817838658E-2</v>
       </c>
       <c r="F14" s="1">
-        <f>E14*1000</f>
+        <f t="shared" si="1"/>
         <v>34.502194817838657</v>
       </c>
     </row>
@@ -40228,11 +40230,11 @@
         <v>235836</v>
       </c>
       <c r="E15">
-        <f>100*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>2.6713478858189588E-2</v>
       </c>
       <c r="F15" s="1">
-        <f>E15*1000</f>
+        <f t="shared" si="1"/>
         <v>26.713478858189589</v>
       </c>
     </row>
@@ -40250,11 +40252,11 @@
         <v>739575</v>
       </c>
       <c r="E16">
-        <f>100*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>2.5825643105837813E-2</v>
       </c>
       <c r="F16" s="1">
-        <f>E16*1000</f>
+        <f t="shared" si="1"/>
         <v>25.825643105837813</v>
       </c>
     </row>
@@ -40272,11 +40274,11 @@
         <v>742652</v>
       </c>
       <c r="E17">
-        <f>100*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>2.5180030485341721E-2</v>
       </c>
       <c r="F17" s="1">
-        <f>E17*1000</f>
+        <f t="shared" si="1"/>
         <v>25.180030485341721</v>
       </c>
     </row>
@@ -40294,11 +40296,11 @@
         <v>263407</v>
       </c>
       <c r="E18">
-        <f>100*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>2.5056281723720326E-2</v>
       </c>
       <c r="F18" s="1">
-        <f>E18*1000</f>
+        <f t="shared" si="1"/>
         <v>25.056281723720325</v>
       </c>
     </row>
@@ -40316,11 +40318,11 @@
         <v>519212</v>
       </c>
       <c r="E19">
-        <f>100*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>2.4267543893438517E-2</v>
       </c>
       <c r="F19" s="1">
-        <f>E19*1000</f>
+        <f t="shared" si="1"/>
         <v>24.267543893438518</v>
       </c>
     </row>
@@ -40338,11 +40340,11 @@
         <v>454973</v>
       </c>
       <c r="E20">
-        <f>100*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>2.3957465607849258E-2</v>
       </c>
       <c r="F20" s="1">
-        <f>E20*1000</f>
+        <f t="shared" si="1"/>
         <v>23.957465607849258</v>
       </c>
     </row>
@@ -40360,11 +40362,11 @@
         <v>354425</v>
       </c>
       <c r="E21">
-        <f>100*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>2.116103548000282E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>E21*1000</f>
+        <f t="shared" si="1"/>
         <v>21.16103548000282</v>
       </c>
     </row>
@@ -40382,11 +40384,11 @@
         <v>218775</v>
       </c>
       <c r="E22">
-        <f>100*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>2.0569077819677751E-2</v>
       </c>
       <c r="F22" s="1">
-        <f>E22*1000</f>
+        <f t="shared" si="1"/>
         <v>20.569077819677752</v>
       </c>
     </row>
@@ -40404,11 +40406,11 @@
         <v>83826</v>
       </c>
       <c r="E23">
-        <f>100*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>2.0280104025004176E-2</v>
       </c>
       <c r="F23" s="1">
-        <f>E23*1000</f>
+        <f t="shared" si="1"/>
         <v>20.280104025004174</v>
       </c>
     </row>
@@ -40426,11 +40428,11 @@
         <v>147790</v>
       </c>
       <c r="E24">
-        <f>100*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.9622437242032612E-2</v>
       </c>
       <c r="F24" s="1">
-        <f>E24*1000</f>
+        <f t="shared" si="1"/>
         <v>19.622437242032611</v>
       </c>
     </row>
@@ -40448,11 +40450,11 @@
         <v>206268</v>
       </c>
       <c r="E25">
-        <f>100*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.745302228169178E-2</v>
       </c>
       <c r="F25" s="1">
-        <f>E25*1000</f>
+        <f t="shared" si="1"/>
         <v>17.45302228169178</v>
       </c>
     </row>
@@ -40470,11 +40472,11 @@
         <v>695797</v>
       </c>
       <c r="E26">
-        <f>100*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.7390129592395484E-2</v>
       </c>
       <c r="F26" s="1">
-        <f>E26*1000</f>
+        <f t="shared" si="1"/>
         <v>17.390129592395486</v>
       </c>
     </row>
@@ -40492,11 +40494,11 @@
         <v>583702</v>
       </c>
       <c r="E27">
-        <f>100*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.6618068809084088E-2</v>
       </c>
       <c r="F27" s="1">
-        <f>E27*1000</f>
+        <f t="shared" si="1"/>
         <v>16.618068809084086</v>
       </c>
     </row>
@@ -40514,11 +40516,11 @@
         <v>683365</v>
       </c>
       <c r="E28">
-        <f>100*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.6389484389747792E-2</v>
       </c>
       <c r="F28" s="1">
-        <f>E28*1000</f>
+        <f t="shared" si="1"/>
         <v>16.389484389747793</v>
       </c>
     </row>
@@ -40536,11 +40538,11 @@
         <v>75168</v>
       </c>
       <c r="E29">
-        <f>100*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.4633886760323542E-2</v>
       </c>
       <c r="F29" s="1">
-        <f>E29*1000</f>
+        <f t="shared" si="1"/>
         <v>14.633886760323543</v>
       </c>
     </row>
@@ -40558,11 +40560,11 @@
         <v>239824</v>
       </c>
       <c r="E30">
-        <f>100*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.4594035626125825E-2</v>
       </c>
       <c r="F30" s="1">
-        <f>E30*1000</f>
+        <f t="shared" si="1"/>
         <v>14.594035626125825</v>
       </c>
     </row>
@@ -40580,11 +40582,11 @@
         <v>192518</v>
       </c>
       <c r="E31">
-        <f>100*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>1.4024662628948982E-2</v>
       </c>
       <c r="F31" s="1">
-        <f>E31*1000</f>
+        <f t="shared" si="1"/>
         <v>14.024662628948981</v>
       </c>
     </row>
@@ -40602,11 +40604,11 @@
         <v>125851</v>
       </c>
       <c r="E32">
-        <f>100*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>1.1124265997091799E-2</v>
       </c>
       <c r="F32" s="1">
-        <f>E32*1000</f>
+        <f t="shared" si="1"/>
         <v>11.124265997091799</v>
       </c>
     </row>
@@ -40624,11 +40626,11 @@
         <v>91850</v>
       </c>
       <c r="E33">
-        <f>100*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>1.0887316276537834E-2</v>
       </c>
       <c r="F33" s="1">
-        <f>E33*1000</f>
+        <f t="shared" si="1"/>
         <v>10.887316276537833</v>
       </c>
     </row>
@@ -40646,11 +40648,11 @@
         <v>148350</v>
       </c>
       <c r="E34">
-        <f>100*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="2">100*C34/D34</f>
         <v>1.0785305021907651E-2</v>
       </c>
       <c r="F34" s="1">
-        <f>E34*1000</f>
+        <f t="shared" ref="F34:F65" si="3">E34*1000</f>
         <v>10.785305021907652</v>
       </c>
     </row>
@@ -40668,11 +40670,11 @@
         <v>434170</v>
       </c>
       <c r="E35">
-        <f>100*C35/D35</f>
+        <f t="shared" si="2"/>
         <v>1.0364603726650851E-2</v>
       </c>
       <c r="F35" s="1">
-        <f>E35*1000</f>
+        <f t="shared" si="3"/>
         <v>10.36460372665085</v>
       </c>
     </row>
@@ -40690,11 +40692,11 @@
         <v>116446</v>
       </c>
       <c r="E36">
-        <f>100*C36/D36</f>
+        <f t="shared" si="2"/>
         <v>1.0305205846486783E-2</v>
       </c>
       <c r="F36" s="1">
-        <f>E36*1000</f>
+        <f t="shared" si="3"/>
         <v>10.305205846486784</v>
       </c>
     </row>
@@ -40712,11 +40714,11 @@
         <v>190006</v>
       </c>
       <c r="E37">
-        <f>100*C37/D37</f>
+        <f t="shared" si="2"/>
         <v>9.4733850509983904E-3</v>
       </c>
       <c r="F37" s="1">
-        <f>E37*1000</f>
+        <f t="shared" si="3"/>
         <v>9.4733850509983899</v>
       </c>
     </row>
@@ -40734,11 +40736,11 @@
         <v>54709</v>
       </c>
       <c r="E38">
-        <f>100*C38/D38</f>
+        <f t="shared" si="2"/>
         <v>9.1392641064541487E-3</v>
       </c>
       <c r="F38" s="1">
-        <f>E38*1000</f>
+        <f t="shared" si="3"/>
         <v>9.1392641064541493</v>
       </c>
     </row>
@@ -40756,11 +40758,11 @@
         <v>80055</v>
       </c>
       <c r="E39">
-        <f>100*C39/D39</f>
+        <f t="shared" si="2"/>
         <v>8.743988507900818E-3</v>
       </c>
       <c r="F39" s="1">
-        <f>E39*1000</f>
+        <f t="shared" si="3"/>
         <v>8.7439885079008182</v>
       </c>
     </row>
@@ -40778,11 +40780,11 @@
         <v>127998</v>
       </c>
       <c r="E40">
-        <f>100*C40/D40</f>
+        <f t="shared" si="2"/>
         <v>8.5938842794418668E-3</v>
       </c>
       <c r="F40" s="1">
-        <f>E40*1000</f>
+        <f t="shared" si="3"/>
         <v>8.5938842794418662</v>
       </c>
     </row>
@@ -40800,11 +40802,11 @@
         <v>196435</v>
       </c>
       <c r="E41">
-        <f>100*C41/D41</f>
+        <f t="shared" si="2"/>
         <v>8.1451879756662508E-3</v>
       </c>
       <c r="F41" s="1">
-        <f>E41*1000</f>
+        <f t="shared" si="3"/>
         <v>8.14518797566625</v>
       </c>
     </row>
@@ -40822,11 +40824,11 @@
         <v>75167</v>
       </c>
       <c r="E42">
-        <f>100*C42/D42</f>
+        <f t="shared" si="2"/>
         <v>7.9822262428991438E-3</v>
       </c>
       <c r="F42" s="1">
-        <f>E42*1000</f>
+        <f t="shared" si="3"/>
         <v>7.9822262428991442</v>
       </c>
     </row>
@@ -40844,11 +40846,11 @@
         <v>180822</v>
       </c>
       <c r="E43">
-        <f>100*C43/D43</f>
+        <f t="shared" si="2"/>
         <v>7.1893906714890887E-3</v>
       </c>
       <c r="F43" s="1">
-        <f>E43*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1893906714890887</v>
       </c>
     </row>
@@ -40866,11 +40868,11 @@
         <v>112055</v>
       </c>
       <c r="E44">
-        <f>100*C44/D44</f>
+        <f t="shared" si="2"/>
         <v>7.1393512114586591E-3</v>
       </c>
       <c r="F44" s="1">
-        <f>E44*1000</f>
+        <f t="shared" si="3"/>
         <v>7.139351211458659</v>
       </c>
     </row>
@@ -40888,11 +40890,11 @@
         <v>84247</v>
       </c>
       <c r="E45">
-        <f>100*C45/D45</f>
+        <f t="shared" si="2"/>
         <v>7.1219153204268399E-3</v>
       </c>
       <c r="F45" s="1">
-        <f>E45*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1219153204268402</v>
       </c>
     </row>
@@ -40910,11 +40912,11 @@
         <v>577212</v>
       </c>
       <c r="E46">
-        <f>100*C46/D46</f>
+        <f t="shared" si="2"/>
         <v>7.1031094294643909E-3</v>
       </c>
       <c r="F46" s="1">
-        <f>E46*1000</f>
+        <f t="shared" si="3"/>
         <v>7.1031094294643911</v>
       </c>
     </row>
@@ -40932,11 +40934,11 @@
         <v>150417</v>
       </c>
       <c r="E47">
-        <f>100*C47/D47</f>
+        <f t="shared" si="2"/>
         <v>6.6481847131640709E-3</v>
       </c>
       <c r="F47" s="1">
-        <f>E47*1000</f>
+        <f t="shared" si="3"/>
         <v>6.6481847131640706</v>
       </c>
     </row>
@@ -40954,11 +40956,11 @@
         <v>32394</v>
       </c>
       <c r="E48">
-        <f>100*C48/D48</f>
+        <f t="shared" si="2"/>
         <v>3.0869914181638576E-3</v>
       </c>
       <c r="F48" s="1">
-        <f>E48*1000</f>
+        <f t="shared" si="3"/>
         <v>3.0869914181638576</v>
       </c>
     </row>
@@ -40976,11 +40978,11 @@
         <v>71544</v>
       </c>
       <c r="E49">
-        <f>100*C49/D49</f>
+        <f t="shared" si="2"/>
         <v>2.7954825002795484E-3</v>
       </c>
       <c r="F49" s="1">
-        <f>E49*1000</f>
+        <f t="shared" si="3"/>
         <v>2.7954825002795483</v>
       </c>
     </row>
@@ -40998,11 +41000,11 @@
         <v>133573</v>
       </c>
       <c r="E50">
-        <f>100*C50/D50</f>
+        <f t="shared" si="2"/>
         <v>2.2459628817201082E-3</v>
       </c>
       <c r="F50" s="1">
-        <f>E50*1000</f>
+        <f t="shared" si="3"/>
         <v>2.2459628817201081</v>
       </c>
     </row>
@@ -41020,11 +41022,11 @@
         <v>57443</v>
       </c>
       <c r="E51">
-        <f>100*C51/D51</f>
+        <f t="shared" si="2"/>
         <v>1.7408561530560731E-3</v>
       </c>
       <c r="F51" s="1">
-        <f>E51*1000</f>
+        <f t="shared" si="3"/>
         <v>1.7408561530560731</v>
       </c>
     </row>
@@ -41042,11 +41044,11 @@
         <v>17140</v>
       </c>
       <c r="E52">
-        <f>100*C52/D52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F52" s="1">
-        <f>E52*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41064,11 +41066,11 @@
         <v>1990</v>
       </c>
       <c r="E53">
-        <f>100*C53/D53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F53" s="1">
-        <f>E53*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41086,11 +41088,11 @@
         <v>4863</v>
       </c>
       <c r="E54">
-        <f>100*C54/D54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f>E54*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41108,11 +41110,11 @@
         <v>7244</v>
       </c>
       <c r="E55">
-        <f>100*C55/D55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f>E55*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41130,11 +41132,11 @@
         <v>344</v>
       </c>
       <c r="E56">
-        <f>100*C56/D56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f>E56*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41152,11 +41154,11 @@
         <v>2594</v>
       </c>
       <c r="E57">
-        <f>100*C57/D57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F57" s="1">
-        <f>E57*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41174,11 +41176,11 @@
         <v>1870</v>
       </c>
       <c r="E58">
-        <f>100*C58/D58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F58" s="1">
-        <f>E58*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41196,11 +41198,11 @@
         <v>2270</v>
       </c>
       <c r="E59">
-        <f>100*C59/D59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F59" s="1">
-        <f>E59*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41218,11 +41220,11 @@
         <v>337</v>
       </c>
       <c r="E60">
-        <f>100*C60/D60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f>E60*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41240,11 +41242,11 @@
         <v>7096</v>
       </c>
       <c r="E61">
-        <f>100*C61/D61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F61" s="1">
-        <f>E61*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41262,11 +41264,11 @@
         <v>176</v>
       </c>
       <c r="E62">
-        <f>100*C62/D62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="1">
-        <f>E62*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41284,11 +41286,11 @@
         <v>3055</v>
       </c>
       <c r="E63">
-        <f>100*C63/D63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F63" s="1">
-        <f>E63*1000</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -41324,6 +41326,1446 @@
   <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
     <sortCondition descending="1" ref="F2:F65"/>
+  </sortState>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566349A1-6E87-4D3A-8645-299B0784CB35}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="27.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>289</v>
+      </c>
+      <c r="D2">
+        <v>259758</v>
+      </c>
+      <c r="E2">
+        <f>100*C2/D2</f>
+        <v>0.11125740111950354</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*1000</f>
+        <v>111.25740111950354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>336</v>
+      </c>
+      <c r="D3">
+        <v>349688</v>
+      </c>
+      <c r="E3">
+        <f>100*C3/D3</f>
+        <v>9.6085653496831458E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>E3*1000</f>
+        <v>96.085653496831455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>217</v>
+      </c>
+      <c r="D4">
+        <v>301185</v>
+      </c>
+      <c r="E4">
+        <f>100*C4/D4</f>
+        <v>7.2048740807145115E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E4*1000</f>
+        <v>72.048740807145109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>160</v>
+      </c>
+      <c r="D5">
+        <v>234661</v>
+      </c>
+      <c r="E5">
+        <f>100*C5/D5</f>
+        <v>6.818346465752724E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E5*1000</f>
+        <v>68.183464657527239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>167794</v>
+      </c>
+      <c r="E6">
+        <f>100*C6/D6</f>
+        <v>5.3637197992776858E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E6*1000</f>
+        <v>53.637197992776855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>173</v>
+      </c>
+      <c r="D7">
+        <v>342296</v>
+      </c>
+      <c r="E7">
+        <f>100*C7/D7</f>
+        <v>5.0541052188748922E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E7*1000</f>
+        <v>50.541052188748921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>65891</v>
+      </c>
+      <c r="E8">
+        <f>100*C8/D8</f>
+        <v>4.7047396457786342E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*1000</f>
+        <v>47.047396457786341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>129</v>
+      </c>
+      <c r="D9">
+        <v>287695</v>
+      </c>
+      <c r="E9">
+        <f>100*C9/D9</f>
+        <v>4.4839152574775366E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*1000</f>
+        <v>44.839152574775369</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>415</v>
+      </c>
+      <c r="D10">
+        <v>939099</v>
+      </c>
+      <c r="E10">
+        <f>100*C10/D10</f>
+        <v>4.4191293995627726E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10*1000</f>
+        <v>44.191293995627724</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>177</v>
+      </c>
+      <c r="D11">
+        <v>411792</v>
+      </c>
+      <c r="E11">
+        <f>100*C11/D11</f>
+        <v>4.2982865135796716E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E11*1000</f>
+        <v>42.982865135796715</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>116</v>
+      </c>
+      <c r="D12">
+        <v>270227</v>
+      </c>
+      <c r="E12">
+        <f>100*C12/D12</f>
+        <v>4.2926872592302025E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E12*1000</f>
+        <v>42.926872592302026</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>215</v>
+      </c>
+      <c r="D13">
+        <v>585470</v>
+      </c>
+      <c r="E13">
+        <f>100*C13/D13</f>
+        <v>3.672263309819461E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>E13*1000</f>
+        <v>36.722633098194606</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>75</v>
+      </c>
+      <c r="D14">
+        <v>209244</v>
+      </c>
+      <c r="E14">
+        <f>100*C14/D14</f>
+        <v>3.5843321672306014E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E14*1000</f>
+        <v>35.843321672306011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>235836</v>
+      </c>
+      <c r="E15">
+        <f>100*C15/D15</f>
+        <v>2.9681643175766211E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E15*1000</f>
+        <v>29.681643175766212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>197</v>
+      </c>
+      <c r="D16">
+        <v>739575</v>
+      </c>
+      <c r="E16">
+        <f>100*C16/D16</f>
+        <v>2.6636919852618058E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E16*1000</f>
+        <v>26.636919852618057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>191</v>
+      </c>
+      <c r="D17">
+        <v>742652</v>
+      </c>
+      <c r="E17">
+        <f>100*C17/D17</f>
+        <v>2.571864076310304E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E17*1000</f>
+        <v>25.718640763103039</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>66</v>
+      </c>
+      <c r="D18">
+        <v>263407</v>
+      </c>
+      <c r="E18">
+        <f>100*C18/D18</f>
+        <v>2.5056281723720326E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*1000</f>
+        <v>25.056281723720325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>128</v>
+      </c>
+      <c r="D19">
+        <v>519212</v>
+      </c>
+      <c r="E19">
+        <f>100*C19/D19</f>
+        <v>2.4652743002858177E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E19*1000</f>
+        <v>24.652743002858177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>109</v>
+      </c>
+      <c r="D20">
+        <v>454973</v>
+      </c>
+      <c r="E20">
+        <f>100*C20/D20</f>
+        <v>2.3957465607849258E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E20*1000</f>
+        <v>23.957465607849258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>83826</v>
+      </c>
+      <c r="E21">
+        <f>100*C21/D21</f>
+        <v>2.2665998616181137E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E21*1000</f>
+        <v>22.665998616181138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>75</v>
+      </c>
+      <c r="D22">
+        <v>354425</v>
+      </c>
+      <c r="E22">
+        <f>100*C22/D22</f>
+        <v>2.116103548000282E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E22*1000</f>
+        <v>21.16103548000282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>45</v>
+      </c>
+      <c r="D23">
+        <v>218775</v>
+      </c>
+      <c r="E23">
+        <f>100*C23/D23</f>
+        <v>2.0569077819677751E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23*1000</f>
+        <v>20.569077819677752</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>147790</v>
+      </c>
+      <c r="E24">
+        <f>100*C24/D24</f>
+        <v>1.9622437242032612E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24*1000</f>
+        <v>19.622437242032611</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>206268</v>
+      </c>
+      <c r="E25">
+        <f>100*C25/D25</f>
+        <v>1.9392246979657534E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f>E25*1000</f>
+        <v>19.392246979657536</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>123</v>
+      </c>
+      <c r="D26">
+        <v>695797</v>
+      </c>
+      <c r="E26">
+        <f>100*C26/D26</f>
+        <v>1.7677569750947475E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*1000</f>
+        <v>17.677569750947477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>99</v>
+      </c>
+      <c r="D27">
+        <v>583702</v>
+      </c>
+      <c r="E27">
+        <f>100*C27/D27</f>
+        <v>1.6960709403085823E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E27*1000</f>
+        <v>16.960709403085822</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>114</v>
+      </c>
+      <c r="D28">
+        <v>683365</v>
+      </c>
+      <c r="E28">
+        <f>100*C28/D28</f>
+        <v>1.6682153753850432E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>E28*1000</f>
+        <v>16.682153753850432</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>75168</v>
+      </c>
+      <c r="E29">
+        <f>100*C29/D29</f>
+        <v>1.5964240102171137E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>E29*1000</f>
+        <v>15.964240102171138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <v>239824</v>
+      </c>
+      <c r="E30">
+        <f>100*C30/D30</f>
+        <v>1.4594035626125825E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f>E30*1000</f>
+        <v>14.594035626125825</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>192518</v>
+      </c>
+      <c r="E31">
+        <f>100*C31/D31</f>
+        <v>1.4024662628948982E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f>E31*1000</f>
+        <v>14.024662628948981</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <v>148350</v>
+      </c>
+      <c r="E32">
+        <f>100*C32/D32</f>
+        <v>1.1459386585776879E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <f>E32*1000</f>
+        <v>11.459386585776878</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>125851</v>
+      </c>
+      <c r="E33">
+        <f>100*C33/D33</f>
+        <v>1.1124265997091799E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f>E33*1000</f>
+        <v>11.124265997091799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>91850</v>
+      </c>
+      <c r="E34">
+        <f>100*C34/D34</f>
+        <v>1.0887316276537834E-2</v>
+      </c>
+      <c r="F34" s="1">
+        <f>E34*1000</f>
+        <v>10.887316276537833</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35">
+        <v>46</v>
+      </c>
+      <c r="D35">
+        <v>434170</v>
+      </c>
+      <c r="E35">
+        <f>100*C35/D35</f>
+        <v>1.059492825390976E-2</v>
+      </c>
+      <c r="F35" s="1">
+        <f>E35*1000</f>
+        <v>10.59492825390976</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>116446</v>
+      </c>
+      <c r="E36">
+        <f>100*C36/D36</f>
+        <v>1.0305205846486783E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <f>E36*1000</f>
+        <v>10.305205846486784</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37">
+        <v>18</v>
+      </c>
+      <c r="D37">
+        <v>190006</v>
+      </c>
+      <c r="E37">
+        <f>100*C37/D37</f>
+        <v>9.4733850509983904E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <f>E37*1000</f>
+        <v>9.4733850509983899</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>54709</v>
+      </c>
+      <c r="E38">
+        <f>100*C38/D38</f>
+        <v>9.1392641064541487E-3</v>
+      </c>
+      <c r="F38" s="1">
+        <f>E38*1000</f>
+        <v>9.1392641064541493</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>80055</v>
+      </c>
+      <c r="E39">
+        <f>100*C39/D39</f>
+        <v>8.743988507900818E-3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>E39*1000</f>
+        <v>8.7439885079008182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>127998</v>
+      </c>
+      <c r="E40">
+        <f>100*C40/D40</f>
+        <v>8.5938842794418668E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <f>E40*1000</f>
+        <v>8.5938842794418662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>196435</v>
+      </c>
+      <c r="E41">
+        <f>100*C41/D41</f>
+        <v>8.1451879756662508E-3</v>
+      </c>
+      <c r="F41" s="1">
+        <f>E41*1000</f>
+        <v>8.14518797566625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42">
+        <v>9</v>
+      </c>
+      <c r="D42">
+        <v>112055</v>
+      </c>
+      <c r="E42">
+        <f>100*C42/D42</f>
+        <v>8.0317701128909905E-3</v>
+      </c>
+      <c r="F42" s="1">
+        <f>E42*1000</f>
+        <v>8.0317701128909906</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>75167</v>
+      </c>
+      <c r="E43">
+        <f>100*C43/D43</f>
+        <v>7.9822262428991438E-3</v>
+      </c>
+      <c r="F43" s="1">
+        <f>E43*1000</f>
+        <v>7.9822262428991442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>180822</v>
+      </c>
+      <c r="E44">
+        <f>100*C44/D44</f>
+        <v>7.1893906714890887E-3</v>
+      </c>
+      <c r="F44" s="1">
+        <f>E44*1000</f>
+        <v>7.1893906714890887</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>84247</v>
+      </c>
+      <c r="E45">
+        <f>100*C45/D45</f>
+        <v>7.1219153204268399E-3</v>
+      </c>
+      <c r="F45" s="1">
+        <f>E45*1000</f>
+        <v>7.1219153204268402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46">
+        <v>41</v>
+      </c>
+      <c r="D46">
+        <v>577212</v>
+      </c>
+      <c r="E46">
+        <f>100*C46/D46</f>
+        <v>7.1031094294643909E-3</v>
+      </c>
+      <c r="F46" s="1">
+        <f>E46*1000</f>
+        <v>7.1031094294643911</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>150417</v>
+      </c>
+      <c r="E47">
+        <f>100*C47/D47</f>
+        <v>6.6481847131640709E-3</v>
+      </c>
+      <c r="F47" s="1">
+        <f>E47*1000</f>
+        <v>6.6481847131640706</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>32394</v>
+      </c>
+      <c r="E48">
+        <f>100*C48/D48</f>
+        <v>3.0869914181638576E-3</v>
+      </c>
+      <c r="F48" s="1">
+        <f>E48*1000</f>
+        <v>3.0869914181638576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>71544</v>
+      </c>
+      <c r="E49">
+        <f>100*C49/D49</f>
+        <v>2.7954825002795484E-3</v>
+      </c>
+      <c r="F49" s="1">
+        <f>E49*1000</f>
+        <v>2.7954825002795483</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>133573</v>
+      </c>
+      <c r="E50">
+        <f>100*C50/D50</f>
+        <v>2.2459628817201082E-3</v>
+      </c>
+      <c r="F50" s="1">
+        <f>E50*1000</f>
+        <v>2.2459628817201081</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>57443</v>
+      </c>
+      <c r="E51">
+        <f>100*C51/D51</f>
+        <v>1.7408561530560731E-3</v>
+      </c>
+      <c r="F51" s="1">
+        <f>E51*1000</f>
+        <v>1.7408561530560731</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>17140</v>
+      </c>
+      <c r="E52">
+        <f>100*C52/D52</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>E52*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1990</v>
+      </c>
+      <c r="E53">
+        <f>100*C53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <f>E53*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>4863</v>
+      </c>
+      <c r="E54">
+        <f>100*C54/D54</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>E54*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>7244</v>
+      </c>
+      <c r="E55">
+        <f>100*C55/D55</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f>E55*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <f>100*C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f>E56*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2594</v>
+      </c>
+      <c r="E57">
+        <f>100*C57/D57</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <f>E57*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>1870</v>
+      </c>
+      <c r="E58">
+        <f>100*C58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <f>E58*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2270</v>
+      </c>
+      <c r="E59">
+        <f>100*C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <f>E59*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>337</v>
+      </c>
+      <c r="E60">
+        <f>100*C60/D60</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <f>E60*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>7096</v>
+      </c>
+      <c r="E61">
+        <f>100*C61/D61</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <f>E61*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>176</v>
+      </c>
+      <c r="E62">
+        <f>100*C62/D62</f>
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>3055</v>
+      </c>
+      <c r="E63">
+        <f>100*C63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <f>E63*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>147</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>547</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E1" xr:uid="{3BDB1864-6F2B-4631-A3FF-3C456AA02B42}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
+    <sortCondition descending="1" ref="F2:F66"/>
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>